<commit_message>
Got rid of useless while
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -831,663 +831,663 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:BF16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row spans="1:58" r="1">
-      <c t="s" r="A1">
+      <c r="A1" t="s">
         <v>80</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>82</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>136</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>110</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>107</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>127</v>
       </c>
-      <c t="s" r="I1">
+      <c r="I1" t="s">
         <v>83</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>103</v>
       </c>
     </row>
     <row spans="1:58" r="2">
-      <c t="s" r="A2">
+      <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>102</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="G2">
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c t="s" r="H2">
+      <c r="H2" t="s">
         <v>65</v>
       </c>
-      <c t="s" r="I2">
+      <c r="I2" t="s">
         <v>128</v>
       </c>
-      <c t="s" r="J2">
+      <c r="J2" t="s">
         <v>119</v>
       </c>
-      <c t="s" r="K2">
+      <c r="K2" t="s">
         <v>108</v>
       </c>
-      <c t="s" r="L2">
+      <c r="L2" t="s">
         <v>42</v>
       </c>
-      <c t="s" r="M2">
+      <c r="M2" t="s">
         <v>52</v>
       </c>
-      <c t="s" r="O2">
-        <v>60</v>
-      </c>
-      <c t="s" r="P2">
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="Q2">
-        <v>60</v>
-      </c>
-      <c t="s" r="R2">
-        <v>60</v>
-      </c>
-      <c t="s" r="S2">
+      <c r="Q2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="T2">
-        <v>60</v>
-      </c>
-      <c t="s" r="U2">
-        <v>60</v>
-      </c>
-      <c t="s" r="V2">
+      <c r="T2" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="W2">
-        <v>60</v>
-      </c>
-      <c t="s" r="X2">
-        <v>60</v>
-      </c>
-      <c t="s" r="Y2">
+      <c r="W2" t="s">
+        <v>60</v>
+      </c>
+      <c r="X2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="Z2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AA2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AB2">
+      <c r="Z2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AC2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AD2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AE2">
+      <c r="AC2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AF2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AG2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AH2">
+      <c r="AF2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AI2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AJ2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AK2">
+      <c r="AI2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AL2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AM2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AN2">
+      <c r="AL2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AO2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AP2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AQ2">
+      <c r="AO2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AR2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AS2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AT2">
+      <c r="AR2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AU2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AV2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AW2">
+      <c r="AU2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AX2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AZ2">
+      <c r="AX2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>133</v>
       </c>
-      <c t="s" r="BA2">
+      <c r="BA2" t="s">
         <v>56</v>
       </c>
-      <c t="s" r="BB2">
+      <c r="BB2" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="BC2">
+      <c r="BC2" t="s">
         <v>109</v>
       </c>
-      <c t="s" r="BD2">
+      <c r="BD2" t="s">
         <v>66</v>
       </c>
-      <c t="s" r="BE2">
+      <c r="BE2" t="s">
         <v>99</v>
       </c>
-      <c t="s" r="BF2">
+      <c r="BF2" t="s">
         <v>106</v>
       </c>
     </row>
     <row spans="1:58" r="3">
-      <c t="s" r="A3">
+      <c r="A3" t="s">
         <v>105</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>112</v>
       </c>
-      <c t="s" r="D3">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="E3">
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="F3">
+      <c r="F3" t="s">
         <v>68</v>
       </c>
-      <c t="s" r="G3">
+      <c r="G3" t="s">
         <v>69</v>
       </c>
-      <c t="s" r="H3">
+      <c r="H3" t="s">
         <v>92</v>
       </c>
-      <c t="s" r="I3">
+      <c r="I3" t="s">
         <v>138</v>
       </c>
-      <c t="s" r="J3">
+      <c r="J3" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="K3">
+      <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c t="s" r="L3">
+      <c r="L3" t="s">
         <v>132</v>
       </c>
-      <c t="s" r="M3">
+      <c r="M3" t="s">
         <v>59</v>
       </c>
-      <c t="s" r="N3">
+      <c r="N3" t="s">
         <v>54</v>
       </c>
-      <c t="s" r="O3">
+      <c r="O3" t="s">
         <v>76</v>
       </c>
-      <c t="s" r="P3">
+      <c r="P3" t="s">
         <v>121</v>
       </c>
-      <c t="s" r="Q3">
+      <c r="Q3" t="s">
         <v>121</v>
       </c>
     </row>
     <row spans="1:58" r="4">
-      <c t="s" r="A4">
+      <c r="A4" t="s">
         <v>120</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>124</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>125</v>
       </c>
-      <c t="s" r="D4">
+      <c r="D4" t="s">
         <v>135</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>113</v>
       </c>
-      <c t="s" r="F4">
+      <c r="F4" t="s">
         <v>123</v>
       </c>
-      <c t="s" r="G4">
+      <c r="G4" t="s">
         <v>130</v>
       </c>
-      <c t="s" r="H4">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="I4">
+      <c r="I4" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="J4">
+      <c r="J4" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="K4">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c t="s" r="L4">
+      <c r="L4" t="s">
         <v>126</v>
       </c>
-      <c t="s" r="M4">
+      <c r="M4" t="s">
         <v>86</v>
       </c>
-      <c t="s" r="N4">
+      <c r="N4" t="s">
         <v>39</v>
       </c>
-      <c t="s" r="O4">
+      <c r="O4" t="s">
         <v>48</v>
       </c>
-      <c t="s" r="P4">
+      <c r="P4" t="s">
         <v>78</v>
       </c>
-      <c t="s" r="Q4">
+      <c r="Q4" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="R4">
+      <c r="R4" t="s">
         <v>88</v>
       </c>
-      <c t="s" r="S4">
+      <c r="S4" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="T4">
+      <c r="T4" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="U4">
+      <c r="U4" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="V4">
+      <c r="V4" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="W4">
+      <c r="W4" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="X4">
+      <c r="X4" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="Y4">
+      <c r="Y4" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="Z4">
+      <c r="Z4" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="AA4">
+      <c r="AA4" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="AB4">
+      <c r="AB4" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="AC4">
+      <c r="AC4" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="AD4">
+      <c r="AD4" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="AE4">
+      <c r="AE4" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="AF4">
+      <c r="AF4" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="AG4">
+      <c r="AG4" t="s">
         <v>78</v>
       </c>
-      <c t="s" r="AH4">
+      <c r="AH4" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="AJ4">
+      <c r="AJ4" t="s">
         <v>53</v>
       </c>
-      <c t="s" r="AK4">
+      <c r="AK4" t="s">
         <v>87</v>
       </c>
-      <c t="s" r="AL4">
+      <c r="AL4" t="s">
         <v>122</v>
       </c>
-      <c t="s" r="AN4">
+      <c r="AN4" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="AO4">
+      <c r="AO4" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="AP4">
+      <c r="AP4" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="AQ4">
+      <c r="AQ4" t="s">
         <v>20</v>
       </c>
     </row>
     <row spans="1:58" r="5">
-      <c t="s" r="A5">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
     <row spans="1:58" r="6">
-      <c t="s" r="A6">
+      <c r="A6" t="s">
         <v>145</v>
       </c>
     </row>
     <row spans="1:58" r="7">
-      <c t="s" r="A7">
+      <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>100</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>101</v>
       </c>
     </row>
     <row spans="1:58" r="8">
-      <c t="s" r="A8">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>124</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>125</v>
       </c>
-      <c t="s" r="D8">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="F8">
+      <c r="F8" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="G8">
+      <c r="G8" t="s">
         <v>81</v>
       </c>
-      <c t="s" r="H8">
+      <c r="H8" t="s">
         <v>97</v>
       </c>
-      <c t="s" r="I8">
+      <c r="I8" t="s">
         <v>63</v>
       </c>
-      <c t="s" r="J8">
+      <c r="J8" t="s">
         <v>116</v>
       </c>
-      <c t="s" r="K8">
+      <c r="K8" t="s">
         <v>117</v>
       </c>
-      <c t="s" r="L8">
+      <c r="L8" t="s">
         <v>17</v>
       </c>
     </row>
     <row spans="1:58" r="9">
-      <c t="s" r="A9">
+      <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>89</v>
       </c>
-      <c t="s" r="D9">
+      <c r="D9" t="s">
         <v>98</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>74</v>
       </c>
-      <c t="s" r="F9">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="G9">
+      <c r="G9" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="H9">
+      <c r="H9" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="I9">
+      <c r="I9" t="s">
         <v>25</v>
       </c>
-      <c t="s" r="J9">
+      <c r="J9" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="K9">
+      <c r="K9" t="s">
         <v>111</v>
       </c>
-      <c t="s" r="L9">
+      <c r="L9" t="s">
         <v>140</v>
       </c>
-      <c t="s" r="M9">
+      <c r="M9" t="s">
         <v>140</v>
       </c>
-      <c t="s" r="N9">
+      <c r="N9" t="s">
         <v>75</v>
       </c>
-      <c t="s" r="O9">
+      <c r="O9" t="s">
         <v>85</v>
       </c>
     </row>
     <row spans="1:58" r="10">
-      <c t="s" r="A10">
+      <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>131</v>
       </c>
-      <c t="s" r="D10">
+      <c r="D10" t="s">
         <v>144</v>
       </c>
-      <c t="s" r="E10">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="F10">
+      <c r="F10" t="s">
         <v>95</v>
       </c>
-      <c t="s" r="G10">
+      <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c t="s" r="H10">
+      <c r="H10" t="s">
         <v>134</v>
       </c>
-      <c t="s" r="I10">
+      <c r="I10" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="J10">
+      <c r="J10" t="s">
         <v>24</v>
       </c>
     </row>
     <row spans="1:58" r="11">
-      <c t="s" r="A11">
+      <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>129</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>139</v>
       </c>
-      <c t="s" r="D11">
+      <c r="D11" t="s">
         <v>137</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" t="s">
         <v>48</v>
       </c>
     </row>
     <row spans="1:58" r="12">
-      <c t="s" r="A12">
+      <c r="A12" t="s">
         <v>70</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="D12">
+      <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="E12">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="F12">
+      <c r="F12" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="I12">
+      <c r="I12" t="s">
         <v>55</v>
       </c>
-      <c t="s" r="J12">
+      <c r="J12" t="s">
         <v>71</v>
       </c>
-      <c t="s" r="K12">
+      <c r="K12" t="s">
         <v>43</v>
       </c>
-      <c t="s" r="L12">
+      <c r="L12" t="s">
         <v>45</v>
       </c>
-      <c t="s" r="M12">
+      <c r="M12" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="N12">
+      <c r="N12" t="s">
         <v>115</v>
       </c>
-      <c t="s" r="O12">
+      <c r="O12" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="P12">
+      <c r="P12" t="s">
         <v>46</v>
       </c>
-      <c t="s" r="Q12">
+      <c r="Q12" t="s">
         <v>44</v>
       </c>
-      <c t="s" r="R12">
+      <c r="R12" t="s">
         <v>37</v>
       </c>
     </row>
     <row spans="1:58" r="13">
-      <c t="s" r="A13">
+      <c r="A13" t="s">
         <v>90</v>
       </c>
     </row>
     <row spans="1:58" r="14">
-      <c t="s" r="A14">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c t="s" r="B14">
+      <c r="B14" t="s">
         <v>142</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C14" t="s">
         <v>143</v>
       </c>
-      <c t="s" r="D14">
+      <c r="D14" t="s">
         <v>146</v>
       </c>
     </row>
     <row spans="1:58" r="15">
-      <c t="s" r="B15">
+      <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="C15">
+      <c r="C15" t="s">
         <v>61</v>
       </c>
-      <c t="s" r="D15">
+      <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c t="s" r="E15">
+      <c r="E15" t="s">
         <v>114</v>
       </c>
-      <c t="s" r="F15">
+      <c r="F15" t="s">
         <v>118</v>
       </c>
-      <c t="s" r="G15">
+      <c r="G15" t="s">
         <v>91</v>
       </c>
     </row>
     <row spans="1:58" r="16">
-      <c t="s" r="B16">
+      <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="C16">
+      <c r="C16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="D16">
+      <c r="D16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="E16">
+      <c r="E16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="F16">
+      <c r="F16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="G16">
+      <c r="G16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="H16">
+      <c r="H16" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75" top="1"/>
+  <pageMargins top="1" header="0.5" footer="0.5" right="0.75" bottom="1" left="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trying to resolve merge.
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -833,7 +833,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:BF16"/>
   <sheetViews>
@@ -841,653 +841,653 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:58" r="1">
-      <c t="s" r="A1">
+    <row r="1" spans="1:58">
+      <c r="A1" t="s">
         <v>80</v>
       </c>
-      <c t="s" r="B1">
+      <c r="B1" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="C1">
+      <c r="C1" t="s">
         <v>82</v>
       </c>
-      <c t="s" r="D1">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c t="s" r="E1">
+      <c r="E1" t="s">
         <v>136</v>
       </c>
-      <c t="s" r="F1">
+      <c r="F1" t="s">
         <v>110</v>
       </c>
-      <c t="s" r="G1">
+      <c r="G1" t="s">
         <v>107</v>
       </c>
-      <c t="s" r="H1">
+      <c r="H1" t="s">
         <v>127</v>
       </c>
-      <c t="s" r="I1">
+      <c r="I1" t="s">
         <v>83</v>
       </c>
-      <c t="s" r="J1">
+      <c r="J1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row spans="1:58" r="2">
-      <c t="s" r="A2">
+    <row r="2" spans="1:58">
+      <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c t="s" r="D2">
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>102</v>
       </c>
-      <c t="s" r="F2">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="G2">
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c t="s" r="H2">
+      <c r="H2" t="s">
         <v>65</v>
       </c>
-      <c t="s" r="I2">
+      <c r="I2" t="s">
         <v>128</v>
       </c>
-      <c t="s" r="J2">
+      <c r="J2" t="s">
         <v>119</v>
       </c>
-      <c t="s" r="K2">
+      <c r="K2" t="s">
         <v>108</v>
       </c>
-      <c t="s" r="L2">
+      <c r="L2" t="s">
         <v>42</v>
       </c>
-      <c t="s" r="M2">
+      <c r="M2" t="s">
         <v>52</v>
       </c>
-      <c t="s" r="O2">
-        <v>60</v>
-      </c>
-      <c t="s" r="P2">
+      <c r="O2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="Q2">
-        <v>60</v>
-      </c>
-      <c t="s" r="R2">
-        <v>60</v>
-      </c>
-      <c t="s" r="S2">
+      <c r="Q2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="T2">
-        <v>60</v>
-      </c>
-      <c t="s" r="U2">
-        <v>60</v>
-      </c>
-      <c t="s" r="V2">
+      <c r="T2" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="W2">
-        <v>60</v>
-      </c>
-      <c t="s" r="X2">
-        <v>60</v>
-      </c>
-      <c t="s" r="Y2">
+      <c r="W2" t="s">
+        <v>60</v>
+      </c>
+      <c r="X2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="Z2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AA2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AB2">
+      <c r="Z2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AC2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AD2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AE2">
+      <c r="AC2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AF2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AG2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AH2">
+      <c r="AF2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AI2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AJ2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AK2">
+      <c r="AI2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AL2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AM2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AN2">
+      <c r="AL2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AO2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AP2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AQ2">
+      <c r="AO2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AR2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AS2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AT2">
+      <c r="AR2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AU2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AV2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AW2">
+      <c r="AU2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW2" t="s">
         <v>73</v>
       </c>
-      <c t="s" r="AX2">
-        <v>60</v>
-      </c>
-      <c t="s" r="AZ2">
+      <c r="AX2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>133</v>
       </c>
-      <c t="s" r="BA2">
+      <c r="BA2" t="s">
         <v>56</v>
       </c>
-      <c t="s" r="BB2">
+      <c r="BB2" t="s">
         <v>34</v>
       </c>
-      <c t="s" r="BC2">
+      <c r="BC2" t="s">
         <v>109</v>
       </c>
-      <c t="s" r="BD2">
+      <c r="BD2" t="s">
         <v>66</v>
       </c>
-      <c t="s" r="BE2">
+      <c r="BE2" t="s">
         <v>99</v>
       </c>
-      <c t="s" r="BF2">
+      <c r="BF2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row spans="1:58" r="3">
-      <c t="s" r="A3">
+    <row r="3" spans="1:58">
+      <c r="A3" t="s">
         <v>105</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c t="s" r="C3">
+      <c r="C3" t="s">
         <v>112</v>
       </c>
-      <c t="s" r="D3">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c t="s" r="E3">
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c t="s" r="F3">
+      <c r="F3" t="s">
         <v>68</v>
       </c>
-      <c t="s" r="G3">
+      <c r="G3" t="s">
         <v>69</v>
       </c>
-      <c t="s" r="H3">
+      <c r="H3" t="s">
         <v>92</v>
       </c>
-      <c t="s" r="I3">
+      <c r="I3" t="s">
         <v>138</v>
       </c>
-      <c t="s" r="J3">
+      <c r="J3" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="K3">
+      <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c t="s" r="L3">
+      <c r="L3" t="s">
         <v>132</v>
       </c>
-      <c t="s" r="M3">
+      <c r="M3" t="s">
         <v>59</v>
       </c>
-      <c t="s" r="N3">
+      <c r="N3" t="s">
         <v>54</v>
       </c>
-      <c t="s" r="O3">
+      <c r="O3" t="s">
         <v>76</v>
       </c>
-      <c t="s" r="P3">
+      <c r="P3" t="s">
         <v>121</v>
       </c>
-      <c t="s" r="Q3">
+      <c r="Q3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row spans="1:58" r="4">
-      <c t="s" r="A4">
+    <row r="4" spans="1:58">
+      <c r="A4" t="s">
         <v>120</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>124</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>125</v>
       </c>
-      <c t="s" r="D4">
+      <c r="D4" t="s">
         <v>135</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>113</v>
       </c>
-      <c t="s" r="F4">
+      <c r="F4" t="s">
         <v>123</v>
       </c>
-      <c t="s" r="G4">
+      <c r="G4" t="s">
         <v>130</v>
       </c>
-      <c t="s" r="H4">
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="I4">
+      <c r="I4" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="J4">
+      <c r="J4" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="K4">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c t="s" r="L4">
+      <c r="L4" t="s">
         <v>126</v>
       </c>
-      <c t="s" r="M4">
+      <c r="M4" t="s">
         <v>86</v>
       </c>
-      <c t="s" r="N4">
+      <c r="N4" t="s">
         <v>39</v>
       </c>
-      <c t="s" r="O4">
+      <c r="O4" t="s">
         <v>48</v>
       </c>
-      <c t="s" r="P4">
+      <c r="P4" t="s">
         <v>78</v>
       </c>
-      <c t="s" r="Q4">
+      <c r="Q4" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="R4">
+      <c r="R4" t="s">
         <v>88</v>
       </c>
-      <c t="s" r="S4">
+      <c r="S4" t="s">
         <v>2</v>
       </c>
-      <c t="s" r="T4">
+      <c r="T4" t="s">
         <v>4</v>
       </c>
-      <c t="s" r="U4">
+      <c r="U4" t="s">
         <v>9</v>
       </c>
-      <c t="s" r="V4">
+      <c r="V4" t="s">
         <v>10</v>
       </c>
-      <c t="s" r="W4">
+      <c r="W4" t="s">
         <v>13</v>
       </c>
-      <c t="s" r="X4">
+      <c r="X4" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="Y4">
+      <c r="Y4" t="s">
         <v>11</v>
       </c>
-      <c t="s" r="Z4">
+      <c r="Z4" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="AA4">
+      <c r="AA4" t="s">
         <v>16</v>
       </c>
-      <c t="s" r="AB4">
+      <c r="AB4" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="AC4">
+      <c r="AC4" t="s">
         <v>5</v>
       </c>
-      <c t="s" r="AD4">
+      <c r="AD4" t="s">
         <v>12</v>
       </c>
-      <c t="s" r="AE4">
+      <c r="AE4" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="AF4">
+      <c r="AF4" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="AG4">
+      <c r="AG4" t="s">
         <v>78</v>
       </c>
-      <c t="s" r="AH4">
+      <c r="AH4" t="s">
         <v>3</v>
       </c>
-      <c t="s" r="AJ4">
+      <c r="AJ4" t="s">
         <v>53</v>
       </c>
-      <c t="s" r="AK4">
+      <c r="AK4" t="s">
         <v>87</v>
       </c>
-      <c t="s" r="AL4">
+      <c r="AL4" t="s">
         <v>122</v>
       </c>
-      <c t="s" r="AN4">
+      <c r="AN4" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="AO4">
+      <c r="AO4" t="s">
         <v>22</v>
       </c>
-      <c t="s" r="AP4">
+      <c r="AP4" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="AQ4">
+      <c r="AQ4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row spans="1:58" r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:58">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row spans="1:58" r="6">
-      <c t="s" r="A6">
+    <row r="6" spans="1:58">
+      <c r="A6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row spans="1:58" r="7">
-      <c t="s" r="A7">
+    <row r="7" spans="1:58">
+      <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c t="s" r="B7">
+      <c r="B7" t="s">
         <v>100</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row spans="1:58" r="8">
-      <c t="s" r="A8">
+    <row r="8" spans="1:58">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c t="s" r="B8">
+      <c r="B8" t="s">
         <v>124</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>125</v>
       </c>
-      <c t="s" r="D8">
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c t="s" r="F8">
+      <c r="F8" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="G8">
+      <c r="G8" t="s">
         <v>81</v>
       </c>
-      <c t="s" r="H8">
+      <c r="H8" t="s">
         <v>97</v>
       </c>
-      <c t="s" r="I8">
+      <c r="I8" t="s">
         <v>63</v>
       </c>
-      <c t="s" r="J8">
+      <c r="J8" t="s">
         <v>116</v>
       </c>
-      <c t="s" r="K8">
+      <c r="K8" t="s">
         <v>117</v>
       </c>
-      <c t="s" r="L8">
+      <c r="L8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row spans="1:58" r="9">
-      <c t="s" r="A9">
+    <row r="9" spans="1:58">
+      <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c t="s" r="B9">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>89</v>
       </c>
-      <c t="s" r="D9">
+      <c r="D9" t="s">
         <v>98</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>74</v>
       </c>
-      <c t="s" r="F9">
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="G9">
+      <c r="G9" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="H9">
+      <c r="H9" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="I9">
+      <c r="I9" t="s">
         <v>25</v>
       </c>
-      <c t="s" r="J9">
+      <c r="J9" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="K9">
+      <c r="K9" t="s">
         <v>111</v>
       </c>
-      <c t="s" r="L9">
+      <c r="L9" t="s">
         <v>140</v>
       </c>
-      <c t="s" r="M9">
+      <c r="M9" t="s">
         <v>140</v>
       </c>
-      <c t="s" r="N9">
+      <c r="N9" t="s">
         <v>75</v>
       </c>
-      <c t="s" r="O9">
+      <c r="O9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row spans="1:58" r="10">
-      <c t="s" r="A10">
+    <row r="10" spans="1:58">
+      <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c t="s" r="B10">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>131</v>
       </c>
-      <c t="s" r="D10">
+      <c r="D10" t="s">
         <v>144</v>
       </c>
-      <c t="s" r="E10">
+      <c r="E10" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="F10">
+      <c r="F10" t="s">
         <v>95</v>
       </c>
-      <c t="s" r="G10">
+      <c r="G10" t="s">
         <v>94</v>
       </c>
-      <c t="s" r="H10">
+      <c r="H10" t="s">
         <v>134</v>
       </c>
-      <c t="s" r="I10">
+      <c r="I10" t="s">
         <v>26</v>
       </c>
-      <c t="s" r="J10">
+      <c r="J10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row spans="1:58" r="11">
-      <c t="s" r="A11">
+    <row r="11" spans="1:58">
+      <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>129</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>139</v>
       </c>
-      <c t="s" r="D11">
+      <c r="D11" t="s">
         <v>137</v>
       </c>
-      <c t="s" r="E11">
+      <c r="E11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row spans="1:58" r="12">
-      <c t="s" r="A12">
+    <row r="12" spans="1:58">
+      <c r="A12" t="s">
         <v>70</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="D12">
+      <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="E12">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="F12">
+      <c r="F12" t="s">
         <v>1</v>
       </c>
-      <c t="s" r="I12">
+      <c r="I12" t="s">
         <v>55</v>
       </c>
-      <c t="s" r="J12">
+      <c r="J12" t="s">
         <v>71</v>
       </c>
-      <c t="s" r="K12">
+      <c r="K12" t="s">
         <v>43</v>
       </c>
-      <c t="s" r="L12">
+      <c r="L12" t="s">
         <v>45</v>
       </c>
-      <c t="s" r="M12">
+      <c r="M12" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="N12">
+      <c r="N12" t="s">
         <v>115</v>
       </c>
-      <c t="s" r="O12">
+      <c r="O12" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="P12">
+      <c r="P12" t="s">
         <v>46</v>
       </c>
-      <c t="s" r="Q12">
+      <c r="Q12" t="s">
         <v>44</v>
       </c>
-      <c t="s" r="R12">
+      <c r="R12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row spans="1:58" r="13">
-      <c t="s" r="A13">
+    <row r="13" spans="1:58">
+      <c r="A13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row spans="1:58" r="14">
-      <c t="s" r="A14">
+    <row r="14" spans="1:58">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c t="s" r="B14">
+      <c r="B14" t="s">
         <v>142</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C14" t="s">
         <v>143</v>
       </c>
-      <c t="s" r="D14">
+      <c r="D14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row spans="1:58" r="15">
-      <c t="s" r="B15">
+    <row r="15" spans="1:58">
+      <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="C15">
+      <c r="C15" t="s">
         <v>61</v>
       </c>
-      <c t="s" r="D15">
+      <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c t="s" r="E15">
+      <c r="E15" t="s">
         <v>114</v>
       </c>
-      <c t="s" r="F15">
+      <c r="F15" t="s">
         <v>118</v>
       </c>
-      <c t="s" r="G15">
+      <c r="G15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row spans="1:58" r="16">
-      <c t="s" r="B16">
+    <row r="16" spans="1:58">
+      <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="C16">
+      <c r="C16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="D16">
+      <c r="D16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="E16">
+      <c r="E16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="F16">
+      <c r="F16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="G16">
+      <c r="G16" t="s">
         <v>141</v>
       </c>
-      <c t="s" r="H16">
+      <c r="H16" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" header="0.5" footer="0.5" bottom="1" right="0.75" top="1"/>
+  <pageMargins header="0.5" footer="0.5" bottom="1" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Just mvoed around some things and added some output
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="308">
   <si>
     <t xml:space="preserve">
 </t>
@@ -99,6 +99,9 @@
     <t xml:space="preserve">
             Advanced Search…
         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve"> Follow OGC on Twitter</t>
@@ -1306,9 +1309,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -1318,114 +1321,114 @@
   <sheetData>
     <row spans="1:2" r="1">
       <c t="s" r="A1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c t="s" r="B1">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row spans="1:2" r="2">
       <c t="s" r="A2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c t="s" r="B2">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row spans="1:2" r="3">
       <c t="s" r="A3">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c t="s" r="B3">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row spans="1:2" r="4">
       <c t="s" r="A4">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c t="s" r="B4">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row spans="1:2" r="5">
       <c t="s" r="A5">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c t="s" r="B5">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row spans="1:2" r="6">
       <c t="s" r="A6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c t="s" r="B6">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row spans="1:2" r="7">
       <c t="s" r="A7">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c t="s" r="B7">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row spans="1:2" r="8">
       <c t="s" r="A8">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c t="s" r="B8">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row spans="1:2" r="9">
       <c t="s" r="A9">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c t="s" r="B9">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row spans="1:2" r="10">
       <c t="s" r="A10">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c t="s" r="B10">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row spans="1:2" r="11">
       <c t="s" r="A11">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c t="s" r="B11">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row spans="1:2" r="12">
       <c t="s" r="A12">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c t="s" r="B12">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row spans="1:2" r="13">
       <c t="s" r="A13">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c t="s" r="B13">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row spans="1:2" r="14">
       <c t="s" r="A14">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c t="s" r="B14">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row spans="1:2" r="15">
@@ -1433,18 +1436,23 @@
         <v>1</v>
       </c>
       <c t="s" r="B15">
-        <v>126</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row spans="1:2" r="16">
+      <c t="s" r="A16">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" left="0.75" top="1" footer="0.5" right="0.75" bottom="1"/>
+  <pageMargins header="0.5" top="1" left="0.75" footer="0.5" right="0.75" bottom="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:B196"/>
   <sheetViews>
@@ -1456,616 +1464,616 @@
   <sheetData>
     <row spans="1:2" r="2">
       <c t="s" r="B2">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row spans="1:2" r="3">
       <c t="s" r="A3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c t="s" r="B3">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row spans="1:2" r="4">
       <c t="s" r="A4">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c t="s" r="B4">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row spans="1:2" r="5">
       <c t="s" r="A5">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c t="s" r="B5">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row spans="1:2" r="6">
       <c t="s" r="A6">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c t="s" r="B6">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row spans="1:2" r="7">
       <c t="s" r="A7">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c t="s" r="B7">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row spans="1:2" r="8">
       <c t="s" r="A8">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c t="s" r="B8">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row spans="1:2" r="9">
       <c t="s" r="A9">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c t="s" r="B9">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row spans="1:2" r="10">
       <c t="s" r="A10">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c t="s" r="B10">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row spans="1:2" r="11">
       <c t="s" r="A11">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c t="s" r="B11">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row spans="1:2" r="13">
       <c t="s" r="B13">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row spans="1:2" r="14">
       <c t="s" r="B14">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row spans="1:2" r="15">
       <c t="s" r="A15">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c t="s" r="B15">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row spans="1:2" r="16">
       <c t="s" r="A16">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c t="s" r="B16">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row spans="1:2" r="17">
       <c t="s" r="A17">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c t="s" r="B17">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row spans="1:2" r="18">
       <c t="s" r="A18">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c t="s" r="B18">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row spans="1:2" r="19">
       <c t="s" r="A19">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c t="s" r="B19">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row spans="1:2" r="20">
       <c t="s" r="A20">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c t="s" r="B20">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row spans="1:2" r="21">
       <c t="s" r="A21">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c t="s" r="B21">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row spans="1:2" r="22">
       <c t="s" r="A22">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c t="s" r="B22">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row spans="1:2" r="23">
       <c t="s" r="A23">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c t="s" r="B23">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row spans="1:2" r="24">
       <c t="s" r="A24">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c t="s" r="B24">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row spans="1:2" r="25">
       <c t="s" r="A25">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c t="s" r="B25">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row spans="1:2" r="26">
       <c t="s" r="B26">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row spans="1:2" r="27">
       <c t="s" r="A27">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B27">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row spans="1:2" r="28">
       <c t="s" r="A28">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B28">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row spans="1:2" r="29">
       <c t="s" r="A29">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B29">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row spans="1:2" r="30">
       <c t="s" r="A30">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B30">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row spans="1:2" r="31">
       <c t="s" r="A31">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B31">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row spans="1:2" r="32">
       <c t="s" r="A32">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B32">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row spans="1:2" r="33">
       <c t="s" r="A33">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B33">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row spans="1:2" r="34">
       <c t="s" r="A34">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B34">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row spans="1:2" r="35">
       <c t="s" r="A35">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B35">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row spans="1:2" r="36">
       <c t="s" r="A36">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B36">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row spans="1:2" r="37">
       <c t="s" r="A37">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B37">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row spans="1:2" r="38">
       <c t="s" r="A38">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B38">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row spans="1:2" r="39">
       <c t="s" r="A39">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B39">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row spans="1:2" r="40">
       <c t="s" r="A40">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B40">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row spans="1:2" r="41">
       <c t="s" r="A41">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B41">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row spans="1:2" r="42">
       <c t="s" r="A42">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B42">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row spans="1:2" r="43">
       <c t="s" r="A43">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B43">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row spans="1:2" r="44">
       <c t="s" r="A44">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B44">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row spans="1:2" r="45">
       <c t="s" r="A45">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B45">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row spans="1:2" r="46">
       <c t="s" r="A46">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B46">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row spans="1:2" r="47">
       <c t="s" r="A47">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B47">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row spans="1:2" r="48">
       <c t="s" r="A48">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B48">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row spans="1:2" r="49">
       <c t="s" r="A49">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B49">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row spans="1:2" r="50">
       <c t="s" r="A50">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B50">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row spans="1:2" r="51">
       <c t="s" r="A51">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B51">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row spans="1:2" r="52">
       <c t="s" r="A52">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B52">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row spans="1:2" r="53">
       <c t="s" r="A53">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B53">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row spans="1:2" r="54">
       <c t="s" r="A54">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B54">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row spans="1:2" r="55">
       <c t="s" r="A55">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B55">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row spans="1:2" r="56">
       <c t="s" r="A56">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B56">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row spans="1:2" r="57">
       <c t="s" r="A57">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c t="s" r="B57">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row spans="1:2" r="58">
       <c t="s" r="A58">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="B58">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row spans="1:2" r="60">
       <c t="s" r="B60">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row spans="1:2" r="61">
       <c t="s" r="A61">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c t="s" r="B61">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row spans="1:2" r="62">
       <c t="s" r="A62">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c t="s" r="B62">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row spans="1:2" r="63">
       <c t="s" r="A63">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c t="s" r="B63">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row spans="1:2" r="64">
       <c t="s" r="A64">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c t="s" r="B64">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row spans="1:2" r="65">
       <c t="s" r="A65">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c t="s" r="B65">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row spans="1:2" r="66">
       <c t="s" r="A66">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c t="s" r="B66">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row spans="1:2" r="67">
       <c t="s" r="A67">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c t="s" r="B67">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row spans="1:2" r="68">
       <c t="s" r="A68">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c t="s" r="B68">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row spans="1:2" r="69">
       <c t="s" r="A69">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c t="s" r="B69">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row spans="1:2" r="70">
       <c t="s" r="A70">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c t="s" r="B70">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row spans="1:2" r="71">
       <c t="s" r="A71">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c t="s" r="B71">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row spans="1:2" r="72">
       <c t="s" r="A72">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c t="s" r="B72">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row spans="1:2" r="73">
       <c t="s" r="A73">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c t="s" r="B73">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row spans="1:2" r="74">
       <c t="s" r="A74">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c t="s" r="B74">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row spans="1:2" r="75">
       <c t="s" r="A75">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c t="s" r="B75">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row spans="1:2" r="77">
       <c t="s" r="B77">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row spans="1:2" r="78">
       <c t="s" r="A78">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c t="s" r="B78">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row spans="1:2" r="79">
       <c t="s" r="A79">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c t="s" r="B79">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row spans="1:2" r="80">
       <c t="s" r="A80">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c t="s" r="B80">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row spans="1:2" r="81">
       <c t="s" r="A81">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c t="s" r="B81">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row spans="1:2" r="82">
       <c t="s" r="A82">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" r="B82">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row spans="1:2" r="83">
       <c t="s" r="A83">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c t="s" r="B83">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row spans="1:2" r="84">
@@ -2073,7 +2081,7 @@
         <v>16</v>
       </c>
       <c t="s" r="B84">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row spans="1:2" r="85">
@@ -2081,79 +2089,79 @@
         <v>0</v>
       </c>
       <c t="s" r="B85">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row spans="1:2" r="86">
       <c t="s" r="A86">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c t="s" r="B86">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row spans="1:2" r="87">
       <c t="s" r="A87">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c t="s" r="B87">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row spans="1:2" r="88">
       <c t="s" r="A88">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c t="s" r="B88">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row spans="1:2" r="89">
       <c t="s" r="A89">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c t="s" r="B89">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row spans="1:2" r="90">
       <c t="s" r="A90">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c t="s" r="B90">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row spans="1:2" r="91">
       <c t="s" r="A91">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c t="s" r="B91">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row spans="1:2" r="92">
       <c t="s" r="A92">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c t="s" r="B92">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row spans="1:2" r="93">
       <c t="s" r="A93">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c t="s" r="B93">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row spans="1:2" r="94">
       <c t="s" r="A94">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c t="s" r="B94">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row spans="1:2" r="95">
@@ -2161,7 +2169,7 @@
         <v>2</v>
       </c>
       <c t="s" r="B95">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row spans="1:2" r="96">
@@ -2169,7 +2177,7 @@
         <v>3</v>
       </c>
       <c t="s" r="B96">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row spans="1:2" r="97">
@@ -2177,7 +2185,7 @@
         <v>8</v>
       </c>
       <c t="s" r="B97">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row spans="1:2" r="98">
@@ -2185,7 +2193,7 @@
         <v>9</v>
       </c>
       <c t="s" r="B98">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row spans="1:2" r="99">
@@ -2193,7 +2201,7 @@
         <v>12</v>
       </c>
       <c t="s" r="B99">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row spans="1:2" r="100">
@@ -2201,7 +2209,7 @@
         <v>6</v>
       </c>
       <c t="s" r="B100">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row spans="1:2" r="101">
@@ -2209,7 +2217,7 @@
         <v>10</v>
       </c>
       <c t="s" r="B101">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row spans="1:2" r="102">
@@ -2217,7 +2225,7 @@
         <v>7</v>
       </c>
       <c t="s" r="B102">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row spans="1:2" r="103">
@@ -2225,7 +2233,7 @@
         <v>15</v>
       </c>
       <c t="s" r="B103">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row spans="1:2" r="104">
@@ -2233,7 +2241,7 @@
         <v>14</v>
       </c>
       <c t="s" r="B104">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row spans="1:2" r="105">
@@ -2241,7 +2249,7 @@
         <v>4</v>
       </c>
       <c t="s" r="B105">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row spans="1:2" r="106">
@@ -2249,7 +2257,7 @@
         <v>11</v>
       </c>
       <c t="s" r="B106">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row spans="1:2" r="107">
@@ -2257,7 +2265,7 @@
         <v>5</v>
       </c>
       <c t="s" r="B107">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row spans="1:2" r="108">
@@ -2265,113 +2273,113 @@
         <v>13</v>
       </c>
       <c t="s" r="B108">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row spans="1:2" r="110">
       <c t="s" r="B110">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row spans="1:2" r="112">
       <c t="s" r="B112">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row spans="1:2" r="113">
       <c t="s" r="B113">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row spans="1:2" r="114">
       <c t="s" r="B114">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row spans="1:2" r="115">
       <c t="s" r="B115">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row spans="1:2" r="116">
       <c t="s" r="B116">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row spans="1:2" r="117">
       <c t="s" r="B117">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row spans="1:2" r="118">
       <c t="s" r="B118">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row spans="1:2" r="120">
       <c t="s" r="B120">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row spans="1:2" r="121">
       <c t="s" r="A121">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c t="s" r="B121">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row spans="1:2" r="122">
       <c t="s" r="A122">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c t="s" r="B122">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row spans="1:2" r="123">
       <c t="s" r="A123">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c t="s" r="B123">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row spans="1:2" r="125">
       <c t="s" r="B125">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row spans="1:2" r="126">
       <c t="s" r="A126">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c t="s" r="B126">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row spans="1:2" r="127">
       <c t="s" r="A127">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c t="s" r="B127">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row spans="1:2" r="128">
       <c t="s" r="A128">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c t="s" r="B128">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row spans="1:2" r="129">
       <c t="s" r="A129">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c t="s" r="B129">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row spans="1:2" r="130">
@@ -2379,15 +2387,15 @@
         <v>1</v>
       </c>
       <c t="s" r="B130">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row spans="1:2" r="131">
       <c t="s" r="A131">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c t="s" r="B131">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row spans="1:2" r="132">
@@ -2395,203 +2403,203 @@
         <v>1</v>
       </c>
       <c t="s" r="B132">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row spans="1:2" r="133">
       <c t="s" r="A133">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c t="s" r="B133">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row spans="1:2" r="134">
       <c t="s" r="A134">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c t="s" r="B134">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row spans="1:2" r="135">
       <c t="s" r="A135">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c t="s" r="B135">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row spans="1:2" r="136">
       <c t="s" r="A136">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c t="s" r="B136">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row spans="1:2" r="137">
       <c t="s" r="A137">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c t="s" r="B137">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row spans="1:2" r="139">
       <c t="s" r="B139">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row spans="1:2" r="140">
       <c t="s" r="A140">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c t="s" r="B140">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row spans="1:2" r="141">
       <c t="s" r="A141">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c t="s" r="B141">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row spans="1:2" r="142">
       <c t="s" r="A142">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c t="s" r="B142">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row spans="1:2" r="143">
       <c t="s" r="A143">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c t="s" r="B143">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row spans="1:2" r="144">
       <c t="s" r="A144">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c t="s" r="B144">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row spans="1:2" r="145">
       <c t="s" r="A145">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c t="s" r="B145">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row spans="1:2" r="146">
       <c t="s" r="A146">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c t="s" r="B146">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row spans="1:2" r="147">
       <c t="s" r="A147">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c t="s" r="B147">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row spans="1:2" r="148">
       <c t="s" r="A148">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c t="s" r="B148">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row spans="1:2" r="149">
       <c t="s" r="A149">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c t="s" r="B149">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row spans="1:2" r="151">
       <c t="s" r="B151">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row spans="1:2" r="152">
       <c t="s" r="A152">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c t="s" r="B152">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row spans="1:2" r="153">
       <c t="s" r="A153">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c t="s" r="B153">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row spans="1:2" r="154">
       <c t="s" r="A154">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="B154">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row spans="1:2" r="155">
       <c t="s" r="A155">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c t="s" r="B155">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row spans="1:2" r="156">
       <c t="s" r="B156">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row spans="1:2" r="157">
       <c t="s" r="A157">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" r="B157">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row spans="1:2" r="159">
       <c t="s" r="B159">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row spans="1:2" r="160">
       <c t="s" r="A160">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c t="s" r="B160">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row spans="1:2" r="161">
       <c t="s" r="A161">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c t="s" r="B161">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row spans="1:2" r="162">
@@ -2599,7 +2607,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B162">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row spans="1:2" r="163">
@@ -2607,7 +2615,7 @@
         <v>1</v>
       </c>
       <c t="s" r="B163">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row spans="1:2" r="164">
@@ -2615,213 +2623,213 @@
         <v>1</v>
       </c>
       <c t="s" r="B164">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row spans="1:2" r="165">
       <c t="s" r="B165">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row spans="1:2" r="166">
       <c t="s" r="B166">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row spans="1:2" r="167">
       <c t="s" r="A167">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c t="s" r="B167">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row spans="1:2" r="168">
       <c t="s" r="A168">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c t="s" r="B168">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row spans="1:2" r="169">
       <c t="s" r="A169">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c t="s" r="B169">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row spans="1:2" r="170">
       <c t="s" r="A170">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c t="s" r="B170">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row spans="1:2" r="171">
       <c t="s" r="A171">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c t="s" r="B171">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row spans="1:2" r="172">
       <c t="s" r="A172">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c t="s" r="B172">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row spans="1:2" r="173">
       <c t="s" r="A173">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c t="s" r="B173">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row spans="1:2" r="174">
       <c t="s" r="A174">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c t="s" r="B174">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row spans="1:2" r="175">
       <c t="s" r="A175">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c t="s" r="B175">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row spans="1:2" r="176">
       <c t="s" r="A176">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c t="s" r="B176">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row spans="1:2" r="177">
       <c t="s" r="A177">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c t="s" r="B177">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row spans="1:2" r="179">
       <c t="s" r="B179">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row spans="1:2" r="180">
       <c t="s" r="A180">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c t="s" r="B180">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row spans="1:2" r="182">
       <c t="s" r="B182">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row spans="1:2" r="183">
       <c t="s" r="A183">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c t="s" r="B183">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row spans="1:2" r="184">
       <c t="s" r="A184">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c t="s" r="B184">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row spans="1:2" r="185">
       <c t="s" r="B185">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row spans="1:2" r="187">
       <c t="s" r="B187">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row spans="1:2" r="188">
       <c t="s" r="A188">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c t="s" r="B188">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row spans="1:2" r="189">
       <c t="s" r="A189">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c t="s" r="B189">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row spans="1:2" r="190">
       <c t="s" r="A190">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c t="s" r="B190">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row spans="1:2" r="191">
       <c t="s" r="A191">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c t="s" r="B191">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row spans="1:2" r="192">
       <c t="s" r="A192">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c t="s" r="B192">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row spans="1:2" r="193">
       <c t="s" r="A193">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c t="s" r="B193">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row spans="1:2" r="195">
       <c t="s" r="B195">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row spans="1:2" r="196">
       <c t="s" r="A196">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c t="s" r="B196">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" left="0.75" top="1" footer="0.5" right="0.75" bottom="1"/>
+  <pageMargins header="0.5" top="1" left="0.75" footer="0.5" right="0.75" bottom="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added headers and source link indication
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="304">
   <si>
     <t xml:space="preserve">
 </t>
@@ -357,9 +357,6 @@
     <t>Report suspected fraud</t>
   </si>
   <si>
-    <t>Review</t>
-  </si>
-  <si>
     <t>SAEON</t>
   </si>
   <si>
@@ -648,12 +645,6 @@
     <t>http://www.earth-syst-sci-data-discuss.net/5/187/2012/essdd-5-187-2012-discussion.html</t>
   </si>
   <si>
-    <t>http://www.earth-syst-sci-data-discuss.net/5/221/2012/essdd-5-221-2012-discussion.html</t>
-  </si>
-  <si>
-    <t>http://www.earth-syst-sci-data-discuss.net/5/243/2012/essdd-5-243-2012-discussion.html</t>
-  </si>
-  <si>
     <t>http://www.earth-syst-sci-data-discuss.net/5/301/2012/essdd-5-301-2012-discussion.html</t>
   </si>
   <si>
@@ -693,9 +684,6 @@
     <t>http://www.earth-syst-sci-data.net/4/47/2012/essd-4-47-2012.html</t>
   </si>
   <si>
-    <t>http://www.earth-syst-sci-data.net/4/75/2012/essd-4-75-2012.html</t>
-  </si>
-  <si>
     <t>http://www.earth-syst-sci-data.net/5/109/2013/essd-5-109-2013.html</t>
   </si>
   <si>
@@ -756,13 +744,7 @@
     <t>http://www.earth-system-science-data.net/index.html</t>
   </si>
   <si>
-    <t>http://www.earth-system-science-data.net/pr_copernicus_article_level_metrics.pdf</t>
-  </si>
-  <si>
     <t>http://www.earth-system-science-data.net/production.html</t>
-  </si>
-  <si>
-    <t>http://www.earth-system-science-data.net/review/review_process_and_interactive_public_discussion.html</t>
   </si>
   <si>
     <t>http://www.earth-system-science-data.net/submission/manuscript_submission.html</t>
@@ -989,13 +971,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="00000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -1018,8 +1007,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1313,24 +1303,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>115</v>
+      <c r="A1" t="s" s="1">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1338,7 +1328,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1346,7 +1336,7 @@
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1354,7 +1344,7 @@
         <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1362,15 +1352,15 @@
         <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1378,15 +1368,15 @@
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1394,7 +1384,7 @@
         <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1402,7 +1392,7 @@
         <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1410,7 +1400,7 @@
         <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1418,7 +1408,7 @@
         <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1426,7 +1416,7 @@
         <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1434,7 +1424,7 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1442,7 +1432,7 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1451,37 +1441,37 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" top="1" left="0.75" bottom="1"/>
+  <pageMargins bottom="1" left="0.75" header="0.5" footer="0.5" top="1" right="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" t="s">
-        <v>115</v>
+      <c r="A1" t="s" s="1">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" t="s">
-        <v>308</v>
+        <v>164</v>
+      </c>
+      <c r="C2" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1489,7 +1479,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1497,7 +1487,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1505,15 +1495,15 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1521,7 +1511,7 @@
         <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1529,15 +1519,15 @@
         <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1545,7 +1535,7 @@
         <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1553,20 +1543,20 @@
         <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="B13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C13" t="s">
-        <v>308</v>
+        <v>203</v>
+      </c>
+      <c r="C13" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1574,7 +1564,7 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1582,7 +1572,7 @@
         <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1590,7 +1580,7 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1598,7 +1588,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1606,7 +1596,7 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1614,68 +1604,68 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1683,23 +1673,23 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1707,23 +1697,23 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1731,7 +1721,7 @@
         <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1739,23 +1729,23 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1768,15 +1758,15 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
         <v>202</v>
@@ -1787,23 +1777,23 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1811,23 +1801,23 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1835,23 +1825,23 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1864,255 +1854,255 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>63</v>
-      </c>
       <c r="B55" t="s">
-        <v>226</v>
+        <v>261</v>
+      </c>
+      <c r="C55" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>227</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B58" t="s">
-        <v>238</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
       <c r="B60" t="s">
-        <v>267</v>
-      </c>
-      <c r="C60" t="s">
-        <v>308</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>302</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>298</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B65" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B66" t="s">
-        <v>244</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>256</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="B69" t="s">
-        <v>187</v>
+        <v>290</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="B70" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>51</v>
-      </c>
-      <c r="B71" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>47</v>
-      </c>
       <c r="B72" t="s">
-        <v>190</v>
+        <v>264</v>
+      </c>
+      <c r="C72" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
-        <v>296</v>
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
         <v>103</v>
       </c>
-      <c r="B75" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
       <c r="B77" t="s">
-        <v>270</v>
-      </c>
-      <c r="C77" t="s">
-        <v>308</v>
+        <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="B81" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B83" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="B84" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B85" t="s">
         <v>269</v>
@@ -2120,7 +2110,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B86" t="s">
         <v>279</v>
@@ -2128,767 +2118,727 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="B87" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="B88" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>292</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B94" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B95" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B96" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>276</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B99" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B100" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>293</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B103" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>14</v>
-      </c>
-      <c r="B104" t="s">
-        <v>253</v>
+        <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>4</v>
-      </c>
       <c r="B105" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>11</v>
-      </c>
-      <c r="B106" t="s">
-        <v>180</v>
+        <v>188</v>
+      </c>
+      <c r="C105" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>5</v>
-      </c>
       <c r="B107" t="s">
-        <v>297</v>
+        <v>239</v>
+      </c>
+      <c r="C107" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>13</v>
-      </c>
       <c r="B108" t="s">
-        <v>301</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="B109" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="B110" t="s">
-        <v>189</v>
-      </c>
-      <c r="C110" t="s">
-        <v>308</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="B111" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="B112" t="s">
-        <v>245</v>
-      </c>
-      <c r="C112" t="s">
-        <v>308</v>
+        <v>246</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="B113" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="B114" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="B115" t="s">
-        <v>241</v>
+        <v>248</v>
+      </c>
+      <c r="C115" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>86</v>
+      </c>
       <c r="B116" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
     </row>
     <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>87</v>
+      </c>
       <c r="B117" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
       <c r="B118" t="s">
-        <v>247</v>
+        <v>294</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="B120" t="s">
-        <v>254</v>
-      </c>
-      <c r="C120" t="s">
-        <v>308</v>
+        <v>174</v>
+      </c>
+      <c r="C120" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="B121" t="s">
-        <v>268</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B122" t="s">
-        <v>255</v>
+        <v>171</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="B123" t="s">
-        <v>300</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>64</v>
+      </c>
+      <c r="B124" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>1</v>
+      </c>
       <c r="B125" t="s">
-        <v>175</v>
-      </c>
-      <c r="C125" t="s">
-        <v>308</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B126" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="B127" t="s">
-        <v>172</v>
+        <v>293</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B128" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="B129" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
+        <v>175</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B132" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" t="s">
-        <v>95</v>
-      </c>
-      <c r="B133" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" t="s">
-        <v>123</v>
-      </c>
       <c r="B134" t="s">
-        <v>154</v>
+        <v>257</v>
+      </c>
+      <c r="C134" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
+        <v>23</v>
+      </c>
+      <c r="B135" t="s">
         <v>123</v>
-      </c>
-      <c r="B135" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B136" t="s">
-        <v>176</v>
+        <v>260</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>74</v>
+        <v>300</v>
       </c>
       <c r="B137" t="s">
-        <v>178</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>21</v>
+      </c>
+      <c r="B138" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>83</v>
+      </c>
       <c r="B139" t="s">
-        <v>263</v>
-      </c>
-      <c r="C139" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B140" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B141" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>306</v>
+        <v>19</v>
       </c>
       <c r="B142" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B143" t="s">
-        <v>305</v>
+        <v>183</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B144" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" t="s">
-        <v>82</v>
-      </c>
-      <c r="B145" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" t="s">
-        <v>116</v>
-      </c>
       <c r="B146" t="s">
-        <v>264</v>
+        <v>252</v>
+      </c>
+      <c r="C146" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="B147" t="s">
-        <v>249</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="B148" t="s">
-        <v>184</v>
+        <v>256</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="B149" t="s">
-        <v>265</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>42</v>
+      </c>
+      <c r="B150" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="B151" t="s">
-        <v>258</v>
-      </c>
-      <c r="C151" t="s">
-        <v>308</v>
+        <v>254</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B152" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" t="s">
-        <v>122</v>
-      </c>
-      <c r="B153" t="s">
-        <v>262</v>
+        <v>184</v>
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" t="s">
-        <v>120</v>
-      </c>
       <c r="B154" t="s">
-        <v>261</v>
+        <v>158</v>
+      </c>
+      <c r="C154" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B155" t="s">
-        <v>259</v>
+        <v>133</v>
       </c>
     </row>
     <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>50</v>
+      </c>
       <c r="B156" t="s">
-        <v>260</v>
+        <v>134</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>114</v>
+        <v>1</v>
       </c>
       <c r="B157" t="s">
-        <v>185</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>1</v>
+      </c>
+      <c r="B158" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>1</v>
+      </c>
       <c r="B159" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="B160" t="s">
         <v>159</v>
       </c>
-      <c r="C159" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" t="s">
-        <v>67</v>
-      </c>
-      <c r="B160" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" t="s">
-        <v>50</v>
-      </c>
       <c r="B161" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B162" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="B163" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B164" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>39</v>
+      </c>
       <c r="B165" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>43</v>
+      </c>
       <c r="B166" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="B167" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B168" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B169" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B170" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B171" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="B172" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" t="s">
-        <v>30</v>
-      </c>
-      <c r="B173" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" t="s">
-        <v>40</v>
-      </c>
       <c r="B174" t="s">
-        <v>144</v>
+        <v>125</v>
+      </c>
+      <c r="C174" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B175" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" t="s">
-        <v>29</v>
-      </c>
-      <c r="B176" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" t="s">
-        <v>31</v>
-      </c>
       <c r="B177" t="s">
-        <v>152</v>
+        <v>298</v>
+      </c>
+      <c r="C177" t="s" s="1">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>191</v>
+      </c>
+      <c r="B178" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>303</v>
+      </c>
       <c r="B179" t="s">
-        <v>126</v>
-      </c>
-      <c r="C179" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" t="s">
-        <v>35</v>
-      </c>
       <c r="B180" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="B182" t="s">
-        <v>304</v>
-      </c>
-      <c r="C182" t="s">
-        <v>308</v>
+        <v>127</v>
+      </c>
+      <c r="C182" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>192</v>
+        <v>50</v>
       </c>
       <c r="B183" t="s">
-        <v>192</v>
+        <v>139</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>309</v>
+        <v>53</v>
       </c>
       <c r="B184" t="s">
-        <v>303</v>
+        <v>138</v>
       </c>
     </row>
     <row r="185" spans="1:3">
+      <c r="A185" t="s">
+        <v>54</v>
+      </c>
       <c r="B185" t="s">
-        <v>170</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
+        <v>98</v>
+      </c>
+      <c r="B186" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>100</v>
+      </c>
       <c r="B187" t="s">
-        <v>128</v>
-      </c>
-      <c r="C187" t="s">
-        <v>308</v>
+        <v>135</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B188" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" t="s">
-        <v>53</v>
-      </c>
-      <c r="B189" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>54</v>
-      </c>
       <c r="B190" t="s">
-        <v>138</v>
+        <v>128</v>
+      </c>
+      <c r="C190" t="s" s="1">
+        <v>302</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="B191" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="A192" t="s">
-        <v>100</v>
-      </c>
-      <c r="B192" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
-      <c r="A193" t="s">
-        <v>79</v>
-      </c>
-      <c r="B193" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="B195" t="s">
-        <v>129</v>
-      </c>
-      <c r="C195" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196" t="s">
-        <v>50</v>
-      </c>
-      <c r="B196" t="s">
-        <v>137</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins header="0.5" right="0.75" footer="0.5" top="1" left="0.75" bottom="1"/>
+  <pageMargins bottom="1" left="0.75" header="0.5" footer="0.5" top="1" right="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Title, label, URL, and organization columns working in Excel First Run.
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -83,13 +83,13 @@
     <t>Label</t>
   </si>
   <si>
+    <t>Org 1</t>
+  </si>
+  <si>
+    <t>Org 2</t>
+  </si>
+  <si>
     <t>Organization</t>
-  </si>
-  <si>
-    <t>Sheet 1</t>
-  </si>
-  <si>
-    <t>Sheet 2</t>
   </si>
   <si>
     <t>Support Center</t>
@@ -535,71 +535,83 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row spans="1:4" r="1">
-      <c s="1" r="A1" t="s">
+      <c s="1" t="s" r="A1">
         <v>25</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c s="1" t="s" r="B1">
         <v>18</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c s="1" t="s" r="C1">
         <v>26</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c s="1" t="s" r="D1">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:4" r="2">
+      <c t="s" r="A2">
+        <v>10</v>
+      </c>
+      <c t="s" r="B2">
+        <v>7</v>
+      </c>
+      <c t="s" r="C2">
+        <v>37</v>
+      </c>
+      <c t="s" r="D2">
+        <v>7</v>
+      </c>
+    </row>
+    <row spans="1:4" r="3">
+      <c t="s" r="A3">
+        <v>8</v>
+      </c>
+      <c t="s" r="B3">
         <v>19</v>
       </c>
-    </row>
-    <row spans="1:4" r="2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row spans="1:4" r="3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+      <c t="s" r="C3">
+        <v>38</v>
+      </c>
+      <c t="s" r="D3">
+        <v>19</v>
+      </c>
+    </row>
+    <row spans="1:4" r="4">
+      <c t="s" r="A4">
+        <v>9</v>
+      </c>
+      <c t="s" r="B4">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row spans="1:4" r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
+      <c t="s" r="C4">
         <v>39</v>
       </c>
+      <c t="s" r="D4">
+        <v>20</v>
+      </c>
     </row>
     <row spans="1:4" r="5">
-      <c r="A5" t="s">
+      <c t="s" r="A5">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c t="s" r="B5">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c t="s" r="C5">
         <v>50</v>
       </c>
+      <c t="s" r="D5">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins top="1" footer="0.5" header="0.5" left="0.75" bottom="1" right="0.75"/>
+  <pageMargins right="0.75" bottom="1" left="0.75" header="0.5" top="1" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -611,196 +623,196 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row spans="1:3" r="1">
-      <c s="1" r="A1" t="s">
+      <c s="1" t="s" r="A1">
         <v>25</v>
       </c>
-      <c s="1" r="B1" t="s">
+      <c s="1" t="s" r="B1">
         <v>26</v>
       </c>
     </row>
     <row spans="1:3" r="2">
-      <c r="B2" t="s">
+      <c t="s" r="B2">
         <v>38</v>
       </c>
-      <c s="1" r="C2" t="s">
+      <c s="1" t="s" r="C2">
         <v>54</v>
       </c>
     </row>
     <row spans="1:3" r="3">
-      <c r="A3" t="s">
+      <c t="s" r="A3">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c t="s" r="B3">
         <v>42</v>
       </c>
     </row>
     <row spans="1:3" r="4">
-      <c r="A4" t="s">
+      <c t="s" r="A4">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c t="s" r="B4">
         <v>52</v>
       </c>
     </row>
     <row spans="1:3" r="6">
-      <c r="B6" t="s">
+      <c t="s" r="B6">
         <v>39</v>
       </c>
-      <c s="1" r="C6" t="s">
+      <c s="1" t="s" r="C6">
         <v>54</v>
       </c>
     </row>
     <row spans="1:3" r="7">
-      <c r="A7" t="s">
+      <c t="s" r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c t="s" r="B7">
         <v>36</v>
       </c>
     </row>
     <row spans="1:3" r="8">
-      <c r="A8" t="s">
+      <c t="s" r="A8">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c t="s" r="B8">
         <v>53</v>
       </c>
     </row>
     <row spans="1:3" r="10">
-      <c r="B10" t="s">
+      <c t="s" r="B10">
         <v>50</v>
       </c>
-      <c s="1" r="C10" t="s">
+      <c s="1" t="s" r="C10">
         <v>54</v>
       </c>
     </row>
     <row spans="1:3" r="11">
-      <c r="A11" t="s">
+      <c t="s" r="A11">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c t="s" r="B11">
         <v>35</v>
       </c>
     </row>
     <row spans="1:3" r="12">
-      <c r="A12" t="s">
+      <c t="s" r="A12">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c t="s" r="B12">
         <v>45</v>
       </c>
     </row>
     <row spans="1:3" r="13">
-      <c r="A13" t="s">
+      <c t="s" r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c t="s" r="B13">
         <v>40</v>
       </c>
     </row>
     <row spans="1:3" r="14">
-      <c r="A14" t="s">
+      <c t="s" r="A14">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c t="s" r="B14">
         <v>43</v>
       </c>
     </row>
     <row spans="1:3" r="15">
-      <c r="A15" t="s">
+      <c t="s" r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c t="s" r="B15">
         <v>47</v>
       </c>
     </row>
     <row spans="1:3" r="16">
-      <c r="A16" t="s">
+      <c t="s" r="A16">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c t="s" r="B16">
         <v>34</v>
       </c>
     </row>
     <row spans="1:3" r="17">
-      <c r="A17" t="s">
+      <c t="s" r="A17">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
+      <c t="s" r="B17">
         <v>41</v>
       </c>
     </row>
     <row spans="1:3" r="18">
-      <c r="A18" t="s">
+      <c t="s" r="A18">
         <v>0</v>
       </c>
-      <c r="B18" t="s">
+      <c t="s" r="B18">
         <v>48</v>
       </c>
     </row>
     <row spans="1:3" r="19">
-      <c r="A19" t="s">
+      <c t="s" r="A19">
         <v>2</v>
       </c>
-      <c r="B19" t="s">
+      <c t="s" r="B19">
         <v>49</v>
       </c>
     </row>
     <row spans="1:3" r="20">
-      <c r="A20" t="s">
+      <c t="s" r="A20">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
+      <c t="s" r="B20">
         <v>51</v>
       </c>
     </row>
     <row spans="1:3" r="21">
-      <c r="A21" t="s">
+      <c t="s" r="A21">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c t="s" r="B21">
         <v>46</v>
       </c>
     </row>
     <row spans="1:3" r="22">
-      <c r="A22" t="s">
+      <c t="s" r="A22">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
+      <c t="s" r="B22">
         <v>44</v>
       </c>
     </row>
     <row spans="1:3" r="23">
-      <c r="A23" t="s">
+      <c t="s" r="A23">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
+      <c t="s" r="B23">
         <v>33</v>
       </c>
     </row>
     <row spans="1:3" r="24">
-      <c r="A24" t="s">
+      <c t="s" r="A24">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c t="s" r="B24">
         <v>32</v>
       </c>
     </row>
     <row spans="1:3" r="25">
-      <c r="A25" t="s">
+      <c t="s" r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c t="s" r="B25">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" footer="0.5" header="0.5" left="0.75" bottom="1" right="0.75"/>
+  <pageMargins right="0.75" bottom="1" left="0.75" header="0.5" top="1" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Title, label, URL, and organization columns working in Excel for both runs.
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t xml:space="preserve">
 Facebook
@@ -38,12 +38,23 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">
+Instagram
+</t>
+  </si>
+  <si>
+    <t>Affiliate - Weebly Partner Page</t>
+  </si>
+  <si>
     <t>Affiliate Program</t>
   </si>
   <si>
     <t>Blog</t>
   </si>
   <si>
+    <t>BuzzFeed</t>
+  </si>
+  <si>
     <t>Buzzfeed</t>
   </si>
   <si>
@@ -65,6 +76,9 @@
     <t>Education Version</t>
   </si>
   <si>
+    <t>Enterprise  - Weebly Partner Page</t>
+  </si>
+  <si>
     <t>Enterprise Program</t>
   </si>
   <si>
@@ -74,15 +88,24 @@
     <t>Google</t>
   </si>
   <si>
+    <t>Howl Attire - Home</t>
+  </si>
+  <si>
     <t>HowlAttire.com</t>
   </si>
   <si>
     <t>Inspiration Center</t>
   </si>
   <si>
+    <t>Inspiration Center - Weebly</t>
+  </si>
+  <si>
     <t>Label</t>
   </si>
   <si>
+    <t>Learn more.</t>
+  </si>
+  <si>
     <t>Org 1</t>
   </si>
   <si>
@@ -95,6 +118,9 @@
     <t>Support Center</t>
   </si>
   <si>
+    <t>The Original Whiskey Ball - Round Ice Mold - The Original Whiskey Ball Ice Mold</t>
+  </si>
+  <si>
     <t>TheOrganicGallery.com</t>
   </si>
   <si>
@@ -107,9 +133,33 @@
     <t>URL</t>
   </si>
   <si>
+    <t xml:space="preserve">Unfold Yoga OC - North Orange County's Boutique Yoga Studio offering yoga classes for all levels of practitioners. </t>
+  </si>
+  <si>
     <t>UnfoldYogaOC.com</t>
   </si>
   <si>
+    <t>Weebly (weebly) on Twitter</t>
+  </si>
+  <si>
+    <t>Weebly - Create a free website and a free blog</t>
+  </si>
+  <si>
+    <t>Weebly - YouTube</t>
+  </si>
+  <si>
+    <t>Weebly Blog - Resources for Websites, eCommerce and Blogging</t>
+  </si>
+  <si>
+    <t>Weebly Designer Platform - The Easiest CMS for Designers and Clients</t>
+  </si>
+  <si>
+    <t>Weebly Support - FAQ &amp; Search</t>
+  </si>
+  <si>
+    <t>Weebly | Facebook</t>
+  </si>
+  <si>
     <t>Yahoo</t>
   </si>
   <si>
@@ -189,6 +239,9 @@
   </si>
   <si>
     <t>source link</t>
+  </si>
+  <si>
+    <t>the organic gallery - aloha</t>
   </si>
 </sst>
 </file>
@@ -528,291 +581,411 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
-    <row spans="1:4" r="1">
-      <c s="1" t="s" r="A1">
-        <v>25</v>
-      </c>
-      <c s="1" t="s" r="B1">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c s="1" t="s" r="C1">
-        <v>26</v>
-      </c>
-      <c s="1" t="s" r="D1">
-        <v>21</v>
-      </c>
-    </row>
-    <row spans="1:4" r="2">
-      <c t="s" r="A2">
-        <v>10</v>
-      </c>
-      <c t="s" r="B2">
-        <v>7</v>
-      </c>
-      <c t="s" r="C2">
-        <v>37</v>
-      </c>
-      <c t="s" r="D2">
-        <v>7</v>
-      </c>
-    </row>
-    <row spans="1:4" r="3">
-      <c t="s" r="A3">
-        <v>8</v>
-      </c>
-      <c t="s" r="B3">
-        <v>19</v>
-      </c>
-      <c t="s" r="C3">
-        <v>38</v>
-      </c>
-      <c t="s" r="D3">
-        <v>19</v>
-      </c>
-    </row>
-    <row spans="1:4" r="4">
-      <c t="s" r="A4">
-        <v>9</v>
-      </c>
-      <c t="s" r="B4">
-        <v>20</v>
-      </c>
-      <c t="s" r="C4">
-        <v>39</v>
-      </c>
-      <c t="s" r="D4">
-        <v>20</v>
-      </c>
-    </row>
-    <row spans="1:4" r="5">
-      <c t="s" r="A5">
-        <v>14</v>
-      </c>
-      <c t="s" r="B5">
-        <v>30</v>
-      </c>
-      <c t="s" r="C5">
-        <v>50</v>
-      </c>
-      <c t="s" r="D5">
-        <v>30</v>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" left="0.75" header="0.5" top="1" footer="0.5"/>
+  <pageMargins bottom="1" top="1" left="0.75" footer="0.5" right="0.75" header="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c s="1" t="s" r="A1">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c s="1" t="s" r="B1">
-        <v>26</v>
-      </c>
-    </row>
-    <row spans="1:3" r="2">
-      <c t="s" r="B2">
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c s="1" t="s" r="C2">
-        <v>54</v>
-      </c>
-    </row>
-    <row spans="1:3" r="3">
-      <c t="s" r="A3">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B3">
-        <v>42</v>
-      </c>
-    </row>
-    <row spans="1:3" r="4">
-      <c t="s" r="A4">
-        <v>28</v>
-      </c>
-      <c t="s" r="B4">
-        <v>52</v>
-      </c>
-    </row>
-    <row spans="1:3" r="6">
-      <c t="s" r="B6">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>39</v>
       </c>
-      <c s="1" t="s" r="C6">
-        <v>54</v>
-      </c>
-    </row>
-    <row spans="1:3" r="7">
-      <c t="s" r="A7">
-        <v>6</v>
-      </c>
-      <c t="s" r="B7">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row spans="1:3" r="8">
-      <c t="s" r="A8">
-        <v>29</v>
-      </c>
-      <c t="s" r="B8">
-        <v>53</v>
-      </c>
-    </row>
-    <row spans="1:3" r="10">
-      <c t="s" r="B10">
-        <v>50</v>
-      </c>
-      <c s="1" t="s" r="C10">
-        <v>54</v>
-      </c>
-    </row>
-    <row spans="1:3" r="11">
-      <c t="s" r="A11">
-        <v>5</v>
-      </c>
-      <c t="s" r="B11">
-        <v>35</v>
-      </c>
-    </row>
-    <row spans="1:3" r="12">
-      <c t="s" r="A12">
-        <v>17</v>
-      </c>
-      <c t="s" r="B12">
-        <v>45</v>
-      </c>
-    </row>
-    <row spans="1:3" r="13">
-      <c t="s" r="A13">
-        <v>11</v>
-      </c>
-      <c t="s" r="B13">
-        <v>40</v>
-      </c>
-    </row>
-    <row spans="1:3" r="14">
-      <c t="s" r="A14">
-        <v>22</v>
-      </c>
-      <c t="s" r="B14">
-        <v>43</v>
-      </c>
-    </row>
-    <row spans="1:3" r="15">
-      <c t="s" r="A15">
-        <v>13</v>
-      </c>
-      <c t="s" r="B15">
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row spans="1:3" r="16">
-      <c t="s" r="A16">
-        <v>4</v>
-      </c>
-      <c t="s" r="B16">
-        <v>34</v>
-      </c>
-    </row>
-    <row spans="1:3" r="17">
-      <c t="s" r="A17">
-        <v>12</v>
-      </c>
-      <c t="s" r="B17">
-        <v>41</v>
-      </c>
-    </row>
-    <row spans="1:3" r="18">
-      <c t="s" r="A18">
-        <v>0</v>
-      </c>
-      <c t="s" r="B18">
-        <v>48</v>
-      </c>
-    </row>
-    <row spans="1:3" r="19">
-      <c t="s" r="A19">
-        <v>2</v>
-      </c>
-      <c t="s" r="B19">
-        <v>49</v>
-      </c>
-    </row>
-    <row spans="1:3" r="20">
-      <c t="s" r="A20">
-        <v>3</v>
-      </c>
-      <c t="s" r="B20">
-        <v>51</v>
-      </c>
-    </row>
-    <row spans="1:3" r="21">
-      <c t="s" r="A21">
-        <v>1</v>
-      </c>
-      <c t="s" r="B21">
-        <v>46</v>
-      </c>
-    </row>
-    <row spans="1:3" r="22">
-      <c t="s" r="A22">
-        <v>16</v>
-      </c>
-      <c t="s" r="B22">
-        <v>44</v>
-      </c>
-    </row>
-    <row spans="1:3" r="23">
-      <c t="s" r="A23">
-        <v>27</v>
-      </c>
-      <c t="s" r="B23">
-        <v>33</v>
-      </c>
-    </row>
-    <row spans="1:3" r="24">
-      <c t="s" r="A24">
-        <v>24</v>
-      </c>
-      <c t="s" r="B24">
-        <v>32</v>
-      </c>
-    </row>
-    <row spans="1:3" r="25">
-      <c t="s" r="A25">
-        <v>23</v>
-      </c>
-      <c t="s" r="B25">
+      <c r="D25" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" left="0.75" header="0.5" top="1" footer="0.5"/>
+  <pageMargins bottom="1" top="1" left="0.75" footer="0.5" right="0.75" header="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Domains to first run and possibly second run
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="481">
   <si>
     <t xml:space="preserve">	 - Institut de recherche pour le développement (IRD)
 	</t>
@@ -235,6 +235,9 @@
     <t>Contact Us — SAEON</t>
   </si>
   <si>
+    <t xml:space="preserve">Copernicus Publications - About Us </t>
+  </si>
+  <si>
     <t xml:space="preserve">Copernicus Publications - Journal Metrics </t>
   </si>
   <si>
@@ -311,6 +314,9 @@
   </si>
   <si>
     <t>ESSD - Abstract - The MAREDAT global database of high performance liquid chromatography marine pigment measurements</t>
+  </si>
+  <si>
+    <t>ESSD - Abstract - The global distribution of pteropods and their contribution to carbonate and carbon biomass in the modern ocean</t>
   </si>
   <si>
     <t xml:space="preserve">ESSD - Alerts &amp; RSS Feeds </t>
@@ -649,6 +655,9 @@
     <t>Next Framework Programme: Horizon 2020</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>OECD Principles and Guidelines 
     for Access to Research Data from Public Funding.</t>
   </si>
@@ -891,6 +900,36 @@
     <t>Workshops</t>
   </si>
   <si>
+    <t>['Atmosphere', 'Ecology', 'Biology', 'Climate', 'Marine Ecology', 'Oceanography']</t>
+  </si>
+  <si>
+    <t>['Ecology', 'Climate']</t>
+  </si>
+  <si>
+    <t>['Fisheries', 'Oceanography', 'Ecology', 'Biology']</t>
+  </si>
+  <si>
+    <t>['Geochemistry', 'Oceanography', 'Climate']</t>
+  </si>
+  <si>
+    <t>['Maps/Imagery', 'Spatial']</t>
+  </si>
+  <si>
+    <t>['Oceanography', 'Ecology', 'Spatial']</t>
+  </si>
+  <si>
+    <t>['Oceanography', 'Geochemistry', 'Maps/Imagery', 'Ecology', 'Climate']</t>
+  </si>
+  <si>
+    <t>['Oceanography']</t>
+  </si>
+  <si>
+    <t>['Spatial']</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
     <t>comparing DAP4 and the CDM</t>
   </si>
   <si>
@@ -1077,6 +1116,9 @@
     <t>http://plone.org</t>
   </si>
   <si>
+    <t>http://publications.copernicus.org</t>
+  </si>
+  <si>
     <t>http://publications.copernicus.org/services/journal_metrics.html</t>
   </si>
   <si>
@@ -1159,6 +1201,9 @@
   </si>
   <si>
     <t>http://www.earth-syst-sci-data.net/4/149/2012/essd-4-149-2012.html</t>
+  </si>
+  <si>
+    <t>http://www.earth-syst-sci-data.net/4/167/2012/essd-4-167-2012.html</t>
   </si>
   <si>
     <t>http://www.earth-syst-sci-data.net/4/37/2012/essd-4-37-2012.html</t>
@@ -1802,82 +1847,94 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s" s="1">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>398</v>
+        <v>413</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>175</v>
+      </c>
+      <c r="E4" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
-        <v>423</v>
+        <v>438</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>228</v>
+      </c>
+      <c r="E5" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1885,13 +1942,16 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C6" t="s">
-        <v>426</v>
+        <v>441</v>
       </c>
       <c r="D6" t="s">
-        <v>244</v>
+        <v>247</v>
+      </c>
+      <c r="E6" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1902,94 +1962,115 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
+      <c r="E7" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
-        <v>463</v>
+        <v>478</v>
       </c>
       <c r="C8" t="s">
-        <v>401</v>
+        <v>416</v>
       </c>
       <c r="D8" t="s">
-        <v>463</v>
+        <v>478</v>
+      </c>
+      <c r="E8" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
-        <v>410</v>
+        <v>425</v>
       </c>
       <c r="D9" t="s">
-        <v>224</v>
+        <v>227</v>
+      </c>
+      <c r="E9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>188</v>
+      </c>
+      <c r="E10" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
-        <v>419</v>
+        <v>434</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>201</v>
+      </c>
+      <c r="E11" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B12" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
-        <v>414</v>
+        <v>429</v>
       </c>
       <c r="D12" t="s">
-        <v>205</v>
+        <v>208</v>
+      </c>
+      <c r="E12" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="D13" t="s">
-        <v>152</v>
+        <v>154</v>
+      </c>
+      <c r="E13" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1997,53 +2078,65 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="D14" t="s">
-        <v>194</v>
+        <v>196</v>
+      </c>
+      <c r="E14" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>460</v>
+        <v>475</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>142</v>
+      </c>
+      <c r="E15" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
+      <c r="E16" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
+        <v>300</v>
+      </c>
+      <c r="E17" t="s">
         <v>287</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" top="1" header="0.5" footer="0.5" left="0.75" right="0.75"/>
+  <pageMargins left="0.75" top="1" right="0.75" header="0.5" footer="0.5" bottom="1"/>
 </worksheet>
 </file>
 
@@ -2052,674 +2145,680 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s" s="1">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>464</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C6" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="D6" t="s">
-        <v>276</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C7" t="s">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="D7" t="s">
-        <v>234</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="D8" t="s">
-        <v>232</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>404</v>
+        <v>419</v>
       </c>
       <c r="D9" t="s">
-        <v>255</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>406</v>
+        <v>421</v>
       </c>
       <c r="D10" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C13" t="s" s="1">
-        <v>464</v>
+        <v>479</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>389</v>
+        <v>404</v>
+      </c>
+      <c r="D14" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>386</v>
+        <v>401</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>388</v>
+        <v>403</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C17" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="D17" t="s">
-        <v>212</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>377</v>
+        <v>392</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>381</v>
+        <v>396</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
-        <v>385</v>
+        <v>400</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C21" t="s">
-        <v>393</v>
+        <v>408</v>
       </c>
       <c r="D21" t="s">
-        <v>259</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C22" t="s">
-        <v>392</v>
+        <v>407</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C23" t="s">
-        <v>391</v>
+        <v>406</v>
       </c>
       <c r="D23" t="s">
-        <v>233</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>368</v>
+        <v>383</v>
+      </c>
+      <c r="D26" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C28" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>372</v>
+        <v>387</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C31" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>367</v>
+        <v>382</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C33" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s">
-        <v>369</v>
+        <v>384</v>
       </c>
       <c r="D34" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C37" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="D37" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
-        <v>358</v>
+        <v>381</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C39" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="B40" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C40" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="D40" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C41" t="s">
         <v>373</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C42" t="s">
-        <v>361</v>
+        <v>388</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C43" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D43" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>362</v>
+        <v>389</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C45" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="D45" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="C46" t="s">
-        <v>351</v>
+        <v>386</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C47" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D47" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C48" t="s">
-        <v>352</v>
+        <v>385</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="C49" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C50" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="D50" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2727,27 +2826,27 @@
         <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C51" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="C52" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2755,27 +2854,27 @@
         <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C53" t="s">
-        <v>382</v>
+        <v>405</v>
       </c>
       <c r="D53" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C54" t="s">
-        <v>383</v>
+        <v>402</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2783,932 +2882,950 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="C55" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C56" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="D56" t="s">
-        <v>163</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" t="s">
+        <v>399</v>
+      </c>
+      <c r="D57" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>98</v>
+      </c>
       <c r="B58" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" t="s">
-        <v>63</v>
-      </c>
-      <c r="C59" t="s">
-        <v>290</v>
-      </c>
-      <c r="D59" t="s">
-        <v>63</v>
+        <v>165</v>
+      </c>
+      <c r="C58" t="s">
+        <v>409</v>
+      </c>
+      <c r="D58" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" t="s">
-        <v>20</v>
-      </c>
       <c r="B60" t="s">
-        <v>237</v>
-      </c>
-      <c r="C60" t="s">
-        <v>348</v>
-      </c>
-      <c r="D60" t="s">
-        <v>237</v>
+        <v>122</v>
+      </c>
+      <c r="C60" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>213</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>458</v>
+        <v>303</v>
       </c>
       <c r="D61" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>240</v>
       </c>
       <c r="C62" t="s">
-        <v>454</v>
+        <v>362</v>
       </c>
       <c r="D62" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>399</v>
+        <v>473</v>
       </c>
       <c r="D63" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
-        <v>400</v>
+        <v>469</v>
       </c>
       <c r="D64" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>248</v>
+        <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="C65" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D65" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>221</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>278</v>
+        <v>153</v>
       </c>
       <c r="C66" t="s">
-        <v>343</v>
+        <v>415</v>
       </c>
       <c r="D66" t="s">
-        <v>278</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>34</v>
+        <v>251</v>
       </c>
       <c r="B67" t="s">
-        <v>33</v>
+        <v>200</v>
       </c>
       <c r="C67" t="s">
-        <v>344</v>
+        <v>427</v>
       </c>
       <c r="D67" t="s">
-        <v>33</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="B68" t="s">
-        <v>47</v>
+        <v>291</v>
       </c>
       <c r="C68" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
       <c r="D68" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>257</v>
+        <v>34</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="D69" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>181</v>
       </c>
       <c r="B70" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C70" t="s">
-        <v>347</v>
+        <v>422</v>
       </c>
       <c r="D70" t="s">
-        <v>68</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>160</v>
+        <v>260</v>
       </c>
       <c r="B71" t="s">
-        <v>167</v>
+        <v>136</v>
       </c>
       <c r="C71" t="s">
-        <v>402</v>
+        <v>359</v>
       </c>
       <c r="D71" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>247</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>452</v>
+        <v>361</v>
       </c>
       <c r="D72" t="s">
-        <v>247</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="B73" t="s">
-        <v>247</v>
+        <v>169</v>
       </c>
       <c r="C73" t="s">
-        <v>376</v>
+        <v>417</v>
       </c>
       <c r="D73" t="s">
-        <v>247</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" t="s">
+        <v>250</v>
+      </c>
+      <c r="C74" t="s">
+        <v>467</v>
+      </c>
+      <c r="D74" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>92</v>
+      </c>
       <c r="B75" t="s">
+        <v>250</v>
+      </c>
+      <c r="C75" t="s">
+        <v>391</v>
+      </c>
+      <c r="D75" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="B77" t="s">
         <v>18</v>
       </c>
-      <c r="C75" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
-        <v>251</v>
-      </c>
-      <c r="C76" t="s">
-        <v>427</v>
-      </c>
-      <c r="D76" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
-        <v>252</v>
-      </c>
-      <c r="C77" t="s">
-        <v>428</v>
-      </c>
-      <c r="D77" t="s">
-        <v>252</v>
+      <c r="C77" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="B78" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="C78" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="D78" t="s">
-        <v>270</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="B79" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="C79" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="D79" t="s">
-        <v>239</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B80" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="C80" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="D80" t="s">
-        <v>250</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="B81" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="C81" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D81" t="s">
-        <v>262</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B82" t="s">
-        <v>17</v>
+        <v>253</v>
       </c>
       <c r="C82" t="s">
-        <v>444</v>
+        <v>460</v>
       </c>
       <c r="D82" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B83" t="s">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="C83" t="s">
-        <v>425</v>
+        <v>465</v>
       </c>
       <c r="D83" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="B84" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>435</v>
+        <v>459</v>
       </c>
       <c r="D84" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B85" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D85" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>188</v>
+        <v>276</v>
       </c>
       <c r="B86" t="s">
-        <v>253</v>
+        <v>147</v>
       </c>
       <c r="C86" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="D86" t="s">
-        <v>253</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>257</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
+        <v>29</v>
       </c>
       <c r="C87" t="s">
-        <v>430</v>
+        <v>461</v>
       </c>
       <c r="D87" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>190</v>
       </c>
       <c r="B88" t="s">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="C88" t="s">
-        <v>431</v>
+        <v>455</v>
       </c>
       <c r="D88" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>245</v>
+        <v>46</v>
       </c>
       <c r="B89" t="s">
-        <v>58</v>
+        <v>191</v>
       </c>
       <c r="C89" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="D89" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>258</v>
+        <v>59</v>
       </c>
       <c r="B90" t="s">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="C90" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D90" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>142</v>
+        <v>248</v>
       </c>
       <c r="B91" t="s">
-        <v>145</v>
+        <v>58</v>
       </c>
       <c r="C91" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="D91" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="B92" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="C92" t="s">
-        <v>442</v>
+        <v>462</v>
       </c>
       <c r="D92" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>147</v>
       </c>
       <c r="C93" t="s">
-        <v>439</v>
+        <v>463</v>
       </c>
       <c r="D93" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>280</v>
+        <v>239</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="C94" t="s">
-        <v>434</v>
+        <v>457</v>
       </c>
       <c r="D94" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>269</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="D95" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>66</v>
+        <v>293</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C96" t="s">
-        <v>432</v>
+        <v>449</v>
       </c>
       <c r="D96" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
       <c r="B97" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>443</v>
+        <v>466</v>
       </c>
       <c r="D97" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="D98" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B99" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C99" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>244</v>
+        <v>125</v>
       </c>
       <c r="B100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C100" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>264</v>
       </c>
       <c r="B101" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C101" t="s">
-        <v>350</v>
+        <v>464</v>
       </c>
       <c r="D101" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>190</v>
+        <v>247</v>
       </c>
       <c r="B102" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>409</v>
+        <v>453</v>
       </c>
       <c r="D102" t="s">
-        <v>15</v>
+        <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C103" t="s">
-        <v>429</v>
+        <v>364</v>
       </c>
       <c r="D103" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C104" t="s">
-        <v>338</v>
+        <v>424</v>
       </c>
       <c r="D104" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>249</v>
+        <v>30</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="D105" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" t="s">
+        <v>351</v>
+      </c>
+      <c r="D106" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>252</v>
+      </c>
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" t="s">
+        <v>468</v>
+      </c>
+      <c r="D107" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108" t="s">
         <v>14</v>
       </c>
-      <c r="C106" t="s">
-        <v>457</v>
-      </c>
-      <c r="D106" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="B108" t="s">
-        <v>346</v>
-      </c>
-      <c r="C108" t="s" s="1">
-        <v>464</v>
+      <c r="C108" t="s">
+        <v>472</v>
+      </c>
+      <c r="D108" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:4">
+      <c r="B110" t="s">
+        <v>360</v>
+      </c>
       <c r="C110" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" t="s">
-        <v>145</v>
-      </c>
-      <c r="C111" t="s">
-        <v>319</v>
+        <v>479</v>
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" t="s">
-        <v>119</v>
-      </c>
-      <c r="C112" t="s">
-        <v>396</v>
+      <c r="C112" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C113" t="s">
-        <v>397</v>
+        <v>332</v>
+      </c>
+      <c r="D113" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C114" t="s">
-        <v>395</v>
+        <v>411</v>
+      </c>
+      <c r="D114" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="C115" t="s">
-        <v>408</v>
+        <v>412</v>
+      </c>
+      <c r="D115" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
+        <v>126</v>
+      </c>
+      <c r="C116" t="s">
+        <v>410</v>
+      </c>
+      <c r="D116" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>183</v>
+      </c>
+      <c r="C117" t="s">
+        <v>423</v>
+      </c>
+      <c r="D117" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
         <v>0</v>
       </c>
-      <c r="C116" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="B118" t="s">
-        <v>271</v>
-      </c>
-      <c r="C118" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" t="s">
-        <v>229</v>
-      </c>
-      <c r="B119" t="s">
-        <v>209</v>
-      </c>
-      <c r="C119" t="s">
-        <v>424</v>
-      </c>
-      <c r="D119" t="s">
-        <v>209</v>
+      <c r="C118" t="s">
+        <v>418</v>
+      </c>
+      <c r="D118" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" t="s">
-        <v>211</v>
-      </c>
       <c r="B120" t="s">
-        <v>210</v>
-      </c>
-      <c r="C120" t="s">
-        <v>411</v>
-      </c>
-      <c r="D120" t="s">
-        <v>210</v>
+        <v>274</v>
+      </c>
+      <c r="C120" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="B121" t="s">
-        <v>271</v>
+        <v>212</v>
       </c>
       <c r="C121" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="D121" t="s">
-        <v>271</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>214</v>
+      </c>
+      <c r="B122" t="s">
+        <v>213</v>
+      </c>
+      <c r="C122" t="s">
+        <v>426</v>
+      </c>
+      <c r="D122" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>150</v>
+      </c>
       <c r="B123" t="s">
-        <v>281</v>
-      </c>
-      <c r="C123" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
-      <c r="A124" t="s">
-        <v>36</v>
-      </c>
-      <c r="B124" t="s">
-        <v>35</v>
-      </c>
-      <c r="C124" t="s">
-        <v>329</v>
-      </c>
-      <c r="D124" t="s">
-        <v>35</v>
+        <v>274</v>
+      </c>
+      <c r="C123" t="s">
+        <v>471</v>
+      </c>
+      <c r="D123" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" t="s">
-        <v>193</v>
-      </c>
       <c r="B125" t="s">
-        <v>192</v>
-      </c>
-      <c r="C125" t="s">
-        <v>330</v>
-      </c>
-      <c r="D125" t="s">
-        <v>192</v>
+        <v>294</v>
+      </c>
+      <c r="C125" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>208</v>
+        <v>36</v>
       </c>
       <c r="B126" t="s">
-        <v>207</v>
+        <v>35</v>
       </c>
       <c r="C126" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="D126" t="s">
-        <v>207</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="B127" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="C127" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="D127" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>211</v>
       </c>
       <c r="B128" t="s">
-        <v>2</v>
+        <v>210</v>
       </c>
       <c r="C128" t="s">
-        <v>288</v>
+        <v>344</v>
       </c>
       <c r="D128" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="B129" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C129" t="s">
-        <v>289</v>
+        <v>345</v>
       </c>
       <c r="D129" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="B130" t="s">
         <v>2</v>
       </c>
       <c r="C130" t="s">
-        <v>455</v>
+        <v>301</v>
       </c>
       <c r="D130" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>235</v>
+        <v>23</v>
       </c>
       <c r="C131" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="D131" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>281</v>
+        <v>2</v>
       </c>
       <c r="C132" t="s">
-        <v>312</v>
+        <v>470</v>
       </c>
       <c r="D132" t="s">
-        <v>281</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3716,13 +3833,13 @@
         <v>20</v>
       </c>
       <c r="B133" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C133" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="D133" t="s">
-        <v>281</v>
+        <v>146</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3730,13 +3847,13 @@
         <v>20</v>
       </c>
       <c r="B134" t="s">
-        <v>166</v>
+        <v>294</v>
       </c>
       <c r="C134" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="D134" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3744,383 +3861,392 @@
         <v>20</v>
       </c>
       <c r="B135" t="s">
-        <v>187</v>
+        <v>294</v>
       </c>
       <c r="C135" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="D135" t="s">
-        <v>187</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>20</v>
+      </c>
+      <c r="B136" t="s">
+        <v>168</v>
+      </c>
+      <c r="C136" t="s">
+        <v>347</v>
+      </c>
+      <c r="D136" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>20</v>
+      </c>
       <c r="B137" t="s">
+        <v>189</v>
+      </c>
+      <c r="C137" t="s">
+        <v>349</v>
+      </c>
+      <c r="D137" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="B139" t="s">
         <v>26</v>
       </c>
-      <c r="C137" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" t="s">
-        <v>199</v>
-      </c>
-      <c r="B138" t="s">
-        <v>31</v>
-      </c>
-      <c r="C138" t="s">
-        <v>282</v>
-      </c>
-      <c r="D138" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" t="s">
-        <v>200</v>
-      </c>
-      <c r="B139" t="s">
-        <v>264</v>
-      </c>
-      <c r="C139" t="s">
-        <v>422</v>
-      </c>
-      <c r="D139" t="s">
-        <v>264</v>
+      <c r="C139" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>27</v>
+        <v>202</v>
       </c>
       <c r="B140" t="s">
-        <v>462</v>
+        <v>31</v>
       </c>
       <c r="C140" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="D140" t="s">
-        <v>462</v>
+        <v>146</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>275</v>
+        <v>203</v>
       </c>
       <c r="B141" t="s">
-        <v>28</v>
+        <v>267</v>
       </c>
       <c r="C141" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
       <c r="D141" t="s">
-        <v>28</v>
+        <v>146</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>204</v>
+        <v>27</v>
       </c>
       <c r="B142" t="s">
-        <v>203</v>
+        <v>477</v>
       </c>
       <c r="C142" t="s">
-        <v>413</v>
+        <v>324</v>
       </c>
       <c r="D142" t="s">
-        <v>203</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>201</v>
+        <v>278</v>
       </c>
       <c r="B143" t="s">
-        <v>202</v>
+        <v>28</v>
       </c>
       <c r="C143" t="s">
-        <v>285</v>
+        <v>476</v>
       </c>
       <c r="D143" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c r="B144" t="s">
-        <v>268</v>
+        <v>206</v>
       </c>
       <c r="C144" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="D144" t="s">
-        <v>268</v>
+        <v>146</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>205</v>
       </c>
       <c r="C145" t="s">
-        <v>405</v>
+        <v>298</v>
       </c>
       <c r="D145" t="s">
-        <v>24</v>
+        <v>146</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>216</v>
+        <v>134</v>
       </c>
       <c r="B146" t="s">
-        <v>22</v>
+        <v>271</v>
       </c>
       <c r="C146" t="s">
-        <v>341</v>
+        <v>435</v>
       </c>
       <c r="D146" t="s">
-        <v>22</v>
+        <v>146</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="B147" t="s">
+        <v>24</v>
+      </c>
+      <c r="C147" t="s">
+        <v>420</v>
+      </c>
+      <c r="D147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>219</v>
+      </c>
+      <c r="B148" t="s">
+        <v>22</v>
+      </c>
+      <c r="C148" t="s">
+        <v>355</v>
+      </c>
+      <c r="D148" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>197</v>
+      </c>
+      <c r="B149" t="s">
         <v>26</v>
       </c>
-      <c r="C147" t="s">
-        <v>421</v>
-      </c>
-      <c r="D147" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="B149" t="s">
-        <v>266</v>
-      </c>
-      <c r="C149" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="A150" t="s">
-        <v>183</v>
-      </c>
-      <c r="B150" t="s">
-        <v>260</v>
-      </c>
-      <c r="C150" t="s">
-        <v>299</v>
-      </c>
-      <c r="D150" t="s">
-        <v>260</v>
+      <c r="C149" t="s">
+        <v>436</v>
+      </c>
+      <c r="D149" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" t="s">
-        <v>20</v>
-      </c>
       <c r="B151" t="s">
-        <v>279</v>
-      </c>
-      <c r="C151" t="s">
-        <v>418</v>
-      </c>
-      <c r="D151" t="s">
-        <v>279</v>
+        <v>269</v>
+      </c>
+      <c r="C151" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>20</v>
+        <v>185</v>
       </c>
       <c r="B152" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="C152" t="s">
-        <v>417</v>
+        <v>312</v>
       </c>
       <c r="D152" t="s">
-        <v>277</v>
+        <v>146</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>58</v>
+        <v>292</v>
       </c>
       <c r="C153" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="D153" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>205</v>
+        <v>20</v>
+      </c>
+      <c r="B154" t="s">
+        <v>290</v>
       </c>
       <c r="C154" t="s">
-        <v>416</v>
+        <v>432</v>
+      </c>
+      <c r="D154" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>231</v>
+        <v>57</v>
       </c>
       <c r="B155" t="s">
-        <v>266</v>
+        <v>58</v>
       </c>
       <c r="C155" t="s">
-        <v>342</v>
+        <v>430</v>
       </c>
       <c r="D155" t="s">
-        <v>266</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>208</v>
+      </c>
+      <c r="C156" t="s">
+        <v>431</v>
+      </c>
+      <c r="D156" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>234</v>
+      </c>
       <c r="B157" t="s">
+        <v>269</v>
+      </c>
+      <c r="C157" t="s">
+        <v>356</v>
+      </c>
+      <c r="D157" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="B159" t="s">
         <v>43</v>
       </c>
-      <c r="C157" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="A158" t="s">
-        <v>170</v>
-      </c>
-      <c r="B158" t="s">
-        <v>169</v>
-      </c>
-      <c r="C158" t="s">
-        <v>292</v>
-      </c>
-      <c r="D158" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="A159" t="s">
-        <v>126</v>
-      </c>
-      <c r="B159" t="s">
-        <v>126</v>
-      </c>
-      <c r="C159" t="s">
-        <v>293</v>
-      </c>
-      <c r="D159" t="s">
-        <v>126</v>
+      <c r="C159" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B160" t="s">
-        <v>2</v>
+        <v>171</v>
       </c>
       <c r="C160" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D160" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B161" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="C161" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D161" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B162" t="s">
         <v>2</v>
       </c>
       <c r="C162" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="D162" t="s">
-        <v>2</v>
+        <v>146</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>154</v>
+        <v>159</v>
+      </c>
+      <c r="B163" t="s">
+        <v>2</v>
       </c>
       <c r="C163" t="s">
-        <v>318</v>
+        <v>327</v>
+      </c>
+      <c r="D163" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>155</v>
+        <v>161</v>
+      </c>
+      <c r="B164" t="s">
+        <v>2</v>
       </c>
       <c r="C164" t="s">
-        <v>315</v>
+        <v>329</v>
+      </c>
+      <c r="D164" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>112</v>
-      </c>
-      <c r="B165" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="C165" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="D165" t="s">
-        <v>70</v>
+        <v>146</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>113</v>
-      </c>
-      <c r="B166" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C166" t="s">
-        <v>304</v>
+        <v>328</v>
       </c>
       <c r="D166" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="B167" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C167" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D167" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4128,294 +4254,325 @@
         <v>115</v>
       </c>
       <c r="B168" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="C168" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="D168" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="B169" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C169" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="D169" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B170" t="s">
-        <v>241</v>
+        <v>54</v>
       </c>
       <c r="C170" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="D170" t="s">
-        <v>241</v>
+        <v>146</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B171" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C171" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="D171" t="s">
-        <v>42</v>
+        <v>146</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B172" t="s">
-        <v>55</v>
+        <v>244</v>
       </c>
       <c r="C172" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="D172" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B173" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C173" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="D173" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B174" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C174" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="D174" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
+        <v>112</v>
+      </c>
+      <c r="B175" t="s">
+        <v>53</v>
+      </c>
+      <c r="C175" t="s">
+        <v>314</v>
+      </c>
+      <c r="D175" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>119</v>
+      </c>
+      <c r="B176" t="s">
+        <v>41</v>
+      </c>
+      <c r="C176" t="s">
+        <v>321</v>
+      </c>
+      <c r="D176" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="s">
         <v>20</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B177" t="s">
         <v>43</v>
       </c>
-      <c r="C175" t="s">
-        <v>310</v>
-      </c>
-      <c r="D175" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4">
-      <c r="B177" t="s">
+      <c r="C177" t="s">
+        <v>323</v>
+      </c>
+      <c r="D177" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="B179" t="s">
         <v>50</v>
       </c>
-      <c r="C177" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4">
-      <c r="A178" t="s">
+      <c r="C179" t="s" s="1">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="s">
         <v>40</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B180" t="s">
         <v>50</v>
       </c>
-      <c r="C178" t="s">
-        <v>283</v>
-      </c>
-      <c r="D178" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4">
-      <c r="B180" t="s">
-        <v>230</v>
-      </c>
-      <c r="C180" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4">
-      <c r="A181" t="s">
-        <v>217</v>
-      </c>
-      <c r="B181" t="s">
-        <v>349</v>
-      </c>
-      <c r="C181" t="s">
-        <v>349</v>
-      </c>
-      <c r="D181" t="s">
-        <v>349</v>
+      <c r="C180" t="s">
+        <v>296</v>
+      </c>
+      <c r="D180" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="182" spans="1:4">
-      <c r="A182" t="s">
-        <v>72</v>
-      </c>
       <c r="B182" t="s">
-        <v>465</v>
-      </c>
-      <c r="C182" t="s">
-        <v>459</v>
-      </c>
-      <c r="D182" t="s">
-        <v>465</v>
+        <v>233</v>
+      </c>
+      <c r="C182" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>161</v>
+        <v>220</v>
+      </c>
+      <c r="B183" t="s">
+        <v>363</v>
       </c>
       <c r="C183" t="s">
-        <v>328</v>
+        <v>363</v>
+      </c>
+      <c r="D183" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="s">
+        <v>73</v>
+      </c>
+      <c r="B184" t="s">
+        <v>480</v>
+      </c>
+      <c r="C184" t="s">
+        <v>474</v>
+      </c>
+      <c r="D184" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="185" spans="1:4">
-      <c r="B185" t="s">
+      <c r="A185" t="s">
+        <v>163</v>
+      </c>
+      <c r="C185" t="s">
+        <v>341</v>
+      </c>
+      <c r="D185" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="B187" t="s">
         <v>25</v>
       </c>
-      <c r="C185" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4">
-      <c r="A186" t="s">
-        <v>44</v>
-      </c>
-      <c r="B186" t="s">
-        <v>126</v>
-      </c>
-      <c r="C186" t="s">
-        <v>298</v>
-      </c>
-      <c r="D186" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4">
-      <c r="A187" t="s">
-        <v>238</v>
-      </c>
-      <c r="B187" t="s">
-        <v>136</v>
-      </c>
-      <c r="C187" t="s">
-        <v>297</v>
-      </c>
-      <c r="D187" t="s">
-        <v>136</v>
+      <c r="C187" t="s" s="1">
+        <v>479</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="B188" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C188" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="D188" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>127</v>
+        <v>241</v>
       </c>
       <c r="B189" t="s">
-        <v>240</v>
+        <v>138</v>
       </c>
       <c r="C189" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="D189" t="s">
-        <v>240</v>
+        <v>146</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B190" t="s">
-        <v>242</v>
+        <v>139</v>
       </c>
       <c r="C190" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
       <c r="D190" t="s">
-        <v>242</v>
+        <v>146</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="B191" t="s">
-        <v>196</v>
+        <v>243</v>
       </c>
       <c r="C191" t="s">
-        <v>340</v>
+        <v>304</v>
       </c>
       <c r="D191" t="s">
-        <v>196</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" t="s">
+        <v>151</v>
+      </c>
+      <c r="B192" t="s">
+        <v>245</v>
+      </c>
+      <c r="C192" t="s">
+        <v>307</v>
+      </c>
+      <c r="D192" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="193" spans="1:4">
+      <c r="A193" t="s">
+        <v>277</v>
+      </c>
       <c r="B193" t="s">
+        <v>198</v>
+      </c>
+      <c r="C193" t="s">
+        <v>354</v>
+      </c>
+      <c r="D193" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="B195" t="s">
         <v>25</v>
       </c>
-      <c r="C193" t="s" s="1">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4">
-      <c r="A194" t="s">
-        <v>125</v>
-      </c>
-      <c r="B194" t="s">
-        <v>126</v>
-      </c>
-      <c r="C194" t="s">
-        <v>295</v>
-      </c>
-      <c r="D194" t="s">
-        <v>126</v>
+      <c r="C195" t="s" s="1">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="s">
+        <v>127</v>
+      </c>
+      <c r="B196" t="s">
+        <v>128</v>
+      </c>
+      <c r="C196" t="s">
+        <v>308</v>
+      </c>
+      <c r="D196" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" top="1" header="0.5" footer="0.5" left="0.75" right="0.75"/>
+  <pageMargins left="0.75" top="1" right="0.75" header="0.5" footer="0.5" bottom="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Not working version of trying to get TLD and country code.
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7110" activeTab="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="First run" sheetId="1" r:id="rId1"/>
-    <sheet name="Second run" sheetId="2" r:id="rId2"/>
-  </sheets>
-  <calcPr calcId="124519"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="First run" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Second run" sheetId="2" r:id="rId2"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
   <si>
     <t xml:space="preserve">
 </t>
@@ -70,13 +71,13 @@
     <t>Catalog</t>
   </si>
   <si>
-    <t>Community</t>
+    <t>Community, Image Collection, Organization</t>
   </si>
   <si>
     <t>Content Type/Format</t>
   </si>
   <si>
-    <t>Data Center</t>
+    <t>Country</t>
   </si>
   <si>
     <t>Designers</t>
@@ -97,6 +98,9 @@
     <t>Enterprise Program</t>
   </si>
   <si>
+    <t>European Union</t>
+  </si>
+  <si>
     <t>Free website | Free blog | Create a free website | Weebly</t>
   </si>
   <si>
@@ -145,9 +149,6 @@
     <t>More »</t>
   </si>
   <si>
-    <t>N, o, n, e</t>
-  </si>
-  <si>
     <t>News</t>
   </si>
   <si>
@@ -191,6 +192,9 @@
   </si>
   <si>
     <t>Support Center</t>
+  </si>
+  <si>
+    <t>TLD</t>
   </si>
   <si>
     <t>The Original Whiskey Ball - Round Ice Mold - The Original Whiskey Ball Ice Mold</t>
@@ -340,8 +344,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,19 +355,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="11.0"/>
+      <color rgb="00000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -382,26 +379,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -480,7 +469,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -515,7 +503,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -691,39 +678,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s" s="1">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s" s="1">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s" s="1">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -731,22 +727,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -754,7 +750,7 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -766,10 +762,10 @@
         <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -777,7 +773,7 @@
         <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
         <v>45</v>
@@ -789,18 +785,18 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -809,68 +805,77 @@
         <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" top="1" right="0.75" left="0.75" footer="0.5" header="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s" s="1">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s" s="1">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s" s="1">
+        <v>55</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -878,7 +883,7 @@
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -887,21 +892,24 @@
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -910,21 +918,21 @@
         <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -936,18 +944,18 @@
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -959,18 +967,18 @@
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
@@ -982,18 +990,18 @@
         <v>41</v>
       </c>
       <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
@@ -1005,18 +1013,18 @@
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -1028,18 +1036,18 @@
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
@@ -1051,10 +1059,10 @@
         <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -1062,7 +1070,7 @@
         <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -1074,21 +1082,21 @@
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
@@ -1097,21 +1105,21 @@
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -1120,21 +1128,21 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
@@ -1143,21 +1151,21 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
@@ -1166,10 +1174,10 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1177,10 +1185,10 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -1189,10 +1197,10 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1200,10 +1208,10 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
@@ -1212,21 +1220,21 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
@@ -1235,21 +1243,21 @@
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -1258,21 +1266,21 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -1281,21 +1289,21 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
@@ -1304,10 +1312,10 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1315,10 +1323,10 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -1327,21 +1335,21 @@
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -1350,21 +1358,21 @@
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
@@ -1373,21 +1381,21 @@
         <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
@@ -1396,21 +1404,21 @@
         <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
@@ -1419,14 +1427,10 @@
         <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" top="1" right="0.75" left="0.75" footer="0.5" header="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Label is right. Everything else is wrong
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="19815" windowHeight="7050" activeTab="1"/>
-  </bookViews>
-  <sheets>
-    <sheet name="First run" sheetId="1" r:id="rId1"/>
-    <sheet name="Second run" sheetId="2" r:id="rId2"/>
-  </sheets>
-  <calcPr calcId="124519"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="First run" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Second run" sheetId="2" r:id="rId2"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
   <si>
     <t xml:space="preserve">
 </t>
@@ -52,9 +53,6 @@
     <t>Affiliate Program</t>
   </si>
   <si>
-    <t>Agriculture/Farming, Ecology</t>
-  </si>
-  <si>
     <t>Blog</t>
   </si>
   <si>
@@ -76,6 +74,15 @@
     <t>Community</t>
   </si>
   <si>
+    <t>Community, Organization, Image Collection</t>
+  </si>
+  <si>
+    <t>Community, Organization, Software, Image Collection</t>
+  </si>
+  <si>
+    <t>Community, Software, Data Service, Image Collection</t>
+  </si>
+  <si>
     <t>Company</t>
   </si>
   <si>
@@ -88,9 +95,6 @@
     <t>Data Service</t>
   </si>
   <si>
-    <t>Data Service, Catalog, Software</t>
-  </si>
-  <si>
     <t>Designers</t>
   </si>
   <si>
@@ -103,6 +107,9 @@
     <t>Ecology</t>
   </si>
   <si>
+    <t>Ecology, Agriculture/Farming</t>
+  </si>
+  <si>
     <t>Education Version</t>
   </si>
   <si>
@@ -130,9 +137,6 @@
     <t>Image Collection</t>
   </si>
   <si>
-    <t>Image Collection, Community, Data Service, Software</t>
-  </si>
-  <si>
     <t>Images</t>
   </si>
   <si>
@@ -178,12 +182,6 @@
     <t>Organization</t>
   </si>
   <si>
-    <t>Organization, Image Collection, Community</t>
-  </si>
-  <si>
-    <t>Organization, Image Collection, Community, Software</t>
-  </si>
-  <si>
     <t>Pangea</t>
   </si>
   <si>
@@ -194,6 +192,9 @@
   </si>
   <si>
     <t>Software</t>
+  </si>
+  <si>
+    <t>Software, Data Service, Catalog</t>
   </si>
   <si>
     <t>Spatial</t>
@@ -325,8 +326,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,11 +337,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="11.0"/>
+      <color rgb="00000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -360,22 +362,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -454,7 +451,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -489,7 +485,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -665,123 +660,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row spans="1:9" r="1">
+      <c r="A1" t="s" s="1">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s" s="1">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="D1" t="s" s="1">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s" s="1">
         <v>58</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" t="s" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row spans="1:9" r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
         <v>83</v>
       </c>
       <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -793,21 +793,21 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="6">
+      <c r="A6" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
@@ -819,63 +819,66 @@
         <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins header="0.5" right="0.75" bottom="1" left="0.75" top="1" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row spans="1:9" r="1">
+      <c r="A1" t="s" s="1">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" t="s" s="1">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s" s="1">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="D1" t="s" s="1">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s" s="1">
         <v>58</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" t="s" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row spans="1:9" r="2">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -883,485 +886,471 @@
         <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="4">
       <c r="A4" t="s">
         <v>72</v>
       </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
       <c r="C4" t="s">
         <v>85</v>
       </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="5">
       <c r="A5" t="s">
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="8">
       <c r="A8" t="s">
         <v>69</v>
       </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
       <c r="C8" t="s">
         <v>86</v>
       </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="9">
       <c r="A9" t="s">
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="10">
       <c r="A10" t="s">
         <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="11">
       <c r="A11" t="s">
         <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>96</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
         <v>44</v>
       </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="12">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="13">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
         <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="14">
       <c r="A14" t="s">
         <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
         <v>44</v>
       </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="15">
       <c r="A15" t="s">
         <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
         <v>44</v>
       </c>
-      <c r="F15" t="s">
-        <v>43</v>
-      </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="16">
       <c r="A16" t="s">
         <v>97</v>
       </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
       <c r="C16" t="s">
         <v>77</v>
       </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row spans="1:9" r="17">
       <c r="B17" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="18">
       <c r="B18" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="19">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="20">
       <c r="B20" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="21">
       <c r="B21" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="22">
       <c r="B22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="23">
       <c r="B23" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="24">
       <c r="B24" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="25">
       <c r="B25" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="26">
       <c r="B26" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row spans="1:9" r="27">
       <c r="B27" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins header="0.5" right="0.75" bottom="1" left="0.75" top="1" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified method of finding organization - now compares organization to list from OPR CA. Ignore labels column - still has bugs.
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -9,6 +9,7 @@
   <s:sheets>
     <s:sheet name="First run" sheetId="1" r:id="rId1"/>
     <s:sheet name="Second run" sheetId="2" r:id="rId2"/>
+    <s:sheet name="List of Official Organizations" sheetId="3" r:id="rId3"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
   <si>
     <t xml:space="preserve">
 </t>
@@ -50,18 +51,186 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>Academia  Chilena de Ciencias, Chile</t>
+  </si>
+  <si>
+    <t>Academia  Mexicana de Ciencias,Mexico</t>
+  </si>
+  <si>
+    <t>Academia Nacional de Ciencias de  Bolivia</t>
+  </si>
+  <si>
+    <t>Academia Nacional de Ciencias del  Peru</t>
+  </si>
+  <si>
+    <t>Academia das Ciencias de Lisboa,  Portugal</t>
+  </si>
+  <si>
+    <t>Academia de Ciencias Físicas,  Matemáticas y Naturales de Venezuela</t>
+  </si>
+  <si>
+    <t>Academia de Ciencias de la República  Dominicana</t>
+  </si>
+  <si>
+    <t>Academies  of Arts, Humanities and Sciences of Canada</t>
+  </si>
+  <si>
+    <t>Academy  of Science of South Africa</t>
+  </si>
+  <si>
+    <t>Academy  of Sciences for the Developing World (TWAS)</t>
+  </si>
+  <si>
+    <t>Academy  of Sciences of the Czech Republic</t>
+  </si>
+  <si>
+    <t>Academy  of Sciences of the Islamic Republic of Iran</t>
+  </si>
+  <si>
+    <t>Academy  of Scientific Research and Technology, Egypt</t>
+  </si>
+  <si>
+    <t>Academy  of the Royal Society of New Zealand</t>
+  </si>
+  <si>
+    <t>Academy of Athens</t>
+  </si>
+  <si>
+    <t>Academy of Sciences  of Moldova</t>
+  </si>
+  <si>
+    <t>Academy of Sciences Malaysia</t>
+  </si>
+  <si>
+    <t>Académie  des Sciences et Techniques du Sénégal</t>
+  </si>
+  <si>
+    <t>Académie  des Sciences, France</t>
+  </si>
+  <si>
+    <t>Accademia  Nazionale dei Lincei, Italy</t>
+  </si>
+  <si>
     <t>Affiliate - Weebly Partner Page</t>
   </si>
   <si>
     <t>Affiliate Program</t>
   </si>
   <si>
-    <t>Biology, Oceanography</t>
+    <t>Africa  Centre for Climate and Earth Systems Science</t>
+  </si>
+  <si>
+    <t>African Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Albanian  Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Amazon  Environmental Research Institute</t>
+  </si>
+  <si>
+    <t>American  Academy of Pediatrics</t>
+  </si>
+  <si>
+    <t>American  Anthropological Association</t>
+  </si>
+  <si>
+    <t>American  Association of State Climatologists (AASC)</t>
+  </si>
+  <si>
+    <t>American  Astronomical Society</t>
+  </si>
+  <si>
+    <t>American  College of Preventive Medicine</t>
+  </si>
+  <si>
+    <t>American  Fisheries Society</t>
+  </si>
+  <si>
+    <t>American  Institute of Physics</t>
+  </si>
+  <si>
+    <t>American  Public Health Association</t>
+  </si>
+  <si>
+    <t>American  Society for Microbiology</t>
+  </si>
+  <si>
+    <t>American  Society of Civil Engineers</t>
+  </si>
+  <si>
+    <t>American  Society of Plant Biologists</t>
+  </si>
+  <si>
+    <t>American  Statistical Association</t>
+  </si>
+  <si>
+    <t>American Association for the  Advancement of Science</t>
+  </si>
+  <si>
+    <t>American Chemical Society</t>
+  </si>
+  <si>
+    <t>American Geophysical Union</t>
+  </si>
+  <si>
+    <t>American Institute of Biological  Sciences</t>
+  </si>
+  <si>
+    <t>American Meteorological Society</t>
+  </si>
+  <si>
+    <t>American Physical Society</t>
+  </si>
+  <si>
+    <t>American Quaternary Association</t>
+  </si>
+  <si>
+    <t>Association of Ecosystem  Research Centers</t>
+  </si>
+  <si>
+    <t>Australian  Academy of Science</t>
+  </si>
+  <si>
+    <t>Australian  Bureau of Meteorology</t>
+  </si>
+  <si>
+    <t>Australian  Institute of Marine Science</t>
+  </si>
+  <si>
+    <t>Australian  Institute of Physics</t>
+  </si>
+  <si>
+    <t>Australian  Marine Sciences Association</t>
+  </si>
+  <si>
+    <t>Australian  Medical Association</t>
+  </si>
+  <si>
+    <t>Australian Coral Reef  Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australian Meteorological and  Oceanographic Society </t>
+  </si>
+  <si>
+    <t>Bangladesh  Academy of Sciences</t>
   </si>
   <si>
     <t>Blog</t>
   </si>
   <si>
+    <t>Botanical  Society of America</t>
+  </si>
+  <si>
+    <t>Brazilian Academy of Sciences</t>
+  </si>
+  <si>
+    <t>British  Antarctic Survey</t>
+  </si>
+  <si>
+    <t>Bulgarian  Academy of Sciences</t>
+  </si>
+  <si>
     <t>CINERGI Home</t>
   </si>
   <si>
@@ -74,21 +243,66 @@
     <t>CINERGI Web Crawler - Home</t>
   </si>
   <si>
+    <t>California  Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Canadian  Association of Physicists</t>
+  </si>
+  <si>
+    <t>Canadian  Geophysical Union</t>
+  </si>
+  <si>
+    <t>Canadian  Society of Soil Science</t>
+  </si>
+  <si>
+    <t>Canadian  Society of Zoologists</t>
+  </si>
+  <si>
+    <t>Canadian Foundation for Climate and Atmospheric  Sciences</t>
+  </si>
+  <si>
+    <t>Canadian Meteorological and Oceanographic Society</t>
+  </si>
+  <si>
     <t>Catalog</t>
   </si>
   <si>
+    <t>Center  for International Forestry Research</t>
+  </si>
+  <si>
+    <t>Center for International Forestry Research</t>
+  </si>
+  <si>
+    <t>Chinese  Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Commonwealth  Scientific and Industrial Research Organization (CSIRO) (Australia)</t>
+  </si>
+  <si>
     <t>Company</t>
   </si>
   <si>
+    <t>Consultative  Group on International Agricultural Research</t>
+  </si>
+  <si>
     <t>Content Type/Format</t>
   </si>
   <si>
     <t>Country</t>
   </si>
   <si>
+    <t>Croatian  Academy of Arts and Sciences</t>
+  </si>
+  <si>
+    <t>Cuban  Academy of Sciences</t>
+  </si>
+  <si>
     <t>Data Publisher for Earth &amp; Environmental Science</t>
   </si>
   <si>
+    <t>Delegation  of the Finnish Academies of Science and Letters</t>
+  </si>
+  <si>
     <t>Designers</t>
   </si>
   <si>
@@ -98,6 +312,12 @@
     <t>EU</t>
   </si>
   <si>
+    <t>Ecological  Society of Australia</t>
+  </si>
+  <si>
+    <t>Ecological Society of America</t>
+  </si>
+  <si>
     <t>Education Version</t>
   </si>
   <si>
@@ -107,15 +327,57 @@
     <t>Enterprise Program</t>
   </si>
   <si>
+    <t>Environmental Protection Agency</t>
+  </si>
+  <si>
+    <t>European  Geosciences Union</t>
+  </si>
+  <si>
+    <t>European  Physical Society</t>
+  </si>
+  <si>
+    <t>European  Science Foundation</t>
+  </si>
+  <si>
+    <t>European Academy of Sciences and  Arts</t>
+  </si>
+  <si>
+    <t>European Federation of  Geologists</t>
+  </si>
+  <si>
     <t>European Union</t>
   </si>
   <si>
+    <t>Federation of American  Scientists</t>
+  </si>
+  <si>
     <t>Free website | Free blog | Create a free website | Weebly</t>
   </si>
   <si>
+    <t>French Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Geological  Society of America</t>
+  </si>
+  <si>
+    <t>Geological  Society of Australia</t>
+  </si>
+  <si>
+    <t>Geological Society of London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgian  Academy of Sciences </t>
+  </si>
+  <si>
+    <t xml:space="preserve">German Academy of Natural Scientists Leopoldina </t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
+    <t>Ghana  Academy of Arts and Sciences</t>
+  </si>
+  <si>
     <t>GitHub · Build software better, together.</t>
   </si>
   <si>
@@ -137,7 +399,7 @@
     <t>Google News</t>
   </si>
   <si>
-    <t>HTTP</t>
+    <t>Government</t>
   </si>
   <si>
     <t>Home - Lifewatch Project</t>
@@ -155,6 +417,9 @@
     <t>Images</t>
   </si>
   <si>
+    <t>Indian National Science Academy</t>
+  </si>
+  <si>
     <t>Inspiration Center</t>
   </si>
   <si>
@@ -164,30 +429,177 @@
     <t>Instagram</t>
   </si>
   <si>
+    <t>Institute  of Ecology and Environmental Management</t>
+  </si>
+  <si>
+    <t>Institute  of Marine Engineering, Science and Technology</t>
+  </si>
+  <si>
+    <t>Institute of  Professional Engineers New Zealand</t>
+  </si>
+  <si>
+    <t>Institution of Mechanical Engineers, UK</t>
+  </si>
+  <si>
+    <t>InterAcademy Council</t>
+  </si>
+  <si>
+    <t>International  Research Institute for Climate and Society</t>
+  </si>
+  <si>
+    <t>International Alliance of Research  Universities</t>
+  </si>
+  <si>
+    <t>International Arctic Science Committee</t>
+  </si>
+  <si>
+    <t>International Association for Great  Lakes Research</t>
+  </si>
+  <si>
+    <t>International Council for Science</t>
+  </si>
+  <si>
+    <t>International Council of  Academies of Engineering and Technological Sciences</t>
+  </si>
+  <si>
+    <t>International Union for Quaternary  Research</t>
+  </si>
+  <si>
+    <t>International Union of Geodesy and  Geophysics</t>
+  </si>
+  <si>
+    <t>International Union of Pure and Applied  Physics</t>
+  </si>
+  <si>
+    <t>Islamic World Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Israel Academy of Sciences and  Humanities</t>
+  </si>
+  <si>
+    <t>Kenya National Academy of  Sciences</t>
+  </si>
+  <si>
+    <t>Korean Academy of  Science and Technology</t>
+  </si>
+  <si>
+    <t>Kosovo Academy of Sciences and Arts</t>
+  </si>
+  <si>
     <t>Label</t>
   </si>
   <si>
+    <t>Latin American Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Latvian Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Lithuanian Academy of  Sciences</t>
+  </si>
+  <si>
     <t>Maps</t>
   </si>
   <si>
     <t>Maps/Imagery</t>
   </si>
   <si>
+    <t>Montenegrin Academy  of Sciences and Arts</t>
+  </si>
+  <si>
     <t>More »</t>
   </si>
   <si>
+    <t xml:space="preserve">National  Center for Atmospheric Research </t>
+  </si>
+  <si>
+    <t>National  Council of Engineers Australia</t>
+  </si>
+  <si>
+    <t>National  Research Council</t>
+  </si>
+  <si>
+    <t>National  Science Foundation</t>
+  </si>
+  <si>
+    <t>National Academy of  Exact, Physical and Natural Sciences, Argentina</t>
+  </si>
+  <si>
+    <t>National Academy of  Sciences of the Kyrgyz Republic</t>
+  </si>
+  <si>
+    <t>National Academy of Sciences of Armenia</t>
+  </si>
+  <si>
+    <t>National Academy of Sciences, Sri Lanka</t>
+  </si>
+  <si>
+    <t>National Academy of Sciences, United  States of America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Aeronautics and Space  Administration </t>
+  </si>
+  <si>
+    <t>National Association  of State Foresters</t>
+  </si>
+  <si>
+    <t>National Association of  Geoscience Teachers</t>
+  </si>
+  <si>
+    <t>National Institute of Water &amp;  Atmospheric Research, New Zealand</t>
+  </si>
+  <si>
+    <t>National Oceanic and Atmospheric  Administration</t>
+  </si>
+  <si>
+    <t>Natural  Science Collections Alliance</t>
+  </si>
+  <si>
+    <t>Natural England</t>
+  </si>
+  <si>
+    <t>Natural Environment Research Council,  UK</t>
+  </si>
+  <si>
+    <t>Network of African Science  Academies</t>
+  </si>
+  <si>
+    <t>New York Academy of Sciences</t>
+  </si>
+  <si>
     <t>News</t>
   </si>
   <si>
+    <t>Nicaraguan Academy of  Sciences</t>
+  </si>
+  <si>
+    <t>Nigerian  Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Non-profit Org</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
+    <t>Norwegian Academy of Sciences and  Letters</t>
+  </si>
+  <si>
+    <t>OKC</t>
+  </si>
+  <si>
     <t>Oceanography</t>
   </si>
   <si>
+    <t>Oceanography, Biology</t>
+  </si>
+  <si>
     <t>Oceanography, Ecology</t>
   </si>
   <si>
+    <t>Oklahoma Climatological Survey</t>
+  </si>
+  <si>
     <t>Org 1</t>
   </si>
   <si>
@@ -197,33 +609,141 @@
     <t>Organization</t>
   </si>
   <si>
+    <t>Organization  of Biological Field Stations</t>
+  </si>
+  <si>
     <t>PANGAEA - Data Publisher for Earth &amp; Environmental Science - About / Imprint</t>
   </si>
   <si>
+    <t>Pakistan Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Palestine Academy for  Science and Technology</t>
+  </si>
+  <si>
     <t>Pangea</t>
   </si>
   <si>
+    <t>Pew  Center on Global Climate Change</t>
+  </si>
+  <si>
+    <t>Polish Academy of Sciences</t>
+  </si>
+  <si>
     <t>Resource Type</t>
   </si>
   <si>
+    <t>Romanian Academy</t>
+  </si>
+  <si>
+    <t>Royal  Danish Academy of Sciences and Letters</t>
+  </si>
+  <si>
+    <t>Royal  Irish Academy</t>
+  </si>
+  <si>
+    <t>Royal  Netherlands Academy of Arts and Sciences</t>
+  </si>
+  <si>
+    <t>Royal Academies for Science and the  Arts of Belgium</t>
+  </si>
+  <si>
+    <t>Royal Academy of Exact, Physical and  Natural Sciences of Spain</t>
+  </si>
+  <si>
+    <t>Royal Astronomical Society, UK</t>
+  </si>
+  <si>
+    <t>Royal Meteorological Society (UK)</t>
+  </si>
+  <si>
+    <t>Royal Netherlands Institute for Sea  Research</t>
+  </si>
+  <si>
+    <t>Royal Scientific Society of Jordan</t>
+  </si>
+  <si>
+    <t>Royal Society of Canada</t>
+  </si>
+  <si>
+    <t>Royal Society of Chemistry, UK</t>
+  </si>
+  <si>
+    <t>Royal Society of the United  Kingdom</t>
+  </si>
+  <si>
+    <t>Royal Swedish Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Russian Academy of  Sciences</t>
+  </si>
+  <si>
+    <t>Science Council of Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science and  Technology, Australia </t>
+  </si>
+  <si>
+    <t>Scientific Committee on  Solar-Terrestrial Physics</t>
+  </si>
+  <si>
+    <t>Scientific Committee on Antarctic  Research</t>
+  </si>
+  <si>
+    <t>Scripps Institution of Oceanography</t>
+  </si>
+  <si>
+    <t>Serbian Academy of  Sciences and Arts</t>
+  </si>
+  <si>
     <t>Sign in</t>
   </si>
   <si>
     <t>Sign in - Google Accounts</t>
   </si>
   <si>
+    <t>Slovak Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Slovenian Academy of Sciences and Arts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Society  of American Foresters  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Society  of Biology (UK)  </t>
+  </si>
+  <si>
+    <t>Society for Ecological Restoration  International</t>
+  </si>
+  <si>
+    <t>Society for Industrial and Applied Mathematics</t>
+  </si>
+  <si>
+    <t>Society of Systematic Biologists</t>
+  </si>
+  <si>
     <t>Software</t>
   </si>
   <si>
     <t>Spatial</t>
   </si>
   <si>
+    <t>Sudan Academy of Sciences</t>
+  </si>
+  <si>
     <t>Support Center</t>
   </si>
   <si>
     <t>TLD</t>
   </si>
   <si>
+    <t>Tanzania Academy of Sciences</t>
+  </si>
+  <si>
+    <t>The  Wildlife Society (international)</t>
+  </si>
+  <si>
     <t>The Original Whiskey Ball - Round Ice Mold - The Original Whiskey Ball Ice Mold</t>
   </si>
   <si>
@@ -236,18 +756,39 @@
     <t>Title</t>
   </si>
   <si>
+    <t>Turkish Academy of  Sciences</t>
+  </si>
+  <si>
     <t>Twitter</t>
   </si>
   <si>
+    <t>UK</t>
+  </si>
+  <si>
     <t>URL</t>
   </si>
   <si>
+    <t>Uganda National  Academy of Sciences</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unfold Yoga OC - North Orange County's Boutique Yoga Studio offering yoga classes for all levels of practitioners. </t>
   </si>
   <si>
     <t>UnfoldYogaOC.com</t>
   </si>
   <si>
+    <t>Union of German  Academies of Sciences and Humanities</t>
+  </si>
+  <si>
+    <t>United  Nations Intergovernmental Panel on Climate Change</t>
+  </si>
+  <si>
+    <t>University Corporation for Atmospheric  Research</t>
+  </si>
+  <si>
+    <t>Verified: Oklahoma Climatological Survey</t>
+  </si>
+  <si>
     <t>Vocabulary</t>
   </si>
   <si>
@@ -278,12 +819,33 @@
     <t>Welcome to Facebook - Log In, Sign Up or Learn More</t>
   </si>
   <si>
+    <t>Woods Hole Oceanographic Institution</t>
+  </si>
+  <si>
+    <t>World  Federation of Public Health Associations</t>
+  </si>
+  <si>
+    <t>World  Health Organization</t>
+  </si>
+  <si>
+    <t>World Association of Zoos and Aquariums</t>
+  </si>
+  <si>
+    <t>World Forestry  Congress</t>
+  </si>
+  <si>
     <t>YouTube</t>
   </si>
   <si>
+    <t>Zimbabwe  Academy of Sciences</t>
+  </si>
+  <si>
     <t>free website</t>
   </si>
   <si>
+    <t>ftp://ftp.funet.fi/pub/standards/RFC/rfc959.txt</t>
+  </si>
+  <si>
     <t>http://TheOrganicGallery.com</t>
   </si>
   <si>
@@ -308,6 +870,9 @@
     <t>http://cinergisheet2.weebly.com</t>
   </si>
   <si>
+    <t>http://climate.ok.gov/</t>
+  </si>
+  <si>
     <t>http://designers.weebly.com/</t>
   </si>
   <si>
@@ -341,6 +906,9 @@
     <t>http://partnerwith.weebly.com/enterprise.html</t>
   </si>
   <si>
+    <t>http://www.cifor.org/</t>
+  </si>
+  <si>
     <t>http://www.facebook.com/weebly</t>
   </si>
   <si>
@@ -375,6 +943,9 @@
   </si>
   <si>
     <t>https://accounts.google.com/ServiceLogin?hl=en&amp;continue=http://www.google.com/</t>
+  </si>
+  <si>
+    <t>l'Académie  des Sciences et Techniques du Sénégal</t>
   </si>
   <si>
     <t>the organic gallery - aloha</t>
@@ -719,887 +1290,1791 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>241</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>245</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>64</v>
+        <v>235</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
+        <v>253</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>278</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
+        <v>231</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>232</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>284</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>300</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins footer="0.5" right="0.75" bottom="1" left="0.75" header="0.5" top="1"/>
+  <pageMargins right="0.75" bottom="1" header="0.5" footer="0.5" left="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1" activeCell="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>241</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>245</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>64</v>
+        <v>235</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>244</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>280</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
+        <v>183</v>
+      </c>
+      <c r="H2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>292</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>298</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>268</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>303</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>268</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>297</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
+        <v>78</v>
+      </c>
+      <c r="I6" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>283</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>270</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>271</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>295</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>289</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>268</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>301</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>268</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>179</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>290</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>296</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>183</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>254</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>294</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>183</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>223</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>304</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>183</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>258</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>276</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H16" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>287</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>281</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>260</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>234</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>285</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>291</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>275</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>256</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>282</v>
       </c>
       <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" t="s">
         <v>83</v>
-      </c>
-      <c r="E22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>261</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>293</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>262</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>299</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>243</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>257</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>302</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>268</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>288</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="F26" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="H26" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" t="s">
+        <v>127</v>
+      </c>
+      <c r="H27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" t="s">
+        <v>248</v>
+      </c>
+      <c r="C28" t="s">
+        <v>274</v>
+      </c>
+      <c r="D28" t="s">
+        <v>247</v>
+      </c>
+      <c r="E28" t="s">
+        <v>188</v>
+      </c>
+      <c r="F28" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" t="s">
+        <v>240</v>
+      </c>
+      <c r="C29" t="s">
+        <v>273</v>
+      </c>
+      <c r="D29" t="s">
+        <v>238</v>
+      </c>
+      <c r="E29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>306</v>
+      </c>
+      <c r="B30" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" t="s">
+        <v>272</v>
+      </c>
+      <c r="D30" t="s">
+        <v>306</v>
+      </c>
+      <c r="E30" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins right="0.75" bottom="1" header="0.5" footer="0.5" left="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:A183"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
         <v>66</v>
       </c>
-      <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" t="s">
-        <v>40</v>
-      </c>
-      <c r="G27" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" t="s">
-        <v>16</v>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins footer="0.5" right="0.75" bottom="1" left="0.75" header="0.5" top="1"/>
+  <pageMargins right="0.75" bottom="1" header="0.5" footer="0.5" left="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Opens FTP correctly and check_link returns working link instead of integer
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="331">
   <si>
     <t xml:space="preserve">
 </t>
@@ -44,6 +44,13 @@
   </si>
   <si>
     <t xml:space="preserve">
+        Funet-palvelut
+        —
+        CSC
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 Instagram
 </t>
   </si>
@@ -216,6 +223,9 @@
     <t>Bangladesh  Academy of Sciences</t>
   </si>
   <si>
+    <t>Biology, Oceanography</t>
+  </si>
+  <si>
     <t>Blog</t>
   </si>
   <si>
@@ -318,6 +328,12 @@
     <t>Ecological Society of America</t>
   </si>
   <si>
+    <t>Ecology, Oceanography</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
     <t>Education Version</t>
   </si>
   <si>
@@ -351,6 +367,9 @@
     <t>Federation of American  Scientists</t>
   </si>
   <si>
+    <t>Flickr: sdsc_ucsd's Photostream</t>
+  </si>
+  <si>
     <t>Free website | Free blog | Create a free website | Weebly</t>
   </si>
   <si>
@@ -402,6 +421,9 @@
     <t>Government</t>
   </si>
   <si>
+    <t>HTTP</t>
+  </si>
+  <si>
     <t>Home - Lifewatch Project</t>
   </si>
   <si>
@@ -414,6 +436,9 @@
     <t>Image Collection, Organization, Community</t>
   </si>
   <si>
+    <t>Image Collection, Portal, Activity, Data Service</t>
+  </si>
+  <si>
     <t>Images</t>
   </si>
   <si>
@@ -591,12 +616,6 @@
     <t>Oceanography</t>
   </si>
   <si>
-    <t>Oceanography, Biology</t>
-  </si>
-  <si>
-    <t>Oceanography, Ecology</t>
-  </si>
-  <si>
     <t>Oklahoma Climatological Survey</t>
   </si>
   <si>
@@ -630,6 +649,12 @@
     <t>Polish Academy of Sciences</t>
   </si>
   <si>
+    <t>Portal, Data Service</t>
+  </si>
+  <si>
+    <t>Research Cyberinfrastructure</t>
+  </si>
+  <si>
     <t>Resource Type</t>
   </si>
   <si>
@@ -678,6 +703,18 @@
     <t>Russian Academy of  Sciences</t>
   </si>
   <si>
+    <t xml:space="preserve">SDSC </t>
+  </si>
+  <si>
+    <t>SDSC Education - Fostering Cyberinfrastructure in Learning and Instruction</t>
+  </si>
+  <si>
+    <t>San Diego Supercomputer Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Diego Supercomputer Center: </t>
+  </si>
+  <si>
     <t>Science Council of Japan</t>
   </si>
   <si>
@@ -726,9 +763,15 @@
     <t>Software</t>
   </si>
   <si>
+    <t>Software Applications</t>
+  </si>
+  <si>
     <t>Spatial</t>
   </si>
   <si>
+    <t>Staff Directory</t>
+  </si>
+  <si>
     <t>Sudan Academy of Sciences</t>
   </si>
   <si>
@@ -786,6 +829,12 @@
     <t>University Corporation for Atmospheric  Research</t>
   </si>
   <si>
+    <t>University of California, San Diego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Support </t>
+  </si>
+  <si>
     <t>Verified: Oklahoma Climatological Survey</t>
   </si>
   <si>
@@ -819,6 +868,9 @@
     <t>Welcome to Facebook - Log In, Sign Up or Learn More</t>
   </si>
   <si>
+    <t>Welcome to Flickr - Photo Sharing</t>
+  </si>
+  <si>
     <t>Woods Hole Oceanographic Institution</t>
   </si>
   <si>
@@ -876,6 +928,9 @@
     <t>http://designers.weebly.com/</t>
   </si>
   <si>
+    <t>http://education.sdsc.edu</t>
+  </si>
+  <si>
     <t>http://education.weebly.com/</t>
   </si>
   <si>
@@ -906,12 +961,18 @@
     <t>http://partnerwith.weebly.com/enterprise.html</t>
   </si>
   <si>
+    <t>http://rci.ucsd.edu/</t>
+  </si>
+  <si>
     <t>http://www.cifor.org/</t>
   </si>
   <si>
     <t>http://www.facebook.com/weebly</t>
   </si>
   <si>
+    <t>http://www.flickr.com/photos/75819710@N05/</t>
+  </si>
+  <si>
     <t>http://www.google.com/history/optout?hl=en</t>
   </si>
   <si>
@@ -927,7 +988,22 @@
     <t>http://www.pangaea.de/about/</t>
   </si>
   <si>
+    <t>http://www.sdsc.edu</t>
+  </si>
+  <si>
+    <t>http://www.sdsc.edu/about/staff_dir.cgi</t>
+  </si>
+  <si>
+    <t>http://www.sdsc.edu/us/</t>
+  </si>
+  <si>
+    <t>http://www.sdsc.edu/us/resources/applications.html</t>
+  </si>
+  <si>
     <t>http://www.twitter.com/weebly</t>
+  </si>
+  <si>
+    <t>http://www.ucsd.edu</t>
   </si>
   <si>
     <t>http://www.weebly.com/?utm_source=internal&amp;utm_medium=footer&amp;utm_campaign=3</t>
@@ -1290,1791 +1366,2095 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>86</v>
+      <c r="A1" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>197</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>248</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F2" t="s">
-        <v>253</v>
+        <v>268</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>187</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>242</v>
+      </c>
+      <c r="G3" t="s">
+        <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F5" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
-        <v>300</v>
+        <v>318</v>
+      </c>
+      <c r="D6" t="s">
+        <v>225</v>
       </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>193</v>
+      </c>
+      <c r="F6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" header="0.5" footer="0.5" left="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>86</v>
+      <c r="A1" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>197</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>248</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="D2" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G3" t="s">
+        <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>129</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="C5" t="s">
-        <v>303</v>
+        <v>327</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="E5" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>129</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
       </c>
       <c r="I6" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="G7" t="s">
+        <v>129</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="G8" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F9" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G9" t="s">
+        <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F10" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G10" t="s">
+        <v>129</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="C11" t="s">
-        <v>301</v>
+        <v>325</v>
       </c>
       <c r="D11" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="E11" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F11" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G11" t="s">
+        <v>129</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E12" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F12" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G12" t="s">
+        <v>129</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E13" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F13" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G13" t="s">
+        <v>129</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="C14" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F14" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G14" t="s">
+        <v>129</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="C15" t="s">
-        <v>304</v>
+        <v>328</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E15" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F15" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="G15" t="s">
+        <v>129</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
-        <v>276</v>
+        <v>319</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="E16" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>205</v>
+      </c>
+      <c r="G16" t="s">
+        <v>129</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>224</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="E17" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F17" t="s">
-        <v>127</v>
+        <v>205</v>
+      </c>
+      <c r="G17" t="s">
+        <v>129</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>266</v>
       </c>
       <c r="C18" t="s">
-        <v>281</v>
+        <v>320</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="E18" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F18" t="s">
-        <v>127</v>
+        <v>205</v>
+      </c>
+      <c r="G18" t="s">
+        <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>260</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C19" t="s">
-        <v>285</v>
+        <v>321</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="E19" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>205</v>
+      </c>
+      <c r="G19" t="s">
+        <v>129</v>
       </c>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>206</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>245</v>
       </c>
       <c r="C20" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>265</v>
       </c>
       <c r="E20" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>205</v>
+      </c>
+      <c r="G20" t="s">
+        <v>129</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>275</v>
+        <v>312</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>278</v>
       </c>
       <c r="E21" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F21" t="s">
-        <v>127</v>
+        <v>205</v>
+      </c>
+      <c r="G21" t="s">
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>256</v>
-      </c>
-      <c r="B22" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="C22" t="s">
-        <v>282</v>
+        <v>323</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>265</v>
       </c>
       <c r="E22" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F22" t="s">
-        <v>127</v>
+        <v>205</v>
+      </c>
+      <c r="G22" t="s">
+        <v>129</v>
       </c>
       <c r="H22" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D23" t="s">
-        <v>262</v>
+        <v>112</v>
       </c>
       <c r="E23" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="G23" t="s">
+        <v>129</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="D24" t="s">
-        <v>243</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F24" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="G24" t="s">
+        <v>129</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D25" t="s">
-        <v>268</v>
+        <v>112</v>
       </c>
       <c r="E25" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="G25" t="s">
+        <v>129</v>
       </c>
       <c r="H25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>275</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>247</v>
       </c>
       <c r="C26" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="G26" t="s">
+        <v>129</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="G27" t="s">
+        <v>129</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>247</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="D28" t="s">
-        <v>247</v>
+        <v>112</v>
       </c>
       <c r="E28" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="G28" t="s">
+        <v>129</v>
       </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>238</v>
+        <v>271</v>
       </c>
       <c r="B29" t="s">
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>273</v>
+        <v>299</v>
       </c>
       <c r="D29" t="s">
-        <v>238</v>
+        <v>112</v>
       </c>
       <c r="E29" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F29" t="s">
-        <v>127</v>
+        <v>133</v>
+      </c>
+      <c r="G29" t="s">
+        <v>129</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="B30" t="s">
-        <v>239</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>311</v>
+      </c>
+      <c r="D30" t="s">
+        <v>277</v>
+      </c>
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>322</v>
+      </c>
+      <c r="D31" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
         <v>272</v>
       </c>
-      <c r="D30" t="s">
-        <v>306</v>
-      </c>
-      <c r="E30" t="s">
-        <v>188</v>
-      </c>
-      <c r="F30" t="s">
-        <v>127</v>
-      </c>
-      <c r="H30" t="s">
-        <v>83</v>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>326</v>
+      </c>
+      <c r="D32" t="s">
+        <v>284</v>
+      </c>
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" t="s">
+        <v>133</v>
+      </c>
+      <c r="G32" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>305</v>
+      </c>
+      <c r="D33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33" t="s">
+        <v>129</v>
+      </c>
+      <c r="H33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>260</v>
+      </c>
+      <c r="B35" t="s">
+        <v>261</v>
+      </c>
+      <c r="C35" t="s">
+        <v>290</v>
+      </c>
+      <c r="D35" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" t="s">
+        <v>129</v>
+      </c>
+      <c r="H35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>251</v>
+      </c>
+      <c r="B36" t="s">
+        <v>253</v>
+      </c>
+      <c r="C36" t="s">
+        <v>289</v>
+      </c>
+      <c r="D36" t="s">
+        <v>251</v>
+      </c>
+      <c r="E36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" t="s">
+        <v>129</v>
+      </c>
+      <c r="H36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>330</v>
+      </c>
+      <c r="B37" t="s">
+        <v>252</v>
+      </c>
+      <c r="C37" t="s">
+        <v>288</v>
+      </c>
+      <c r="D37" t="s">
+        <v>330</v>
+      </c>
+      <c r="E37" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" t="s">
+        <v>133</v>
+      </c>
+      <c r="G37" t="s">
+        <v>129</v>
+      </c>
+      <c r="H37" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" header="0.5" footer="0.5" left="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:A183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" bottom="1" header="0.5" footer="0.5" left="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Functional term definition/pointer function. Needs more terms to be added to both the program and the testbed.
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -11,7 +11,6 @@
     <s:sheet name="Second run" sheetId="2" r:id="rId2"/>
     <s:sheet name="List of Official Organizations" sheetId="3" r:id="rId3"/>
     <s:sheet name="List of Country Codes" sheetId="4" r:id="rId4"/>
-    <s:sheet name="List of Social Media" sheetId="5" r:id="rId5"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -19,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="580">
   <si>
     <t xml:space="preserve">
 </t>
@@ -178,6 +177,9 @@
     <t>African Academy of Sciences</t>
   </si>
   <si>
+    <t>Agriculture/Farming, Ecology</t>
+  </si>
+  <si>
     <t>Albanian  Academy of Sciences</t>
   </si>
   <si>
@@ -544,9 +546,6 @@
     <t>Ecological Society of America</t>
   </si>
   <si>
-    <t>Ecology, Agriculture/Farming</t>
-  </si>
-  <si>
     <t>Education</t>
   </si>
   <si>
@@ -775,6 +774,9 @@
     <t>IT = Italy</t>
   </si>
   <si>
+    <t>Image Collection, Activity, Portal, Data Service</t>
+  </si>
+  <si>
     <t>Images</t>
   </si>
   <si>
@@ -1222,9 +1224,6 @@
     <t>Portal, Data Service</t>
   </si>
   <si>
-    <t>Portal, Image Collection, Activity, Data Service</t>
-  </si>
-  <si>
     <t>QA = Qatar</t>
   </si>
   <si>
@@ -1486,6 +1485,9 @@
     <t>Tanzania Academy of Sciences</t>
   </si>
   <si>
+    <t>Term Definitions</t>
+  </si>
+  <si>
     <t>The  Wildlife Society (international)</t>
   </si>
   <si>
@@ -1640,6 +1642,15 @@
   </si>
   <si>
     <t>Zimbabwe  Academy of Sciences</t>
+  </si>
+  <si>
+    <t>[['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/bio.jpg, ', 'http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/bio.jpg, '], []]</t>
+  </si>
+  <si>
+    <t>[[], ['http://cinergiterms.weebly.com/uploads/7/5/1/1/7511984/catalog.jpg, ']]</t>
+  </si>
+  <si>
+    <t>[[], []]</t>
   </si>
   <si>
     <t>free website</t>
@@ -2099,11 +2110,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2111,85 +2122,91 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
-    <row spans="1:10" r="1">
-      <c t="s" s="1" r="A1">
-        <v>486</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>296</v>
-      </c>
-      <c t="s" s="1" r="C1">
-        <v>494</v>
-      </c>
-      <c t="s" s="1" r="D1">
-        <v>374</v>
-      </c>
-      <c t="s" s="1" r="E1">
-        <v>155</v>
-      </c>
-      <c t="s" s="1" r="F1">
+    <row spans="1:11" r="1">
+      <c s="1" t="s" r="A1">
+        <v>487</v>
+      </c>
+      <c s="1" t="s" r="B1">
+        <v>297</v>
+      </c>
+      <c s="1" t="s" r="C1">
+        <v>495</v>
+      </c>
+      <c s="1" t="s" r="D1">
+        <v>375</v>
+      </c>
+      <c s="1" t="s" r="E1">
+        <v>156</v>
+      </c>
+      <c s="1" t="s" r="F1">
         <v>403</v>
       </c>
-      <c t="s" s="1" r="G1">
-        <v>141</v>
-      </c>
-      <c t="s" s="1" r="H1">
+      <c s="1" t="s" r="G1">
+        <v>142</v>
+      </c>
+      <c s="1" t="s" r="H1">
         <v>473</v>
       </c>
-      <c t="s" s="1" r="I1">
-        <v>142</v>
-      </c>
-      <c t="s" s="1" r="J1">
+      <c s="1" t="s" r="I1">
+        <v>143</v>
+      </c>
+      <c s="1" t="s" r="J1">
         <v>454</v>
       </c>
-    </row>
-    <row spans="1:10" r="2">
+      <c s="1" t="s" r="K1">
+        <v>484</v>
+      </c>
+    </row>
+    <row spans="1:11" r="2">
       <c t="s" r="A2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c t="s" r="B2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c t="s" r="C2">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c t="s" r="D2">
         <v>192</v>
       </c>
       <c t="s" r="E2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c t="s" r="F2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c t="s" r="G2">
         <v>233</v>
       </c>
       <c t="s" r="H2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J2">
-        <v>326</v>
-      </c>
-    </row>
-    <row spans="1:10" r="3">
+        <v>327</v>
+      </c>
+      <c t="s" r="K2">
+        <v>539</v>
+      </c>
+    </row>
+    <row spans="1:11" r="3">
       <c t="s" r="A3">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c t="s" r="B3">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c t="s" r="C3">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c t="s" r="D3">
         <v>192</v>
       </c>
       <c t="s" r="E3">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c t="s" r="F3">
         <v>460</v>
@@ -2198,24 +2215,27 @@
         <v>233</v>
       </c>
       <c t="s" r="H3">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I3">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J3">
-        <v>326</v>
-      </c>
-    </row>
-    <row spans="1:10" r="4">
+        <v>327</v>
+      </c>
+      <c t="s" r="K3">
+        <v>537</v>
+      </c>
+    </row>
+    <row spans="1:11" r="4">
       <c t="s" r="A4">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c t="s" r="B4">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c t="s" r="C4">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c t="s" r="D4">
         <v>192</v>
@@ -2224,54 +2244,60 @@
         <v>462</v>
       </c>
       <c t="s" r="F4">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c t="s" r="G4">
         <v>233</v>
       </c>
       <c t="s" r="H4">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J4">
-        <v>326</v>
-      </c>
-    </row>
-    <row spans="1:10" r="5">
+        <v>327</v>
+      </c>
+      <c t="s" r="K4">
+        <v>538</v>
+      </c>
+    </row>
+    <row spans="1:11" r="5">
       <c t="s" r="A5">
         <v>222</v>
       </c>
       <c t="s" r="B5">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c t="s" r="C5">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c t="s" r="D5">
         <v>222</v>
       </c>
       <c t="s" r="E5">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F5">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G5">
         <v>233</v>
       </c>
       <c t="s" r="H5">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I5">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J5">
         <v>189</v>
       </c>
-    </row>
-    <row spans="1:10" r="6">
+      <c t="s" r="K5">
+        <v>539</v>
+      </c>
+    </row>
+    <row spans="1:11" r="6">
       <c t="s" r="A6">
         <v>440</v>
       </c>
@@ -2279,16 +2305,16 @@
         <v>0</v>
       </c>
       <c t="s" r="C6">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c t="s" r="D6">
         <v>440</v>
       </c>
       <c t="s" r="E6">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F6">
-        <v>396</v>
+        <v>247</v>
       </c>
       <c t="s" r="G6">
         <v>233</v>
@@ -2297,13 +2323,16 @@
         <v>171</v>
       </c>
       <c t="s" r="I6">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c t="s" r="J6">
-        <v>326</v>
-      </c>
-    </row>
-    <row spans="1:10" r="7">
+        <v>327</v>
+      </c>
+      <c t="s" r="K6">
+        <v>539</v>
+      </c>
+    </row>
+    <row spans="1:11" r="7">
       <c t="s" r="A7">
         <v>192</v>
       </c>
@@ -2311,30 +2340,30 @@
         <v>422</v>
       </c>
       <c t="s" r="C7">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c t="s" r="E7">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="J7">
-        <v>326</v>
-      </c>
-    </row>
-    <row spans="1:10" r="8">
+        <v>327</v>
+      </c>
+    </row>
+    <row spans="1:11" r="8">
       <c t="s" r="B8">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c t="s" r="C8">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" top="1" header="0.5" footer="0.5" left="0.75" bottom="1"/>
+  <pageMargins top="1" left="0.75" right="0.75" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -2347,55 +2376,55 @@
   <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
   <sheetData>
     <row spans="1:10" r="1">
-      <c t="s" s="1" r="A1">
-        <v>486</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>296</v>
-      </c>
-      <c t="s" s="1" r="C1">
-        <v>494</v>
-      </c>
-      <c t="s" s="1" r="D1">
-        <v>374</v>
-      </c>
-      <c t="s" s="1" r="E1">
-        <v>155</v>
-      </c>
-      <c t="s" s="1" r="F1">
+      <c s="1" t="s" r="A1">
+        <v>487</v>
+      </c>
+      <c s="1" t="s" r="B1">
+        <v>297</v>
+      </c>
+      <c s="1" t="s" r="C1">
+        <v>495</v>
+      </c>
+      <c s="1" t="s" r="D1">
+        <v>375</v>
+      </c>
+      <c s="1" t="s" r="E1">
+        <v>156</v>
+      </c>
+      <c s="1" t="s" r="F1">
         <v>403</v>
       </c>
-      <c t="s" s="1" r="G1">
-        <v>141</v>
-      </c>
-      <c t="s" s="1" r="H1">
+      <c s="1" t="s" r="G1">
+        <v>142</v>
+      </c>
+      <c s="1" t="s" r="H1">
         <v>473</v>
       </c>
-      <c t="s" s="1" r="I1">
-        <v>142</v>
-      </c>
-      <c t="s" s="1" r="J1">
+      <c s="1" t="s" r="I1">
+        <v>143</v>
+      </c>
+      <c s="1" t="s" r="J1">
         <v>453</v>
       </c>
     </row>
     <row spans="1:10" r="2">
       <c t="s" r="A2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c t="s" r="B2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c t="s" r="C2">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c t="s" r="D2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c t="s" r="E2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G2">
         <v>233</v>
@@ -2407,68 +2436,68 @@
         <v>204</v>
       </c>
       <c t="s" r="J2">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="3">
       <c t="s" r="A3">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c t="s" r="B3">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c t="s" r="C3">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c t="s" r="D3">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c t="s" r="E3">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F3">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c t="s" r="G3">
         <v>233</v>
       </c>
       <c t="s" r="I3">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c t="s" r="J3">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="4">
       <c t="s" r="A4">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c t="s" r="B4">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c t="s" r="C4">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c t="s" r="D4">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c t="s" r="E4">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F4">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c t="s" r="G4">
         <v>233</v>
       </c>
       <c t="s" r="H4">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I4">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J4">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="5">
@@ -2476,28 +2505,28 @@
         <v>235</v>
       </c>
       <c t="s" r="B5">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c t="s" r="C5">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c t="s" r="D5">
         <v>235</v>
       </c>
       <c t="s" r="E5">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F5">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c t="s" r="G5">
         <v>233</v>
       </c>
       <c t="s" r="I5">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c t="s" r="J5">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="6">
@@ -2508,28 +2537,28 @@
         <v>221</v>
       </c>
       <c t="s" r="C6">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c t="s" r="D6">
         <v>220</v>
       </c>
       <c t="s" r="E6">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F6">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c t="s" r="G6">
         <v>233</v>
       </c>
       <c t="s" r="H6">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I6">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J6">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="7">
@@ -2537,19 +2566,19 @@
         <v>6</v>
       </c>
       <c t="s" r="B7">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c t="s" r="C7">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c t="s" r="D7">
         <v>5</v>
       </c>
       <c t="s" r="E7">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F7">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c t="s" r="G7">
         <v>233</v>
@@ -2558,7 +2587,7 @@
         <v>181</v>
       </c>
       <c t="s" r="J7">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="8">
@@ -2566,31 +2595,31 @@
         <v>224</v>
       </c>
       <c t="s" r="B8">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c t="s" r="C8">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c t="s" r="D8">
         <v>222</v>
       </c>
       <c t="s" r="E8">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F8">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G8">
         <v>233</v>
       </c>
       <c t="s" r="H8">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I8">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J8">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="9">
@@ -2598,63 +2627,63 @@
         <v>225</v>
       </c>
       <c t="s" r="B9">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c t="s" r="C9">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c t="s" r="D9">
         <v>222</v>
       </c>
       <c t="s" r="E9">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F9">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G9">
         <v>233</v>
       </c>
       <c t="s" r="H9">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I9">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J9">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="10">
       <c t="s" r="A10">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c t="s" r="B10">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c t="s" r="C10">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c t="s" r="D10">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c t="s" r="E10">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F10">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G10">
         <v>233</v>
       </c>
       <c t="s" r="H10">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I10">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J10">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="11">
@@ -2662,31 +2691,31 @@
         <v>226</v>
       </c>
       <c t="s" r="B11">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c t="s" r="C11">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c t="s" r="D11">
         <v>222</v>
       </c>
       <c t="s" r="E11">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F11">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G11">
         <v>233</v>
       </c>
       <c t="s" r="H11">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I11">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J11">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="12">
@@ -2694,31 +2723,31 @@
         <v>223</v>
       </c>
       <c t="s" r="B12">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c t="s" r="C12">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c t="s" r="D12">
         <v>222</v>
       </c>
       <c t="s" r="E12">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F12">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G12">
         <v>233</v>
       </c>
       <c t="s" r="H12">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I12">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J12">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="13">
@@ -2726,31 +2755,31 @@
         <v>222</v>
       </c>
       <c t="s" r="B13">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c t="s" r="C13">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c t="s" r="D13">
         <v>222</v>
       </c>
       <c t="s" r="E13">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F13">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G13">
         <v>233</v>
       </c>
       <c t="s" r="H13">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I13">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J13">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="14">
@@ -2761,28 +2790,28 @@
         <v>449</v>
       </c>
       <c t="s" r="C14">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c t="s" r="D14">
         <v>222</v>
       </c>
       <c t="s" r="E14">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="F14">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c t="s" r="G14">
         <v>233</v>
       </c>
       <c t="s" r="H14">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I14">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J14">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="15">
@@ -2793,16 +2822,16 @@
         <v>463</v>
       </c>
       <c t="s" r="C15">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c t="s" r="D15">
         <v>440</v>
       </c>
       <c t="s" r="E15">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F15">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" r="G15">
         <v>233</v>
@@ -2811,10 +2840,10 @@
         <v>171</v>
       </c>
       <c t="s" r="I15">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c t="s" r="J15">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="16">
@@ -2825,16 +2854,16 @@
         <v>171</v>
       </c>
       <c t="s" r="C16">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c t="s" r="D16">
         <v>440</v>
       </c>
       <c t="s" r="E16">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F16">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" r="G16">
         <v>233</v>
@@ -2843,10 +2872,10 @@
         <v>171</v>
       </c>
       <c t="s" r="I16">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c t="s" r="J16">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="17">
@@ -2854,19 +2883,19 @@
         <v>6</v>
       </c>
       <c t="s" r="B17">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c t="s" r="C17">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c t="s" r="D17">
         <v>440</v>
       </c>
       <c t="s" r="E17">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F17">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" r="G17">
         <v>233</v>
@@ -2875,10 +2904,10 @@
         <v>171</v>
       </c>
       <c t="s" r="I17">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c t="s" r="J17">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="18">
@@ -2889,16 +2918,16 @@
         <v>461</v>
       </c>
       <c t="s" r="C18">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c t="s" r="D18">
         <v>440</v>
       </c>
       <c t="s" r="E18">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F18">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" r="G18">
         <v>233</v>
@@ -2907,10 +2936,10 @@
         <v>171</v>
       </c>
       <c t="s" r="I18">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c t="s" r="J18">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="19">
@@ -2921,16 +2950,16 @@
         <v>463</v>
       </c>
       <c t="s" r="C19">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c t="s" r="D19">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c t="s" r="E19">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F19">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" r="G19">
         <v>233</v>
@@ -2939,30 +2968,30 @@
         <v>171</v>
       </c>
       <c t="s" r="I19">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c t="s" r="J19">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="20">
       <c t="s" r="A20">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c t="s" r="B20">
         <v>402</v>
       </c>
       <c t="s" r="C20">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c t="s" r="D20">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c t="s" r="E20">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c t="s" r="F20">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c t="s" r="G20">
         <v>233</v>
@@ -2971,7 +3000,7 @@
         <v>171</v>
       </c>
       <c t="s" r="I20">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c t="s" r="J20">
         <v>191</v>
@@ -2979,98 +3008,98 @@
     </row>
     <row spans="1:10" r="21">
       <c t="s" r="A21">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c t="s" r="B21">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c t="s" r="C21">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c t="s" r="D21">
         <v>192</v>
       </c>
       <c t="s" r="E21">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F21">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G21">
         <v>233</v>
       </c>
       <c t="s" r="H21">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I21">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J21">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row spans="1:10" r="22">
       <c t="s" r="A22">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c t="s" r="B22">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c t="s" r="C22">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c t="s" r="D22">
         <v>192</v>
       </c>
       <c t="s" r="E22">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F22">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G22">
         <v>233</v>
       </c>
       <c t="s" r="H22">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I22">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J22">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="23">
       <c t="s" r="A23">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c t="s" r="B23">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c t="s" r="C23">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c t="s" r="D23">
         <v>192</v>
       </c>
       <c t="s" r="E23">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F23">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G23">
         <v>233</v>
       </c>
       <c t="s" r="H23">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I23">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J23">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="24">
@@ -3081,28 +3110,28 @@
         <v>465</v>
       </c>
       <c t="s" r="C24">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c t="s" r="D24">
         <v>192</v>
       </c>
       <c t="s" r="E24">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F24">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G24">
         <v>233</v>
       </c>
       <c t="s" r="H24">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I24">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J24">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="25">
@@ -3113,92 +3142,92 @@
         <v>174</v>
       </c>
       <c t="s" r="C25">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c t="s" r="D25">
         <v>192</v>
       </c>
       <c t="s" r="E25">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F25">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G25">
         <v>233</v>
       </c>
       <c t="s" r="H25">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I25">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J25">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="26">
       <c t="s" r="A26">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c t="s" r="B26">
         <v>45</v>
       </c>
       <c t="s" r="C26">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c t="s" r="D26">
         <v>192</v>
       </c>
       <c t="s" r="E26">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F26">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G26">
         <v>233</v>
       </c>
       <c t="s" r="H26">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I26">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J26">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="27">
       <c t="s" r="A27">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c t="s" r="B27">
         <v>172</v>
       </c>
       <c t="s" r="C27">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c t="s" r="D27">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c t="s" r="E27">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F27">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G27">
         <v>233</v>
       </c>
       <c t="s" r="H27">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I27">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J27">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="28">
@@ -3209,25 +3238,25 @@
         <v>1</v>
       </c>
       <c t="s" r="C28">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c t="s" r="D28">
         <v>236</v>
       </c>
       <c t="s" r="E28">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F28">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G28">
         <v>233</v>
       </c>
       <c t="s" r="H28">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I28">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J28">
         <v>189</v>
@@ -3235,107 +3264,107 @@
     </row>
     <row spans="1:10" r="29">
       <c t="s" r="A29">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c t="s" r="B29">
         <v>3</v>
       </c>
       <c t="s" r="C29">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c t="s" r="D29">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c t="s" r="E29">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F29">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G29">
         <v>233</v>
       </c>
       <c t="s" r="H29">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I29">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J29">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row spans="1:10" r="30">
       <c t="s" r="A30">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c t="s" r="B30">
         <v>4</v>
       </c>
       <c t="s" r="C30">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c t="s" r="D30">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c t="s" r="E30">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F30">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G30">
         <v>233</v>
       </c>
       <c t="s" r="H30">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I30">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J30">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:10" r="31">
       <c t="s" r="A31">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c t="s" r="B31">
         <v>2</v>
       </c>
       <c t="s" r="C31">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c t="s" r="D31">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c t="s" r="E31">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c t="s" r="F31">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" r="G31">
         <v>233</v>
       </c>
       <c t="s" r="H31">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c t="s" r="I31">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="J31">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" top="1" header="0.5" footer="0.5" left="0.75" bottom="1"/>
+  <pageMargins top="1" left="0.75" right="0.75" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -3459,257 +3488,257 @@
     </row>
     <row spans="1:1" r="24">
       <c t="s" r="A24">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row spans="1:1" r="25">
       <c t="s" r="A25">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row spans="1:1" r="26">
       <c t="s" r="A26">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row spans="1:1" r="27">
       <c t="s" r="A27">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row spans="1:1" r="28">
       <c t="s" r="A28">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row spans="1:1" r="29">
       <c t="s" r="A29">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row spans="1:1" r="30">
       <c t="s" r="A30">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row spans="1:1" r="31">
       <c t="s" r="A31">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row spans="1:1" r="32">
       <c t="s" r="A32">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row spans="1:1" r="33">
       <c t="s" r="A33">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row spans="1:1" r="34">
       <c t="s" r="A34">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row spans="1:1" r="35">
       <c t="s" r="A35">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row spans="1:1" r="36">
       <c t="s" r="A36">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row spans="1:1" r="37">
       <c t="s" r="A37">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row spans="1:1" r="38">
       <c t="s" r="A38">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row spans="1:1" r="39">
       <c t="s" r="A39">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row spans="1:1" r="40">
       <c t="s" r="A40">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row spans="1:1" r="41">
       <c t="s" r="A41">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row spans="1:1" r="42">
       <c t="s" r="A42">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row spans="1:1" r="43">
       <c t="s" r="A43">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row spans="1:1" r="44">
       <c t="s" r="A44">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row spans="1:1" r="45">
       <c t="s" r="A45">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row spans="1:1" r="46">
       <c t="s" r="A46">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row spans="1:1" r="47">
       <c t="s" r="A47">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row spans="1:1" r="48">
       <c t="s" r="A48">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row spans="1:1" r="49">
       <c t="s" r="A49">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row spans="1:1" r="50">
       <c t="s" r="A50">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row spans="1:1" r="51">
       <c t="s" r="A51">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row spans="1:1" r="52">
       <c t="s" r="A52">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row spans="1:1" r="53">
       <c t="s" r="A53">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row spans="1:1" r="54">
       <c t="s" r="A54">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row spans="1:1" r="55">
       <c t="s" r="A55">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row spans="1:1" r="56">
       <c t="s" r="A56">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row spans="1:1" r="57">
       <c t="s" r="A57">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row spans="1:1" r="58">
       <c t="s" r="A58">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row spans="1:1" r="59">
       <c t="s" r="A59">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row spans="1:1" r="60">
       <c t="s" r="A60">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row spans="1:1" r="61">
       <c t="s" r="A61">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row spans="1:1" r="62">
       <c t="s" r="A62">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row spans="1:1" r="63">
       <c t="s" r="A63">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row spans="1:1" r="64">
       <c t="s" r="A64">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row spans="1:1" r="65">
       <c t="s" r="A65">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row spans="1:1" r="66">
       <c t="s" r="A66">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row spans="1:1" r="67">
       <c t="s" r="A67">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row spans="1:1" r="68">
       <c t="s" r="A68">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row spans="1:1" r="69">
       <c t="s" r="A69">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row spans="1:1" r="70">
       <c t="s" r="A70">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row spans="1:1" r="71">
       <c t="s" r="A71">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row spans="1:1" r="72">
       <c t="s" r="A72">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row spans="1:1" r="73">
       <c t="s" r="A73">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row spans="1:1" r="74">
       <c t="s" r="A74">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row spans="1:1" r="75">
@@ -3784,267 +3813,267 @@
     </row>
     <row spans="1:1" r="89">
       <c t="s" r="A89">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row spans="1:1" r="90">
       <c t="s" r="A90">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row spans="1:1" r="91">
       <c t="s" r="A91">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row spans="1:1" r="92">
       <c t="s" r="A92">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row spans="1:1" r="93">
       <c t="s" r="A93">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row spans="1:1" r="94">
       <c t="s" r="A94">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row spans="1:1" r="95">
       <c t="s" r="A95">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row spans="1:1" r="96">
       <c t="s" r="A96">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row spans="1:1" r="97">
       <c t="s" r="A97">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row spans="1:1" r="98">
       <c t="s" r="A98">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row spans="1:1" r="99">
       <c t="s" r="A99">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row spans="1:1" r="100">
       <c t="s" r="A100">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row spans="1:1" r="101">
       <c t="s" r="A101">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row spans="1:1" r="102">
       <c t="s" r="A102">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row spans="1:1" r="103">
       <c t="s" r="A103">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row spans="1:1" r="104">
       <c t="s" r="A104">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row spans="1:1" r="105">
       <c t="s" r="A105">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row spans="1:1" r="106">
       <c t="s" r="A106">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row spans="1:1" r="107">
       <c t="s" r="A107">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row spans="1:1" r="108">
       <c t="s" r="A108">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row spans="1:1" r="109">
       <c t="s" r="A109">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row spans="1:1" r="110">
       <c t="s" r="A110">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row spans="1:1" r="111">
       <c t="s" r="A111">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row spans="1:1" r="112">
       <c t="s" r="A112">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row spans="1:1" r="113">
       <c t="s" r="A113">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row spans="1:1" r="114">
       <c t="s" r="A114">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row spans="1:1" r="115">
       <c t="s" r="A115">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row spans="1:1" r="116">
       <c t="s" r="A116">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row spans="1:1" r="117">
       <c t="s" r="A117">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row spans="1:1" r="118">
       <c t="s" r="A118">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row spans="1:1" r="119">
       <c t="s" r="A119">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row spans="1:1" r="120">
       <c t="s" r="A120">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row spans="1:1" r="121">
       <c t="s" r="A121">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row spans="1:1" r="122">
       <c t="s" r="A122">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row spans="1:1" r="123">
       <c t="s" r="A123">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row spans="1:1" r="124">
       <c t="s" r="A124">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row spans="1:1" r="125">
       <c t="s" r="A125">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row spans="1:1" r="126">
       <c t="s" r="A126">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row spans="1:1" r="127">
       <c t="s" r="A127">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row spans="1:1" r="128">
       <c t="s" r="A128">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row spans="1:1" r="129">
       <c t="s" r="A129">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row spans="1:1" r="130">
       <c t="s" r="A130">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row spans="1:1" r="131">
       <c t="s" r="A131">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row spans="1:1" r="132">
       <c t="s" r="A132">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row spans="1:1" r="133">
       <c t="s" r="A133">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row spans="1:1" r="134">
       <c t="s" r="A134">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row spans="1:1" r="135">
       <c t="s" r="A135">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row spans="1:1" r="136">
       <c t="s" r="A136">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row spans="1:1" r="137">
       <c t="s" r="A137">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row spans="1:1" r="138">
       <c t="s" r="A138">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row spans="1:1" r="139">
       <c t="s" r="A139">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row spans="1:1" r="140">
       <c t="s" r="A140">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row spans="1:1" r="141">
       <c t="s" r="A141">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row spans="1:1" r="142">
@@ -4199,71 +4228,71 @@
     </row>
     <row spans="1:1" r="172">
       <c t="s" r="A172">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row spans="1:1" r="173">
       <c t="s" r="A173">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row spans="1:1" r="174">
       <c t="s" r="A174">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row spans="1:1" r="175">
       <c t="s" r="A175">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row spans="1:1" r="176">
       <c t="s" r="A176">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row spans="1:1" r="177">
       <c t="s" r="A177">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row spans="1:1" r="178">
       <c t="s" r="A178">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row spans="1:1" r="179">
       <c t="s" r="A179">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row spans="1:1" r="180">
       <c t="s" r="A180">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row spans="1:1" r="181">
       <c t="s" r="A181">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row spans="1:1" r="182">
       <c t="s" r="A182">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row spans="1:1" r="183">
       <c t="s" r="A183">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" top="1" header="0.5" footer="0.5" left="0.75" bottom="1"/>
+  <pageMargins top="1" left="0.75" right="0.75" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -4357,252 +4386,252 @@
     </row>
     <row spans="1:1" r="17">
       <c t="s" r="A17">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row spans="1:1" r="18">
       <c t="s" r="A18">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row spans="1:1" r="19">
       <c t="s" r="A19">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row spans="1:1" r="20">
       <c t="s" r="A20">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row spans="1:1" r="21">
       <c t="s" r="A21">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row spans="1:1" r="22">
       <c t="s" r="A22">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row spans="1:1" r="23">
       <c t="s" r="A23">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row spans="1:1" r="24">
       <c t="s" r="A24">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row spans="1:1" r="25">
       <c t="s" r="A25">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row spans="1:1" r="26">
       <c t="s" r="A26">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row spans="1:1" r="27">
       <c t="s" r="A27">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row spans="1:1" r="28">
       <c t="s" r="A28">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row spans="1:1" r="29">
       <c t="s" r="A29">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row spans="1:1" r="30">
       <c t="s" r="A30">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row spans="1:1" r="31">
       <c t="s" r="A31">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row spans="1:1" r="32">
       <c t="s" r="A32">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row spans="1:1" r="33">
       <c t="s" r="A33">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row spans="1:1" r="34">
       <c t="s" r="A34">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row spans="1:1" r="35">
       <c t="s" r="A35">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row spans="1:1" r="36">
       <c t="s" r="A36">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row spans="1:1" r="37">
       <c t="s" r="A37">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row spans="1:1" r="38">
       <c t="s" r="A38">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row spans="1:1" r="39">
       <c t="s" r="A39">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row spans="1:1" r="40">
       <c t="s" r="A40">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row spans="1:1" r="41">
       <c t="s" r="A41">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row spans="1:1" r="42">
       <c t="s" r="A42">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row spans="1:1" r="43">
       <c t="s" r="A43">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row spans="1:1" r="44">
       <c t="s" r="A44">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row spans="1:1" r="45">
       <c t="s" r="A45">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row spans="1:1" r="46">
       <c t="s" r="A46">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row spans="1:1" r="47">
       <c t="s" r="A47">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row spans="1:1" r="48">
       <c t="s" r="A48">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row spans="1:1" r="49">
       <c t="s" r="A49">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row spans="1:1" r="50">
       <c t="s" r="A50">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row spans="1:1" r="51">
       <c t="s" r="A51">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row spans="1:1" r="52">
       <c t="s" r="A52">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row spans="1:1" r="53">
       <c t="s" r="A53">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row spans="1:1" r="54">
       <c t="s" r="A54">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row spans="1:1" r="55">
       <c t="s" r="A55">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row spans="1:1" r="56">
       <c t="s" r="A56">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row spans="1:1" r="57">
       <c t="s" r="A57">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row spans="1:1" r="58">
       <c t="s" r="A58">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row spans="1:1" r="59">
       <c t="s" r="A59">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row spans="1:1" r="60">
       <c t="s" r="A60">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row spans="1:1" r="61">
       <c t="s" r="A61">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row spans="1:1" r="62">
       <c t="s" r="A62">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row spans="1:1" r="63">
       <c t="s" r="A63">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row spans="1:1" r="64">
       <c t="s" r="A64">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row spans="1:1" r="65">
       <c t="s" r="A65">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row spans="1:1" r="66">
       <c t="s" r="A66">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row spans="1:1" r="67">
@@ -4807,367 +4836,367 @@
     </row>
     <row spans="1:1" r="107">
       <c t="s" r="A107">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row spans="1:1" r="108">
       <c t="s" r="A108">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row spans="1:1" r="109">
       <c t="s" r="A109">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row spans="1:1" r="110">
       <c t="s" r="A110">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row spans="1:1" r="111">
       <c t="s" r="A111">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row spans="1:1" r="112">
       <c t="s" r="A112">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row spans="1:1" r="113">
       <c t="s" r="A113">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row spans="1:1" r="114">
       <c t="s" r="A114">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row spans="1:1" r="115">
       <c t="s" r="A115">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row spans="1:1" r="116">
       <c t="s" r="A116">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row spans="1:1" r="117">
       <c t="s" r="A117">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row spans="1:1" r="118">
       <c t="s" r="A118">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row spans="1:1" r="119">
       <c t="s" r="A119">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row spans="1:1" r="120">
       <c t="s" r="A120">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row spans="1:1" r="121">
       <c t="s" r="A121">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row spans="1:1" r="122">
       <c t="s" r="A122">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row spans="1:1" r="123">
       <c t="s" r="A123">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row spans="1:1" r="124">
       <c t="s" r="A124">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row spans="1:1" r="125">
       <c t="s" r="A125">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row spans="1:1" r="126">
       <c t="s" r="A126">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row spans="1:1" r="127">
       <c t="s" r="A127">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row spans="1:1" r="128">
       <c t="s" r="A128">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row spans="1:1" r="129">
       <c t="s" r="A129">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row spans="1:1" r="130">
       <c t="s" r="A130">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row spans="1:1" r="131">
       <c t="s" r="A131">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row spans="1:1" r="132">
       <c t="s" r="A132">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row spans="1:1" r="133">
       <c t="s" r="A133">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row spans="1:1" r="134">
       <c t="s" r="A134">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row spans="1:1" r="135">
       <c t="s" r="A135">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row spans="1:1" r="136">
       <c t="s" r="A136">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row spans="1:1" r="137">
       <c t="s" r="A137">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row spans="1:1" r="138">
       <c t="s" r="A138">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row spans="1:1" r="139">
       <c t="s" r="A139">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row spans="1:1" r="140">
       <c t="s" r="A140">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row spans="1:1" r="141">
       <c t="s" r="A141">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row spans="1:1" r="142">
       <c t="s" r="A142">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row spans="1:1" r="143">
       <c t="s" r="A143">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row spans="1:1" r="144">
       <c t="s" r="A144">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row spans="1:1" r="145">
       <c t="s" r="A145">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row spans="1:1" r="146">
       <c t="s" r="A146">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row spans="1:1" r="147">
       <c t="s" r="A147">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row spans="1:1" r="148">
       <c t="s" r="A148">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row spans="1:1" r="149">
       <c t="s" r="A149">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row spans="1:1" r="150">
       <c t="s" r="A150">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row spans="1:1" r="151">
       <c t="s" r="A151">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row spans="1:1" r="152">
       <c t="s" r="A152">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row spans="1:1" r="153">
       <c t="s" r="A153">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row spans="1:1" r="154">
       <c t="s" r="A154">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row spans="1:1" r="155">
       <c t="s" r="A155">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row spans="1:1" r="156">
       <c t="s" r="A156">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row spans="1:1" r="157">
       <c t="s" r="A157">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row spans="1:1" r="158">
       <c t="s" r="A158">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row spans="1:1" r="159">
       <c t="s" r="A159">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row spans="1:1" r="160">
       <c t="s" r="A160">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row spans="1:1" r="161">
       <c t="s" r="A161">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row spans="1:1" r="162">
       <c t="s" r="A162">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row spans="1:1" r="163">
       <c t="s" r="A163">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row spans="1:1" r="164">
       <c t="s" r="A164">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row spans="1:1" r="165">
       <c t="s" r="A165">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row spans="1:1" r="166">
       <c t="s" r="A166">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row spans="1:1" r="167">
       <c t="s" r="A167">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row spans="1:1" r="168">
       <c t="s" r="A168">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row spans="1:1" r="169">
       <c t="s" r="A169">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row spans="1:1" r="170">
       <c t="s" r="A170">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row spans="1:1" r="171">
       <c t="s" r="A171">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row spans="1:1" r="172">
       <c t="s" r="A172">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row spans="1:1" r="173">
       <c t="s" r="A173">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row spans="1:1" r="174">
       <c t="s" r="A174">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row spans="1:1" r="175">
       <c t="s" r="A175">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row spans="1:1" r="176">
       <c t="s" r="A176">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row spans="1:1" r="177">
       <c t="s" r="A177">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row spans="1:1" r="178">
       <c t="s" r="A178">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row spans="1:1" r="179">
       <c t="s" r="A179">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row spans="1:1" r="180">
@@ -5377,127 +5406,127 @@
     </row>
     <row spans="1:1" r="221">
       <c t="s" r="A221">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row spans="1:1" r="222">
       <c t="s" r="A222">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row spans="1:1" r="223">
       <c t="s" r="A223">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row spans="1:1" r="224">
       <c t="s" r="A224">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row spans="1:1" r="225">
       <c t="s" r="A225">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row spans="1:1" r="226">
       <c t="s" r="A226">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row spans="1:1" r="227">
       <c t="s" r="A227">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row spans="1:1" r="228">
       <c t="s" r="A228">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row spans="1:1" r="229">
       <c t="s" r="A229">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row spans="1:1" r="230">
       <c t="s" r="A230">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row spans="1:1" r="231">
       <c t="s" r="A231">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row spans="1:1" r="232">
       <c t="s" r="A232">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row spans="1:1" r="233">
       <c t="s" r="A233">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row spans="1:1" r="234">
       <c t="s" r="A234">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row spans="1:1" r="235">
       <c t="s" r="A235">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row spans="1:1" r="236">
       <c t="s" r="A236">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row spans="1:1" r="237">
       <c t="s" r="A237">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row spans="1:1" r="238">
       <c t="s" r="A238">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row spans="1:1" r="239">
       <c t="s" r="A239">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row spans="1:1" r="240">
       <c t="s" r="A240">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row spans="1:1" r="241">
       <c t="s" r="A241">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row spans="1:1" r="242">
       <c t="s" r="A242">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row spans="1:1" r="243">
       <c t="s" r="A243">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row spans="1:1" r="244">
       <c t="s" r="A244">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row spans="1:1" r="245">
       <c t="s" r="A245">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row spans="1:1" r="246">
@@ -5512,17 +5541,17 @@
     </row>
     <row spans="1:1" r="248">
       <c t="s" r="A248">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row spans="1:1" r="249">
       <c t="s" r="A249">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row spans="1:1" r="250">
       <c t="s" r="A250">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row spans="1:1" r="251">
@@ -5532,73 +5561,15 @@
     </row>
     <row spans="1:1" r="252">
       <c t="s" r="A252">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row spans="1:1" r="253">
       <c t="s" r="A253">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" top="1" header="0.5" footer="0.5" left="0.75" bottom="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" baseColWidth="10"/>
-  <sheetData>
-    <row spans="1:2" r="1">
-      <c t="s" r="A1">
-        <v>326</v>
-      </c>
-      <c t="s" r="B1">
-        <v>547</v>
-      </c>
-    </row>
-    <row spans="1:2" r="2">
-      <c t="s" r="A2">
-        <v>517</v>
-      </c>
-      <c t="s" r="B2">
-        <v>539</v>
-      </c>
-    </row>
-    <row spans="1:2" r="3">
-      <c t="s" r="A3">
-        <v>326</v>
-      </c>
-      <c t="s" r="B3">
-        <v>557</v>
-      </c>
-    </row>
-    <row spans="1:2" r="4">
-      <c t="s" r="A4">
-        <v>326</v>
-      </c>
-      <c t="s" r="B4">
-        <v>568</v>
-      </c>
-    </row>
-    <row spans="1:2" r="5">
-      <c t="s" r="A5">
-        <v>326</v>
-      </c>
-      <c t="s" r="B5">
-        <v>552</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins right="0.75" top="1" header="0.5" footer="0.5" left="0.75" bottom="1"/>
+  <pageMargins top="1" left="0.75" right="0.75" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working recursive version, for two runs. Needs to be tested on more than two.
</commit_message>
<xml_diff>
--- a/Crawl.xlsx
+++ b/Crawl.xlsx
@@ -7,8 +7,8 @@
     <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet name="First run" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Second run" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <s:sheet name="0" sheetId="2" r:id="rId2"/>
     <s:sheet name="List of Official Organizations" sheetId="3" r:id="rId3"/>
     <s:sheet name="List of Country Codes" sheetId="4" r:id="rId4"/>
   </s:sheets>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="466">
   <si>
     <t>AD = Andorra</t>
   </si>
@@ -131,6 +131,9 @@
     <t>Accademia  Nazionale dei Lincei, Italy</t>
   </si>
   <si>
+    <t>Activity, Data Service, Image Collection, Portal</t>
+  </si>
+  <si>
     <t>Africa  Centre for Climate and Earth Systems Science</t>
   </si>
   <si>
@@ -317,6 +320,12 @@
     <t>CI = Cote D'Ivoire (Ivory Coast)</t>
   </si>
   <si>
+    <t>CINERGI WEB CRAWLER sheet 1 - Home</t>
+  </si>
+  <si>
+    <t>CINERGI WEb crawler sheet 2 - Home</t>
+  </si>
+  <si>
     <t>CK = Cook Islands</t>
   </si>
   <si>
@@ -356,6 +365,9 @@
     <t>CZ = Czech Republic</t>
   </si>
   <si>
+    <t>Cadastral, Human Dimensions</t>
+  </si>
+  <si>
     <t>California  Academy of Sciences</t>
   </si>
   <si>
@@ -377,6 +389,9 @@
     <t>Canadian Meteorological and Oceanographic Society</t>
   </si>
   <si>
+    <t>Catalog</t>
+  </si>
+  <si>
     <t>Center  for International Forestry Research</t>
   </si>
   <si>
@@ -386,6 +401,9 @@
     <t>Commonwealth  Scientific and Industrial Research Organization (CSIRO) (Australia)</t>
   </si>
   <si>
+    <t>Community</t>
+  </si>
+  <si>
     <t>Consultative  Group on International Agricultural Research</t>
   </si>
   <si>
@@ -500,6 +518,9 @@
     <t>Federation of American  Scientists</t>
   </si>
   <si>
+    <t>Free website | Free blog | Create a free website | Weebly</t>
+  </si>
+  <si>
     <t>French Academy of Sciences</t>
   </si>
   <si>
@@ -578,6 +599,9 @@
     <t>Ghana  Academy of Arts and Sciences</t>
   </si>
   <si>
+    <t>Google</t>
+  </si>
+  <si>
     <t>HK = Hong Kong</t>
   </si>
   <si>
@@ -593,6 +617,9 @@
     <t>HT = Haiti</t>
   </si>
   <si>
+    <t>HTTP</t>
+  </si>
+  <si>
     <t>HU = Hungary</t>
   </si>
   <si>
@@ -950,6 +977,12 @@
     <t>Nigerian  Academy of Sciences</t>
   </si>
   <si>
+    <t>No disciplines found</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Norwegian Academy of Sciences and  Letters</t>
   </si>
   <si>
@@ -1139,6 +1172,9 @@
     <t>SZ = Swaziland</t>
   </si>
   <si>
+    <t>San Diego Supercomputer Center</t>
+  </si>
+  <si>
     <t>Sb = Solomon Islands</t>
   </si>
   <si>
@@ -1166,6 +1202,9 @@
     <t>Slovenian Academy of Sciences and Arts</t>
   </si>
   <si>
+    <t>Social Media?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Society  of American Foresters  </t>
   </si>
   <si>
@@ -1181,6 +1220,9 @@
     <t>Society of Systematic Biologists</t>
   </si>
   <si>
+    <t>Software</t>
+  </si>
+  <si>
     <t>Sudan Academy of Sciences</t>
   </si>
   <si>
@@ -1238,6 +1280,9 @@
     <t>Tanzania Academy of Sciences</t>
   </si>
   <si>
+    <t>Term Definitions</t>
+  </si>
+  <si>
     <t>The  Wildlife Society (international)</t>
   </si>
   <si>
@@ -1310,6 +1355,9 @@
     <t>WS = Samoa</t>
   </si>
   <si>
+    <t>Welcome to Facebook - Log In, Sign Up or Learn More</t>
+  </si>
+  <si>
     <t>Woods Hole Oceanographic Institution</t>
   </si>
   <si>
@@ -1347,6 +1395,24 @@
   </si>
   <si>
     <t>Zimbabwe  Academy of Sciences</t>
+  </si>
+  <si>
+    <t>http://cinergisheet1.weebly.com</t>
+  </si>
+  <si>
+    <t>http://cinergisheet2.weebly.com</t>
+  </si>
+  <si>
+    <t>http://facebook.com</t>
+  </si>
+  <si>
+    <t>http://google.com</t>
+  </si>
+  <si>
+    <t>http://www.sdsc.edu</t>
+  </si>
+  <si>
+    <t>http://www.weebly.com/?utm_source=internal&amp;utm_medium=footer&amp;utm_campaign=3</t>
   </si>
   <si>
     <t>l'Académie  des Sciences et Techniques du Sénégal</t>
@@ -1691,9 +1757,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1" activeCell="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins header="0.5" left="0.75" bottom="1" right="0.75" top="1" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
+  </sheetPr>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -1701,91 +1784,210 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:9" r="1">
-      <c t="s" r="A1" s="1">
-        <v>407</v>
-      </c>
-      <c t="s" r="B1" s="1">
-        <v>247</v>
-      </c>
-      <c t="s" r="C1" s="1">
-        <v>413</v>
-      </c>
-      <c t="s" r="D1" s="1">
-        <v>314</v>
-      </c>
-      <c t="s" r="E1" s="1">
-        <v>134</v>
-      </c>
-      <c t="s" r="F1" s="1">
-        <v>338</v>
-      </c>
-      <c t="s" r="G1" s="1">
+    <row spans="1:11" r="1">
+      <c s="1" t="s" r="A1">
+        <v>422</v>
+      </c>
+      <c s="1" t="s" r="B1">
+        <v>256</v>
+      </c>
+      <c s="1" t="s" r="C1">
+        <v>428</v>
+      </c>
+      <c s="1" t="s" r="D1">
+        <v>325</v>
+      </c>
+      <c s="1" t="s" r="E1">
+        <v>140</v>
+      </c>
+      <c s="1" t="s" r="F1">
+        <v>349</v>
+      </c>
+      <c s="1" t="s" r="G1">
+        <v>129</v>
+      </c>
+      <c s="1" t="s" r="H1">
+        <v>409</v>
+      </c>
+      <c s="1" t="s" r="I1">
+        <v>130</v>
+      </c>
+      <c s="1" t="s" r="J1">
+        <v>394</v>
+      </c>
+      <c s="1" t="s" r="K1">
+        <v>420</v>
+      </c>
+    </row>
+    <row spans="1:11" r="2">
+      <c t="s" r="A2">
+        <v>100</v>
+      </c>
+      <c t="s" r="C2">
+        <v>459</v>
+      </c>
+      <c t="s" r="D2">
+        <v>100</v>
+      </c>
+      <c t="s" r="E2">
+        <v>319</v>
+      </c>
+      <c t="s" r="F2">
+        <v>400</v>
+      </c>
+      <c t="s" r="G2">
+        <v>199</v>
+      </c>
+    </row>
+    <row spans="1:11" r="3">
+      <c t="s" r="A3">
+        <v>101</v>
+      </c>
+      <c t="s" r="C3">
+        <v>460</v>
+      </c>
+      <c t="s" r="D3">
+        <v>101</v>
+      </c>
+      <c t="s" r="E3">
+        <v>319</v>
+      </c>
+      <c t="s" r="F3">
         <v>123</v>
       </c>
-      <c t="s" r="H1" s="1">
-        <v>395</v>
-      </c>
-      <c t="s" r="I1" s="1">
-        <v>124</v>
+      <c t="s" r="G3">
+        <v>199</v>
+      </c>
+    </row>
+    <row spans="1:11" r="4">
+      <c t="s" r="A4">
+        <v>445</v>
+      </c>
+      <c t="s" r="C4">
+        <v>461</v>
+      </c>
+      <c t="s" r="D4">
+        <v>445</v>
+      </c>
+      <c t="s" r="E4">
+        <v>319</v>
+      </c>
+      <c t="s" r="F4">
+        <v>320</v>
+      </c>
+      <c t="s" r="G4">
+        <v>199</v>
+      </c>
+    </row>
+    <row spans="1:11" r="5">
+      <c t="s" r="A5">
+        <v>193</v>
+      </c>
+      <c t="s" r="C5">
+        <v>462</v>
+      </c>
+      <c t="s" r="D5">
+        <v>193</v>
+      </c>
+      <c t="s" r="E5">
+        <v>319</v>
+      </c>
+      <c t="s" r="F5">
+        <v>320</v>
+      </c>
+      <c t="s" r="G5">
+        <v>199</v>
+      </c>
+    </row>
+    <row spans="1:11" r="6">
+      <c t="s" r="A6">
+        <v>384</v>
+      </c>
+      <c t="s" r="C6">
+        <v>463</v>
+      </c>
+      <c t="s" r="D6">
+        <v>384</v>
+      </c>
+      <c t="s" r="E6">
+        <v>115</v>
+      </c>
+      <c t="s" r="F6">
+        <v>37</v>
+      </c>
+      <c t="s" r="G6">
+        <v>199</v>
+      </c>
+    </row>
+    <row spans="1:11" r="7">
+      <c t="s" r="A7">
+        <v>166</v>
+      </c>
+      <c t="s" r="C7">
+        <v>464</v>
+      </c>
+      <c t="s" r="D7">
+        <v>166</v>
+      </c>
+      <c t="s" r="E7">
+        <v>319</v>
+      </c>
+      <c t="s" r="F7">
+        <v>127</v>
+      </c>
+      <c t="s" r="G7">
+        <v>199</v>
+      </c>
+    </row>
+    <row spans="1:11" r="8">
+      <c t="s" r="A8">
+        <v>166</v>
+      </c>
+      <c t="s" r="C8">
+        <v>464</v>
+      </c>
+      <c t="s" r="D8">
+        <v>166</v>
+      </c>
+      <c t="s" r="E8">
+        <v>319</v>
+      </c>
+      <c t="s" r="F8">
+        <v>127</v>
+      </c>
+      <c t="s" r="G8">
+        <v>199</v>
+      </c>
+    </row>
+    <row spans="1:11" r="9">
+      <c t="s" r="A9">
+        <v>166</v>
+      </c>
+      <c t="s" r="C9">
+        <v>464</v>
+      </c>
+      <c t="s" r="D9">
+        <v>166</v>
+      </c>
+      <c t="s" r="E9">
+        <v>319</v>
+      </c>
+      <c t="s" r="F9">
+        <v>127</v>
+      </c>
+      <c t="s" r="G9">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" footer="0.5" header="0.5" right="0.75" bottom="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row spans="1:9" r="1">
-      <c t="s" r="A1" s="1">
-        <v>407</v>
-      </c>
-      <c t="s" r="B1" s="1">
-        <v>247</v>
-      </c>
-      <c t="s" r="C1" s="1">
-        <v>413</v>
-      </c>
-      <c t="s" r="D1" s="1">
-        <v>314</v>
-      </c>
-      <c t="s" r="E1" s="1">
-        <v>134</v>
-      </c>
-      <c t="s" r="F1" s="1">
-        <v>338</v>
-      </c>
-      <c t="s" r="G1" s="1">
-        <v>123</v>
-      </c>
-      <c t="s" r="H1" s="1">
-        <v>395</v>
-      </c>
-      <c t="s" r="I1" s="1">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins top="1" left="0.75" footer="0.5" header="0.5" right="0.75" bottom="1"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" right="0.75" top="1" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A183"/>
   <sheetViews>
@@ -1897,823 +2099,823 @@
     </row>
     <row spans="1:1" r="22">
       <c t="s" r="A22">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row spans="1:1" r="23">
       <c t="s" r="A23">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row spans="1:1" r="24">
       <c t="s" r="A24">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row spans="1:1" r="25">
       <c t="s" r="A25">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row spans="1:1" r="26">
       <c t="s" r="A26">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row spans="1:1" r="27">
       <c t="s" r="A27">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row spans="1:1" r="28">
       <c t="s" r="A28">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row spans="1:1" r="29">
       <c t="s" r="A29">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row spans="1:1" r="30">
       <c t="s" r="A30">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row spans="1:1" r="31">
       <c t="s" r="A31">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row spans="1:1" r="32">
       <c t="s" r="A32">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row spans="1:1" r="33">
       <c t="s" r="A33">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row spans="1:1" r="34">
       <c t="s" r="A34">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row spans="1:1" r="35">
       <c t="s" r="A35">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row spans="1:1" r="36">
       <c t="s" r="A36">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row spans="1:1" r="37">
       <c t="s" r="A37">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row spans="1:1" r="38">
       <c t="s" r="A38">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row spans="1:1" r="39">
       <c t="s" r="A39">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row spans="1:1" r="40">
       <c t="s" r="A40">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row spans="1:1" r="41">
       <c t="s" r="A41">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row spans="1:1" r="42">
       <c t="s" r="A42">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row spans="1:1" r="43">
       <c t="s" r="A43">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row spans="1:1" r="44">
       <c t="s" r="A44">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row spans="1:1" r="45">
       <c t="s" r="A45">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row spans="1:1" r="46">
       <c t="s" r="A46">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row spans="1:1" r="47">
       <c t="s" r="A47">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row spans="1:1" r="48">
       <c t="s" r="A48">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row spans="1:1" r="49">
       <c t="s" r="A49">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row spans="1:1" r="50">
       <c t="s" r="A50">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row spans="1:1" r="51">
       <c t="s" r="A51">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row spans="1:1" r="52">
       <c t="s" r="A52">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row spans="1:1" r="53">
       <c t="s" r="A53">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row spans="1:1" r="54">
       <c t="s" r="A54">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row spans="1:1" r="55">
       <c t="s" r="A55">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row spans="1:1" r="56">
       <c t="s" r="A56">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row spans="1:1" r="57">
       <c t="s" r="A57">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row spans="1:1" r="58">
       <c t="s" r="A58">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row spans="1:1" r="59">
       <c t="s" r="A59">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row spans="1:1" r="60">
       <c t="s" r="A60">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row spans="1:1" r="61">
       <c t="s" r="A61">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row spans="1:1" r="62">
       <c t="s" r="A62">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row spans="1:1" r="63">
       <c t="s" r="A63">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row spans="1:1" r="64">
       <c t="s" r="A64">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row spans="1:1" r="65">
       <c t="s" r="A65">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row spans="1:1" r="66">
       <c t="s" r="A66">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row spans="1:1" r="67">
       <c t="s" r="A67">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row spans="1:1" r="68">
       <c t="s" r="A68">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row spans="1:1" r="69">
       <c t="s" r="A69">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row spans="1:1" r="70">
       <c t="s" r="A70">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row spans="1:1" r="71">
       <c t="s" r="A71">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row spans="1:1" r="72">
       <c t="s" r="A72">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row spans="1:1" r="73">
       <c t="s" r="A73">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row spans="1:1" r="74">
       <c t="s" r="A74">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row spans="1:1" r="75">
       <c t="s" r="A75">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row spans="1:1" r="76">
       <c t="s" r="A76">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row spans="1:1" r="77">
       <c t="s" r="A77">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row spans="1:1" r="78">
       <c t="s" r="A78">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row spans="1:1" r="79">
       <c t="s" r="A79">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row spans="1:1" r="80">
       <c t="s" r="A80">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row spans="1:1" r="81">
       <c t="s" r="A81">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row spans="1:1" r="82">
       <c t="s" r="A82">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row spans="1:1" r="83">
       <c t="s" r="A83">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row spans="1:1" r="84">
       <c t="s" r="A84">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row spans="1:1" r="85">
       <c t="s" r="A85">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row spans="1:1" r="86">
       <c t="s" r="A86">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row spans="1:1" r="87">
       <c t="s" r="A87">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row spans="1:1" r="88">
       <c t="s" r="A88">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row spans="1:1" r="89">
       <c t="s" r="A89">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row spans="1:1" r="90">
       <c t="s" r="A90">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row spans="1:1" r="91">
       <c t="s" r="A91">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row spans="1:1" r="92">
       <c t="s" r="A92">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row spans="1:1" r="93">
       <c t="s" r="A93">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row spans="1:1" r="94">
       <c t="s" r="A94">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row spans="1:1" r="95">
       <c t="s" r="A95">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row spans="1:1" r="96">
       <c t="s" r="A96">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row spans="1:1" r="97">
       <c t="s" r="A97">
-        <v>211</v>
+        <v>220</v>
       </c>
     </row>
     <row spans="1:1" r="98">
       <c t="s" r="A98">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row spans="1:1" r="99">
       <c t="s" r="A99">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row spans="1:1" r="100">
       <c t="s" r="A100">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row spans="1:1" r="101">
       <c t="s" r="A101">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row spans="1:1" r="102">
       <c t="s" r="A102">
-        <v>215</v>
+        <v>224</v>
       </c>
     </row>
     <row spans="1:1" r="103">
       <c t="s" r="A103">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row spans="1:1" r="104">
       <c t="s" r="A104">
-        <v>217</v>
+        <v>226</v>
       </c>
     </row>
     <row spans="1:1" r="105">
       <c t="s" r="A105">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row spans="1:1" r="106">
       <c t="s" r="A106">
-        <v>233</v>
+        <v>242</v>
       </c>
     </row>
     <row spans="1:1" r="107">
       <c t="s" r="A107">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
     <row spans="1:1" r="108">
       <c t="s" r="A108">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
     <row spans="1:1" r="109">
       <c t="s" r="A109">
-        <v>443</v>
+        <v>465</v>
       </c>
     </row>
     <row spans="1:1" r="110">
       <c t="s" r="A110">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row spans="1:1" r="111">
       <c t="s" r="A111">
-        <v>249</v>
+        <v>258</v>
       </c>
     </row>
     <row spans="1:1" r="112">
       <c t="s" r="A112">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row spans="1:1" r="113">
       <c t="s" r="A113">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row spans="1:1" r="114">
       <c t="s" r="A114">
-        <v>293</v>
+        <v>302</v>
       </c>
     </row>
     <row spans="1:1" r="115">
       <c t="s" r="A115">
-        <v>295</v>
+        <v>304</v>
       </c>
     </row>
     <row spans="1:1" r="116">
       <c t="s" r="A116">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row spans="1:1" r="117">
       <c t="s" r="A117">
-        <v>296</v>
+        <v>305</v>
       </c>
     </row>
     <row spans="1:1" r="118">
       <c t="s" r="A118">
-        <v>297</v>
+        <v>306</v>
       </c>
     </row>
     <row spans="1:1" r="119">
       <c t="s" r="A119">
-        <v>298</v>
+        <v>307</v>
       </c>
     </row>
     <row spans="1:1" r="120">
       <c t="s" r="A120">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row spans="1:1" r="121">
       <c t="s" r="A121">
-        <v>299</v>
+        <v>308</v>
       </c>
     </row>
     <row spans="1:1" r="122">
       <c t="s" r="A122">
-        <v>289</v>
+        <v>298</v>
       </c>
     </row>
     <row spans="1:1" r="123">
       <c t="s" r="A123">
-        <v>290</v>
+        <v>299</v>
       </c>
     </row>
     <row spans="1:1" r="124">
       <c t="s" r="A124">
-        <v>301</v>
+        <v>310</v>
       </c>
     </row>
     <row spans="1:1" r="125">
       <c t="s" r="A125">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row spans="1:1" r="126">
       <c t="s" r="A126">
-        <v>291</v>
+        <v>300</v>
       </c>
     </row>
     <row spans="1:1" r="127">
       <c t="s" r="A127">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row spans="1:1" r="128">
       <c t="s" r="A128">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row spans="1:1" r="129">
       <c t="s" r="A129">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row spans="1:1" r="130">
       <c t="s" r="A130">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row spans="1:1" r="131">
       <c t="s" r="A131">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row spans="1:1" r="132">
       <c t="s" r="A132">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
     <row spans="1:1" r="133">
       <c t="s" r="A133">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row spans="1:1" r="134">
       <c t="s" r="A134">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row spans="1:1" r="135">
       <c t="s" r="A135">
-        <v>310</v>
+        <v>321</v>
       </c>
     </row>
     <row spans="1:1" r="136">
       <c t="s" r="A136">
-        <v>313</v>
+        <v>324</v>
       </c>
     </row>
     <row spans="1:1" r="137">
       <c t="s" r="A137">
-        <v>315</v>
+        <v>326</v>
       </c>
     </row>
     <row spans="1:1" r="138">
       <c t="s" r="A138">
-        <v>329</v>
+        <v>340</v>
       </c>
     </row>
     <row spans="1:1" r="139">
       <c t="s" r="A139">
-        <v>330</v>
+        <v>341</v>
       </c>
     </row>
     <row spans="1:1" r="140">
       <c t="s" r="A140">
-        <v>331</v>
+        <v>342</v>
       </c>
     </row>
     <row spans="1:1" r="141">
       <c t="s" r="A141">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row spans="1:1" r="142">
       <c t="s" r="A142">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row spans="1:1" r="143">
       <c t="s" r="A143">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row spans="1:1" r="144">
       <c t="s" r="A144">
-        <v>344</v>
+        <v>355</v>
       </c>
     </row>
     <row spans="1:1" r="145">
       <c t="s" r="A145">
-        <v>345</v>
+        <v>356</v>
       </c>
     </row>
     <row spans="1:1" r="146">
       <c t="s" r="A146">
-        <v>340</v>
+        <v>351</v>
       </c>
     </row>
     <row spans="1:1" r="147">
       <c t="s" r="A147">
-        <v>341</v>
+        <v>352</v>
       </c>
     </row>
     <row spans="1:1" r="148">
       <c t="s" r="A148">
-        <v>346</v>
+        <v>357</v>
       </c>
     </row>
     <row spans="1:1" r="149">
       <c t="s" r="A149">
-        <v>342</v>
+        <v>353</v>
       </c>
     </row>
     <row spans="1:1" r="150">
       <c t="s" r="A150">
-        <v>347</v>
+        <v>358</v>
       </c>
     </row>
     <row spans="1:1" r="151">
       <c t="s" r="A151">
-        <v>348</v>
+        <v>359</v>
       </c>
     </row>
     <row spans="1:1" r="152">
       <c t="s" r="A152">
-        <v>349</v>
+        <v>360</v>
       </c>
     </row>
     <row spans="1:1" r="153">
       <c t="s" r="A153">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row spans="1:1" r="154">
       <c t="s" r="A154">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row spans="1:1" r="155">
       <c t="s" r="A155">
-        <v>352</v>
+        <v>363</v>
       </c>
     </row>
     <row spans="1:1" r="156">
       <c t="s" r="A156">
-        <v>353</v>
+        <v>364</v>
       </c>
     </row>
     <row spans="1:1" r="157">
       <c t="s" r="A157">
-        <v>375</v>
+        <v>387</v>
       </c>
     </row>
     <row spans="1:1" r="158">
       <c t="s" r="A158">
-        <v>374</v>
+        <v>386</v>
       </c>
     </row>
     <row spans="1:1" r="159">
       <c t="s" r="A159">
-        <v>377</v>
+        <v>389</v>
       </c>
     </row>
     <row spans="1:1" r="160">
       <c t="s" r="A160">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row spans="1:1" r="161">
       <c t="s" r="A161">
-        <v>378</v>
+        <v>390</v>
       </c>
     </row>
     <row spans="1:1" r="162">
       <c t="s" r="A162">
-        <v>379</v>
+        <v>391</v>
       </c>
     </row>
     <row spans="1:1" r="163">
       <c t="s" r="A163">
-        <v>380</v>
+        <v>392</v>
       </c>
     </row>
     <row spans="1:1" r="164">
       <c t="s" r="A164">
-        <v>381</v>
+        <v>393</v>
       </c>
     </row>
     <row spans="1:1" r="165">
       <c t="s" r="A165">
-        <v>384</v>
+        <v>397</v>
       </c>
     </row>
     <row spans="1:1" r="166">
       <c t="s" r="A166">
-        <v>385</v>
+        <v>398</v>
       </c>
     </row>
     <row spans="1:1" r="167">
       <c t="s" r="A167">
-        <v>382</v>
+        <v>395</v>
       </c>
     </row>
     <row spans="1:1" r="168">
       <c t="s" r="A168">
-        <v>383</v>
+        <v>396</v>
       </c>
     </row>
     <row spans="1:1" r="169">
       <c t="s" r="A169">
-        <v>386</v>
+        <v>399</v>
       </c>
     </row>
     <row spans="1:1" r="170">
       <c t="s" r="A170">
-        <v>387</v>
+        <v>401</v>
       </c>
     </row>
     <row spans="1:1" r="171">
       <c t="s" r="A171">
-        <v>405</v>
+        <v>419</v>
       </c>
     </row>
     <row spans="1:1" r="172">
       <c t="s" r="A172">
-        <v>406</v>
+        <v>421</v>
       </c>
     </row>
     <row spans="1:1" r="173">
       <c t="s" r="A173">
-        <v>408</v>
+        <v>423</v>
       </c>
     </row>
     <row spans="1:1" r="174">
       <c t="s" r="A174">
-        <v>417</v>
+        <v>432</v>
       </c>
     </row>
     <row spans="1:1" r="175">
       <c t="s" r="A175">
-        <v>418</v>
+        <v>433</v>
       </c>
     </row>
     <row spans="1:1" r="176">
       <c t="s" r="A176">
-        <v>419</v>
+        <v>434</v>
       </c>
     </row>
     <row spans="1:1" r="177">
       <c t="s" r="A177">
-        <v>420</v>
+        <v>435</v>
       </c>
     </row>
     <row spans="1:1" r="178">
       <c t="s" r="A178">
-        <v>430</v>
+        <v>446</v>
       </c>
     </row>
     <row spans="1:1" r="179">
       <c t="s" r="A179">
-        <v>433</v>
+        <v>449</v>
       </c>
     </row>
     <row spans="1:1" r="180">
       <c t="s" r="A180">
-        <v>431</v>
+        <v>447</v>
       </c>
     </row>
     <row spans="1:1" r="181">
       <c t="s" r="A181">
-        <v>434</v>
+        <v>450</v>
       </c>
     </row>
     <row spans="1:1" r="182">
       <c t="s" r="A182">
-        <v>432</v>
+        <v>448</v>
       </c>
     </row>
     <row spans="1:1" r="183">
       <c t="s" r="A183">
-        <v>442</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" footer="0.5" header="0.5" right="0.75" bottom="1"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" right="0.75" top="1" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
   <dimension ref="A1:A253"/>
   <sheetViews>
@@ -2805,1172 +3007,1172 @@
     </row>
     <row spans="1:1" r="17">
       <c t="s" r="A17">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row spans="1:1" r="18">
       <c t="s" r="A18">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row spans="1:1" r="19">
       <c t="s" r="A19">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row spans="1:1" r="20">
       <c t="s" r="A20">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row spans="1:1" r="21">
       <c t="s" r="A21">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row spans="1:1" r="22">
       <c t="s" r="A22">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row spans="1:1" r="23">
       <c t="s" r="A23">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row spans="1:1" r="24">
       <c t="s" r="A24">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row spans="1:1" r="25">
       <c t="s" r="A25">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row spans="1:1" r="26">
       <c t="s" r="A26">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row spans="1:1" r="27">
       <c t="s" r="A27">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row spans="1:1" r="28">
       <c t="s" r="A28">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row spans="1:1" r="29">
       <c t="s" r="A29">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row spans="1:1" r="30">
       <c t="s" r="A30">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row spans="1:1" r="31">
       <c t="s" r="A31">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row spans="1:1" r="32">
       <c t="s" r="A32">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row spans="1:1" r="33">
       <c t="s" r="A33">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row spans="1:1" r="34">
       <c t="s" r="A34">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row spans="1:1" r="35">
       <c t="s" r="A35">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row spans="1:1" r="36">
       <c t="s" r="A36">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row spans="1:1" r="37">
       <c t="s" r="A37">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row spans="1:1" r="38">
       <c t="s" r="A38">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row spans="1:1" r="39">
       <c t="s" r="A39">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row spans="1:1" r="40">
       <c t="s" r="A40">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row spans="1:1" r="41">
       <c t="s" r="A41">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row spans="1:1" r="42">
       <c t="s" r="A42">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row spans="1:1" r="43">
       <c t="s" r="A43">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row spans="1:1" r="44">
       <c t="s" r="A44">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row spans="1:1" r="45">
       <c t="s" r="A45">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row spans="1:1" r="46">
       <c t="s" r="A46">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row spans="1:1" r="47">
       <c t="s" r="A47">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row spans="1:1" r="48">
       <c t="s" r="A48">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row spans="1:1" r="49">
       <c t="s" r="A49">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row spans="1:1" r="50">
       <c t="s" r="A50">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row spans="1:1" r="51">
       <c t="s" r="A51">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row spans="1:1" r="52">
       <c t="s" r="A52">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row spans="1:1" r="53">
       <c t="s" r="A53">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row spans="1:1" r="54">
       <c t="s" r="A54">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row spans="1:1" r="55">
       <c t="s" r="A55">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row spans="1:1" r="56">
       <c t="s" r="A56">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row spans="1:1" r="57">
       <c t="s" r="A57">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row spans="1:1" r="58">
       <c t="s" r="A58">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row spans="1:1" r="59">
       <c t="s" r="A59">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row spans="1:1" r="60">
       <c t="s" r="A60">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row spans="1:1" r="61">
       <c t="s" r="A61">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row spans="1:1" r="62">
       <c t="s" r="A62">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row spans="1:1" r="63">
       <c t="s" r="A63">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row spans="1:1" r="64">
       <c t="s" r="A64">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row spans="1:1" r="65">
       <c t="s" r="A65">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row spans="1:1" r="66">
       <c t="s" r="A66">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row spans="1:1" r="67">
       <c t="s" r="A67">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row spans="1:1" r="68">
       <c t="s" r="A68">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row spans="1:1" r="69">
       <c t="s" r="A69">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row spans="1:1" r="70">
       <c t="s" r="A70">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row spans="1:1" r="71">
       <c t="s" r="A71">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row spans="1:1" r="72">
       <c t="s" r="A72">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row spans="1:1" r="73">
       <c t="s" r="A73">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row spans="1:1" r="74">
       <c t="s" r="A74">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row spans="1:1" r="75">
       <c t="s" r="A75">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row spans="1:1" r="76">
       <c t="s" r="A76">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row spans="1:1" r="77">
       <c t="s" r="A77">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row spans="1:1" r="78">
       <c t="s" r="A78">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row spans="1:1" r="79">
       <c t="s" r="A79">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row spans="1:1" r="80">
       <c t="s" r="A80">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row spans="1:1" r="81">
       <c t="s" r="A81">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row spans="1:1" r="82">
       <c t="s" r="A82">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row spans="1:1" r="83">
       <c t="s" r="A83">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row spans="1:1" r="84">
       <c t="s" r="A84">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row spans="1:1" r="85">
       <c t="s" r="A85">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row spans="1:1" r="86">
       <c t="s" r="A86">
-        <v>174</v>
+        <v>181</v>
       </c>
     </row>
     <row spans="1:1" r="87">
       <c t="s" r="A87">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row spans="1:1" r="88">
       <c t="s" r="A88">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row spans="1:1" r="89">
       <c t="s" r="A89">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row spans="1:1" r="90">
       <c t="s" r="A90">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row spans="1:1" r="91">
       <c t="s" r="A91">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row spans="1:1" r="92">
       <c t="s" r="A92">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row spans="1:1" r="93">
       <c t="s" r="A93">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row spans="1:1" r="94">
       <c t="s" r="A94">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row spans="1:1" r="95">
       <c t="s" r="A95">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row spans="1:1" r="96">
       <c t="s" r="A96">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row spans="1:1" r="97">
       <c t="s" r="A97">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row spans="1:1" r="98">
       <c t="s" r="A98">
-        <v>192</v>
+        <v>201</v>
       </c>
     </row>
     <row spans="1:1" r="99">
       <c t="s" r="A99">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row spans="1:1" r="100">
       <c t="s" r="A100">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row spans="1:1" r="101">
       <c t="s" r="A101">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row spans="1:1" r="102">
       <c t="s" r="A102">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row spans="1:1" r="103">
       <c t="s" r="A103">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row spans="1:1" r="104">
       <c t="s" r="A104">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row spans="1:1" r="105">
       <c t="s" r="A105">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row spans="1:1" r="106">
       <c t="s" r="A106">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row spans="1:1" r="107">
       <c t="s" r="A107">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row spans="1:1" r="108">
       <c t="s" r="A108">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row spans="1:1" r="109">
       <c t="s" r="A109">
-        <v>221</v>
+        <v>230</v>
       </c>
     </row>
     <row spans="1:1" r="110">
       <c t="s" r="A110">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row spans="1:1" r="111">
       <c t="s" r="A111">
-        <v>223</v>
+        <v>232</v>
       </c>
     </row>
     <row spans="1:1" r="112">
       <c t="s" r="A112">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row spans="1:1" r="113">
       <c t="s" r="A113">
-        <v>225</v>
+        <v>234</v>
       </c>
     </row>
     <row spans="1:1" r="114">
       <c t="s" r="A114">
-        <v>226</v>
+        <v>235</v>
       </c>
     </row>
     <row spans="1:1" r="115">
       <c t="s" r="A115">
-        <v>227</v>
+        <v>236</v>
       </c>
     </row>
     <row spans="1:1" r="116">
       <c t="s" r="A116">
-        <v>228</v>
+        <v>237</v>
       </c>
     </row>
     <row spans="1:1" r="117">
       <c t="s" r="A117">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row spans="1:1" r="118">
       <c t="s" r="A118">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row spans="1:1" r="119">
       <c t="s" r="A119">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row spans="1:1" r="120">
       <c t="s" r="A120">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row spans="1:1" r="121">
       <c t="s" r="A121">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row spans="1:1" r="122">
       <c t="s" r="A122">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
     <row spans="1:1" r="123">
       <c t="s" r="A123">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row spans="1:1" r="124">
       <c t="s" r="A124">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row spans="1:1" r="125">
       <c t="s" r="A125">
-        <v>240</v>
+        <v>249</v>
       </c>
     </row>
     <row spans="1:1" r="126">
       <c t="s" r="A126">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row spans="1:1" r="127">
       <c t="s" r="A127">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row spans="1:1" r="128">
       <c t="s" r="A128">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row spans="1:1" r="129">
       <c t="s" r="A129">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row spans="1:1" r="130">
       <c t="s" r="A130">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row spans="1:1" r="131">
       <c t="s" r="A131">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row spans="1:1" r="132">
       <c t="s" r="A132">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row spans="1:1" r="133">
       <c t="s" r="A133">
-        <v>252</v>
+        <v>261</v>
       </c>
     </row>
     <row spans="1:1" r="134">
       <c t="s" r="A134">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row spans="1:1" r="135">
       <c t="s" r="A135">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row spans="1:1" r="136">
       <c t="s" r="A136">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row spans="1:1" r="137">
       <c t="s" r="A137">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row spans="1:1" r="138">
       <c t="s" r="A138">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
     <row spans="1:1" r="139">
       <c t="s" r="A139">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row spans="1:1" r="140">
       <c t="s" r="A140">
-        <v>260</v>
+        <v>269</v>
       </c>
     </row>
     <row spans="1:1" r="141">
       <c t="s" r="A141">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row spans="1:1" r="142">
       <c t="s" r="A142">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row spans="1:1" r="143">
       <c t="s" r="A143">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row spans="1:1" r="144">
       <c t="s" r="A144">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row spans="1:1" r="145">
       <c t="s" r="A145">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row spans="1:1" r="146">
       <c t="s" r="A146">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row spans="1:1" r="147">
       <c t="s" r="A147">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
     <row spans="1:1" r="148">
       <c t="s" r="A148">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row spans="1:1" r="149">
       <c t="s" r="A149">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row spans="1:1" r="150">
       <c t="s" r="A150">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row spans="1:1" r="151">
       <c t="s" r="A151">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row spans="1:1" r="152">
       <c t="s" r="A152">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row spans="1:1" r="153">
       <c t="s" r="A153">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row spans="1:1" r="154">
       <c t="s" r="A154">
-        <v>276</v>
+        <v>285</v>
       </c>
     </row>
     <row spans="1:1" r="155">
       <c t="s" r="A155">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row spans="1:1" r="156">
       <c t="s" r="A156">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row spans="1:1" r="157">
       <c t="s" r="A157">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row spans="1:1" r="158">
       <c t="s" r="A158">
-        <v>281</v>
+        <v>290</v>
       </c>
     </row>
     <row spans="1:1" r="159">
       <c t="s" r="A159">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row spans="1:1" r="160">
       <c t="s" r="A160">
-        <v>283</v>
+        <v>292</v>
       </c>
     </row>
     <row spans="1:1" r="161">
       <c t="s" r="A161">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row spans="1:1" r="162">
       <c t="s" r="A162">
-        <v>285</v>
+        <v>294</v>
       </c>
     </row>
     <row spans="1:1" r="163">
       <c t="s" r="A163">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row spans="1:1" r="164">
       <c t="s" r="A164">
-        <v>287</v>
+        <v>296</v>
       </c>
     </row>
     <row spans="1:1" r="165">
       <c t="s" r="A165">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row spans="1:1" r="166">
       <c t="s" r="A166">
-        <v>311</v>
+        <v>322</v>
       </c>
     </row>
     <row spans="1:1" r="167">
       <c t="s" r="A167">
-        <v>316</v>
+        <v>327</v>
       </c>
     </row>
     <row spans="1:1" r="168">
       <c t="s" r="A168">
-        <v>317</v>
+        <v>328</v>
       </c>
     </row>
     <row spans="1:1" r="169">
       <c t="s" r="A169">
-        <v>318</v>
+        <v>329</v>
       </c>
     </row>
     <row spans="1:1" r="170">
       <c t="s" r="A170">
-        <v>319</v>
+        <v>330</v>
       </c>
     </row>
     <row spans="1:1" r="171">
       <c t="s" r="A171">
-        <v>320</v>
+        <v>331</v>
       </c>
     </row>
     <row spans="1:1" r="172">
       <c t="s" r="A172">
-        <v>321</v>
+        <v>332</v>
       </c>
     </row>
     <row spans="1:1" r="173">
       <c t="s" r="A173">
-        <v>322</v>
+        <v>333</v>
       </c>
     </row>
     <row spans="1:1" r="174">
       <c t="s" r="A174">
-        <v>323</v>
+        <v>334</v>
       </c>
     </row>
     <row spans="1:1" r="175">
       <c t="s" r="A175">
-        <v>324</v>
+        <v>335</v>
       </c>
     </row>
     <row spans="1:1" r="176">
       <c t="s" r="A176">
-        <v>325</v>
+        <v>336</v>
       </c>
     </row>
     <row spans="1:1" r="177">
       <c t="s" r="A177">
-        <v>326</v>
+        <v>337</v>
       </c>
     </row>
     <row spans="1:1" r="178">
       <c t="s" r="A178">
-        <v>327</v>
+        <v>338</v>
       </c>
     </row>
     <row spans="1:1" r="179">
       <c t="s" r="A179">
-        <v>328</v>
+        <v>339</v>
       </c>
     </row>
     <row spans="1:1" r="180">
       <c t="s" r="A180">
-        <v>333</v>
+        <v>344</v>
       </c>
     </row>
     <row spans="1:1" r="181">
       <c t="s" r="A181">
-        <v>334</v>
+        <v>345</v>
       </c>
     </row>
     <row spans="1:1" r="182">
       <c t="s" r="A182">
-        <v>335</v>
+        <v>346</v>
       </c>
     </row>
     <row spans="1:1" r="183">
       <c t="s" r="A183">
-        <v>336</v>
+        <v>347</v>
       </c>
     </row>
     <row spans="1:1" r="184">
       <c t="s" r="A184">
-        <v>337</v>
+        <v>348</v>
       </c>
     </row>
     <row spans="1:1" r="185">
       <c t="s" r="A185">
-        <v>354</v>
+        <v>365</v>
       </c>
     </row>
     <row spans="1:1" r="186">
       <c t="s" r="A186">
-        <v>373</v>
+        <v>385</v>
       </c>
     </row>
     <row spans="1:1" r="187">
       <c t="s" r="A187">
-        <v>355</v>
+        <v>366</v>
       </c>
     </row>
     <row spans="1:1" r="188">
       <c t="s" r="A188">
-        <v>356</v>
+        <v>367</v>
       </c>
     </row>
     <row spans="1:1" r="189">
       <c t="s" r="A189">
-        <v>357</v>
+        <v>368</v>
       </c>
     </row>
     <row spans="1:1" r="190">
       <c t="s" r="A190">
-        <v>358</v>
+        <v>369</v>
       </c>
     </row>
     <row spans="1:1" r="191">
       <c t="s" r="A191">
-        <v>359</v>
+        <v>370</v>
       </c>
     </row>
     <row spans="1:1" r="192">
       <c t="s" r="A192">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
     <row spans="1:1" r="193">
       <c t="s" r="A193">
-        <v>361</v>
+        <v>372</v>
       </c>
     </row>
     <row spans="1:1" r="194">
       <c t="s" r="A194">
-        <v>362</v>
+        <v>373</v>
       </c>
     </row>
     <row spans="1:1" r="195">
       <c t="s" r="A195">
-        <v>363</v>
+        <v>374</v>
       </c>
     </row>
     <row spans="1:1" r="196">
       <c t="s" r="A196">
-        <v>364</v>
+        <v>375</v>
       </c>
     </row>
     <row spans="1:1" r="197">
       <c t="s" r="A197">
-        <v>365</v>
+        <v>376</v>
       </c>
     </row>
     <row spans="1:1" r="198">
       <c t="s" r="A198">
-        <v>366</v>
+        <v>377</v>
       </c>
     </row>
     <row spans="1:1" r="199">
       <c t="s" r="A199">
-        <v>367</v>
+        <v>378</v>
       </c>
     </row>
     <row spans="1:1" r="200">
       <c t="s" r="A200">
-        <v>368</v>
+        <v>379</v>
       </c>
     </row>
     <row spans="1:1" r="201">
       <c t="s" r="A201">
-        <v>369</v>
+        <v>380</v>
       </c>
     </row>
     <row spans="1:1" r="202">
       <c t="s" r="A202">
-        <v>370</v>
+        <v>381</v>
       </c>
     </row>
     <row spans="1:1" r="203">
       <c t="s" r="A203">
-        <v>371</v>
+        <v>382</v>
       </c>
     </row>
     <row spans="1:1" r="204">
       <c t="s" r="A204">
-        <v>372</v>
+        <v>383</v>
       </c>
     </row>
     <row spans="1:1" r="205">
       <c t="s" r="A205">
-        <v>388</v>
+        <v>402</v>
       </c>
     </row>
     <row spans="1:1" r="206">
       <c t="s" r="A206">
-        <v>389</v>
+        <v>403</v>
       </c>
     </row>
     <row spans="1:1" r="207">
       <c t="s" r="A207">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row spans="1:1" r="208">
       <c t="s" r="A208">
-        <v>391</v>
+        <v>405</v>
       </c>
     </row>
     <row spans="1:1" r="209">
       <c t="s" r="A209">
-        <v>392</v>
+        <v>406</v>
       </c>
     </row>
     <row spans="1:1" r="210">
       <c t="s" r="A210">
-        <v>393</v>
+        <v>407</v>
       </c>
     </row>
     <row spans="1:1" r="211">
       <c t="s" r="A211">
-        <v>394</v>
+        <v>408</v>
       </c>
     </row>
     <row spans="1:1" r="212">
       <c t="s" r="A212">
-        <v>396</v>
+        <v>410</v>
       </c>
     </row>
     <row spans="1:1" r="213">
       <c t="s" r="A213">
-        <v>397</v>
+        <v>411</v>
       </c>
     </row>
     <row spans="1:1" r="214">
       <c t="s" r="A214">
-        <v>398</v>
+        <v>412</v>
       </c>
     </row>
     <row spans="1:1" r="215">
       <c t="s" r="A215">
-        <v>399</v>
+        <v>413</v>
       </c>
     </row>
     <row spans="1:1" r="216">
       <c t="s" r="A216">
-        <v>400</v>
+        <v>414</v>
       </c>
     </row>
     <row spans="1:1" r="217">
       <c t="s" r="A217">
-        <v>401</v>
+        <v>415</v>
       </c>
     </row>
     <row spans="1:1" r="218">
       <c t="s" r="A218">
-        <v>402</v>
+        <v>416</v>
       </c>
     </row>
     <row spans="1:1" r="219">
       <c t="s" r="A219">
-        <v>403</v>
+        <v>417</v>
       </c>
     </row>
     <row spans="1:1" r="220">
       <c t="s" r="A220">
-        <v>404</v>
+        <v>418</v>
       </c>
     </row>
     <row spans="1:1" r="221">
       <c t="s" r="A221">
-        <v>409</v>
+        <v>424</v>
       </c>
     </row>
     <row spans="1:1" r="222">
       <c t="s" r="A222">
-        <v>410</v>
+        <v>425</v>
       </c>
     </row>
     <row spans="1:1" r="223">
       <c t="s" r="A223">
-        <v>411</v>
+        <v>426</v>
       </c>
     </row>
     <row spans="1:1" r="224">
       <c t="s" r="A224">
-        <v>412</v>
+        <v>427</v>
       </c>
     </row>
     <row spans="1:1" r="225">
       <c t="s" r="A225">
-        <v>414</v>
+        <v>429</v>
       </c>
     </row>
     <row spans="1:1" r="226">
       <c t="s" r="A226">
-        <v>415</v>
+        <v>430</v>
       </c>
     </row>
     <row spans="1:1" r="227">
       <c t="s" r="A227">
-        <v>416</v>
+        <v>431</v>
       </c>
     </row>
     <row spans="1:1" r="228">
       <c t="s" r="A228">
-        <v>421</v>
+        <v>436</v>
       </c>
     </row>
     <row spans="1:1" r="229">
       <c t="s" r="A229">
-        <v>422</v>
+        <v>437</v>
       </c>
     </row>
     <row spans="1:1" r="230">
       <c t="s" r="A230">
-        <v>423</v>
+        <v>438</v>
       </c>
     </row>
     <row spans="1:1" r="231">
       <c t="s" r="A231">
-        <v>424</v>
+        <v>439</v>
       </c>
     </row>
     <row spans="1:1" r="232">
       <c t="s" r="A232">
-        <v>425</v>
+        <v>440</v>
       </c>
     </row>
     <row spans="1:1" r="233">
       <c t="s" r="A233">
-        <v>426</v>
+        <v>441</v>
       </c>
     </row>
     <row spans="1:1" r="234">
       <c t="s" r="A234">
-        <v>427</v>
+        <v>442</v>
       </c>
     </row>
     <row spans="1:1" r="235">
       <c t="s" r="A235">
-        <v>428</v>
+        <v>443</v>
       </c>
     </row>
     <row spans="1:1" r="236">
       <c t="s" r="A236">
-        <v>429</v>
+        <v>444</v>
       </c>
     </row>
     <row spans="1:1" r="237">
       <c t="s" r="A237">
-        <v>435</v>
+        <v>451</v>
       </c>
     </row>
     <row spans="1:1" r="238">
       <c t="s" r="A238">
-        <v>436</v>
+        <v>452</v>
       </c>
     </row>
     <row spans="1:1" r="239">
       <c t="s" r="A239">
-        <v>437</v>
+        <v>453</v>
       </c>
     </row>
     <row spans="1:1" r="240">
       <c t="s" r="A240">
-        <v>438</v>
+        <v>454</v>
       </c>
     </row>
     <row spans="1:1" r="241">
       <c t="s" r="A241">
-        <v>439</v>
+        <v>455</v>
       </c>
     </row>
     <row spans="1:1" r="242">
       <c t="s" r="A242">
-        <v>440</v>
+        <v>456</v>
       </c>
     </row>
     <row spans="1:1" r="243">
       <c t="s" r="A243">
-        <v>441</v>
+        <v>457</v>
       </c>
     </row>
     <row spans="1:1" r="244">
       <c t="s" r="A244">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row spans="1:1" r="245">
       <c t="s" r="A245">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row spans="1:1" r="246">
       <c t="s" r="A246">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row spans="1:1" r="247">
       <c t="s" r="A247">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row spans="1:1" r="248">
       <c t="s" r="A248">
-        <v>256</v>
+        <v>265</v>
       </c>
     </row>
     <row spans="1:1" r="249">
       <c t="s" r="A249">
-        <v>278</v>
+        <v>287</v>
       </c>
     </row>
     <row spans="1:1" r="250">
       <c t="s" r="A250">
-        <v>312</v>
+        <v>323</v>
       </c>
     </row>
     <row spans="1:1" r="251">
@@ -3980,15 +4182,15 @@
     </row>
     <row spans="1:1" r="252">
       <c t="s" r="A252">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row spans="1:1" r="253">
       <c t="s" r="A253">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins top="1" left="0.75" footer="0.5" header="0.5" right="0.75" bottom="1"/>
+  <pageMargins header="0.5" left="0.75" bottom="1" right="0.75" top="1" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>